<commit_message>
Partial results with Chris' updates
</commit_message>
<xml_diff>
--- a/results/1019/2022-1019_resnet34_malmotest_cifar.xlsx
+++ b/results/1019/2022-1019_resnet34_malmotest_cifar.xlsx
@@ -606,7 +606,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -635,37 +635,37 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5']</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[81, 97, 100, 111, 135]</t>
+          <t>[81, 103, 110, 113, 154, 206, 250, 250, 250, 250, 271, 271, 306, 331, 331, 331, 331, 331, 331, 369, 369, 369, 379, 397, 397, 408, 408, 408, 408, 408, 408, 408, 408, 408, 408, 408, 408, 451, 498, 498, 515, 515, 515, 515, 515, 520, 520, 560, 579, 579, 579, 579, 581, 581, 581, 620, 620, 620, 624, 624, 624, 630, 669, 671, 671, 707, 707, 707, 719, 719, 751, 751, 751, 751, 794, 815, 815, 850, 894, 894, 894, 908, 917, 924, 926, 949, 949, 949, 949, 949, 967, 967, 967, 967, 967, 972, 972, 991, 994, 994, 1001, 1008, 1016, 1020, 1023, 1049, 1049, 1049, 1049, 1049, 1054, 1054, 1054, 1088, 1088, 1114, 1151, 1196, 1216, 1233, 1233]</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>[0.342, 0.365, 0.38, 0.387, 0.395]</t>
+          <t>[0.342, 0.361, 0.38, 0.376, 0.378, 0.387, 0.406, 0.406, 0.406, 0.406, 0.41, 0.41, 0.412, 0.415, 0.415, 0.415, 0.415, 0.415, 0.415, 0.414, 0.414, 0.414, 0.415, 0.415, 0.415, 0.414, 0.414, 0.414, 0.414, 0.414, 0.414, 0.414, 0.414, 0.414, 0.414, 0.414, 0.414, 0.434, 0.436, 0.436, 0.445, 0.445, 0.445, 0.445, 0.445, 0.451, 0.451, 0.477, 0.487, 0.487, 0.487, 0.487, 0.487, 0.487, 0.487, 0.483, 0.483, 0.483, 0.494, 0.494, 0.494, 0.496, 0.496, 0.504, 0.504, 0.515, 0.515, 0.515, 0.521, 0.521, 0.521, 0.521, 0.521, 0.521, 0.526, 0.526, 0.526, 0.53, 0.53, 0.53, 0.53, 0.536, 0.536, 0.539, 0.539, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.549, 0.549, 0.547, 0.551, 0.551, 0.549, 0.549, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.547, 0.549, 0.551, 0.549, 0.558, 0.56, 0.56]</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[0, 30, 60, 90, 120]</t>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>[0, 18.236424016952512, 34.08466680049896, 56.91897404193878, 79.69941833019257]</t>
+          <t>[0, 14.238859248161326, 30.584168601036062, 54.06408069133755, 75.44980390071866, 100.90120275020597, 111.29249092340467, 137.74763594865797, 151.46075209379194, 151.46075209379194, 160.58210184574125, 165.89301402568816, 182.54957349300383, 205.94067118167877, 216.32914750576018, 240.42414352893826, 274.01413934230806, 296.42167184352877, 314.13456789255144, 330.7262953400612, 336.52962003946305, 354.25521584749225, 367.4702325940132, 389.2008349061012, 401.7083367466926, 423.913519346714, 451.50811578035353, 472.4707615494728, 491.6068103671074, 523.2977817416191, 529.9474246263504, 551.6735692739487, 567.0441504240036, 584.0344890117645, 601.8847670078278, 624.8867324352265, 637.9007064342499, 655.9134069919586, 670.4367328643799, 670.8564328670502, 690.669384431839, 713.7037794828416, 735.2904783487321, 757.5305744886399, 778.4053435087204, 792.4294032335282, 800.2396621465683, 810.7229883670807, 829.1413764715195, 859.366010260582, 864.784878396988, 885.7102738618852, 887.6779209971429, 911.887320315838, 922.863535130024, 945.5411580681802, 978.2071539998055, 997.3626424908639, 1017.7100149989129, 1034.2148728728296, 1040.9854283690454, 1055.7535365343094, 1081.211882853508, 1102.4255895614624, 1126.8980884552002, 1140.5269421815872, 1165.8882149457932, 1180.9806281924248, 1200.696478641033, 1222.472106182575, 1230.9785199999808, 1243.7656226992606, 1265.0178682446478, 1282.1447900652884, 1306.3008828520774, 1324.2272478222847, 1331.9338646173476, 1344.8094705581664, 1368.5259495973587, 1392.1389447450638, 1397.6977461457252, 1415.2337995171547, 1438.0681573748589, 1463.6221938490867, 1484.5430100321769, 1507.5471589922904, 1515.5967592120169, 1542.9967260241506, 1555.9888626456259, 1555.9888626456259, 1564.7525124073027, 1587.3306627273557, 1605.0922231674192, 1625.3255253791806, 1646.4928902387617, 1669.1665069818494, 1685.8406611680982, 1703.434461712837, 1719.1293334007262, 1719.5490334033964, 1741.3872358798978, 1758.0333147525785, 1776.0912307977674, 1797.26188313961, 1820.042327427864, 1845.4937262773512, 1853.5433264970777, 1880.4710069894788, 1893.0990226745603, 1893.0990226745603, 1903.4198111295698, 1925.3931240320203, 1935.8538418769833, 1942.3296284198757, 1959.5679224491116, 1985.5087712764737, 1995.5707715511319, 2021.4872748374935, 2041.1978252410884, 2055.39758541584, 2076.3616905689237]</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>[0, 4.25, 4.3, 6.63, 24.3]</t>
+          <t>[0, 3.74, 3.92, 4.41, 17.48, 32.93, 43.82, 43.88, 43.94, 44.01, 50.2, 50.33, 56.76, 63.21, 63.34, 63.49, 63.55, 63.6, 63.66, 74.1, 74.24, 74.36, 77.53, 82.49, 82.62, 85.37, 85.44, 85.51, 85.58, 85.66, 85.72, 85.78, 85.83, 85.9, 85.98, 86.07, 86.14, 99.34, 120.17, 120.26, 131.65, 131.73, 131.81, 131.89, 132.11, 134.84, 134.95, 143.64, 149.22, 149.32, 149.41, 149.53, 151.27, 151.38, 151.48, 168.96, 169.06, 169.29, 170.23, 170.33, 170.54, 171.68, 181.06, 181.67, 181.77, 187.34, 187.42, 187.57, 189.48, 189.78, 198.07, 198.31, 198.5, 198.7, 210.73, 216.07, 216.17, 225.44, 237.42, 237.67, 237.77, 243.23, 245.86, 248.31, 249.19, 253.47, 253.59, 253.82, 254.08, 254.17, 260.79, 260.92, 261.04, 261.12, 261.2, 263.06, 263.38, 267.5, 268.56, 268.68, 271.36, 275.11, 276.66, 278.73, 280.73, 288.54, 288.68, 288.84, 288.94, 289.23, 292.03, 292.12, 292.43, 301.33, 301.58, 306.12, 317.81, 334.86, 349.54, 357.75, 357.85]</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>[0, -10, -10, 0, -10, -10, -10, -10, -10, -10, 0, 0, 0, -10, -10, -10, -20, -20, -20, 0, -20, 0, -20, 0, -20, -20, 0, 0, 0, -20, 0, 0, -20, -20, -20, 0, 0, 0, 0, -20, -10, -20, -20, -20, -20, -20, -20, -10, -20, 0, -10, 0, 0, 0, 0, 0, 0, 0, -10, 0, -10, -10, 0, 0, 0, 0, 0, -10, -10, 0, 0, 0, 0, -10, 0, 0, 0, 0, 0, 0, -20]</t>
+          <t>[0, -20, -10, 0, -10, -10, -10, -10, 0, -20, -10, 0, -10, -10, 0, 0, 0, -20, -20, 0, -20, 0, -20, 0, 0, 0, -10, 0, -10, 0, 0, -10, -20, -20, -20, 0, -20, -10, 0, 0, -20, -10, -20, 0, 0, -20, 0, 0, -10, 0, -20, -20, 0, -20, 0, -10, 0, -10, -20, 0, -20, -20, 0, 0, -20, 0, 0, -10, 0, 0, 0, 0, 0, -10, -10, 0, 0, 0, 0, -10, 0]</t>
         </is>
       </c>
     </row>
@@ -675,7 +675,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -704,37 +704,37 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2']</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[81, 96, 105, 110, 115]</t>
+          <t>[81, 83, 104, 107, 136, 189, 222, 222, 222, 222, 243, 253, 256, 260, 300, 347, 377, 377, 377, 377, 394, 408, 444, 444, 444, 475, 475, 475, 475, 475, 495, 513, 513, 513, 513, 544, 544, 545, 545, 545, 549, 549, 549, 549, 585, 586, 586, 626, 644, 644, 644, 644, 678, 718, 718, 751, 751, 751, 770, 770, 770, 770, 772, 775, 775, 775, 775, 775, 775, 807, 807, 807, 827, 827, 832, 850, 850, 890, 937, 937, 962, 967, 976, 976, 976, 997, 997, 998, 998, 998, 1016, 1016, 1018, 1025, 1025, 1031, 1036, 1038, 1038, 1038, 1045, 1045, 1046, 1046, 1046, 1060, 1060, 1063, 1080, 1080, 1081, 1081, 1098, 1105, 1105, 1109, 1109, 1112, 1112, 1112, 1112]</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>[0.342, 0.372, 0.397, 0.395, 0.408]</t>
+          <t>[0.342, 0.353, 0.367, 0.367, 0.383, 0.374, 0.383, 0.383, 0.383, 0.383, 0.383, 0.382, 0.382, 0.382, 0.393, 0.397, 0.389, 0.389, 0.389, 0.389, 0.385, 0.382, 0.389, 0.389, 0.389, 0.391, 0.391, 0.391, 0.391, 0.391, 0.391, 0.389, 0.389, 0.389, 0.389, 0.397, 0.397, 0.4, 0.4, 0.4, 0.402, 0.402, 0.402, 0.402, 0.41, 0.41, 0.41, 0.417, 0.417, 0.417, 0.417, 0.417, 0.427, 0.434, 0.434, 0.438, 0.438, 0.438, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.447, 0.451, 0.451, 0.47, 0.474, 0.474, 0.487, 0.487, 0.489, 0.489, 0.489, 0.489, 0.489, 0.489, 0.489, 0.489, 0.489, 0.489, 0.489, 0.491, 0.491, 0.492, 0.494, 0.492, 0.492, 0.492, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.506, 0.506, 0.506, 0.506, 0.506, 0.506, 0.506, 0.504, 0.504, 0.502, 0.502, 0.502, 0.502]</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[0, 30, 60, 90, 120]</t>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>[0, 22.054460763931267, 43.12224800586698, 66.89114811420438, 90.60140645503998]</t>
+          <t>[0, 15.943641805648802, 32.21402776241301, 53.66765954494474, 76.44810383319853, 102.38895266056059, 111.77344046831129, 138.70112096071242, 151.76592141389844, 151.76592141389844, 160.48982098102567, 180.8902866601944, 197.33506660461424, 217.74458758831022, 238.66540377140043, 264.1168026208877, 273.33910281658166, 297.70796401500695, 310.80239901542654, 310.80239901542654, 320.06284856796253, 333.2430622577666, 355.9257377386092, 375.87110300064074, 401.32250185012805, 414.7662580490111, 429.55579406023014, 440.79878418445577, 463.4431498289107, 484.72387378215774, 493.12625377178176, 500.79820970296845, 524.8422034621237, 544.0096334099768, 569.9504822373389, 586.9617185711859, 609.3126027524469, 622.5476127326485, 636.8675952374932, 658.6432200610634, 677.0084059417244, 699.8825415551659, 722.6748344838616, 746.0986232936378, 769.5627124011512, 786.0449994266029, 793.0681427180763, 805.034203523397, 822.5067526042457, 846.1197477519507, 851.1318783581252, 859.5843858778471, 875.7650436460966, 899.7070408880705, 910.998866039514, 930.3693339407439, 962.3220300257201, 979.5884872496123, 1000.9934027254576, 1025.42419925332, 1032.0738421380513, 1059.1732846438879, 1060.6009897410863, 1082.9680715262884, 1096.2260234773153, 1118.431214088201, 1142.2352633178227, 1163.2841515243047, 1178.2846020638935, 1194.9410615384572, 1200.6579370677464, 1221.53207604289, 1240.265024775266, 1260.1590421617025, 1282.5190958678716, 1306.8397214591496, 1323.9205623328678, 1340.6765628516666, 1355.9759845435613, 1356.3956845462315, 1377.8143337428562, 1388.9054914295666, 1404.1500815212719, 1422.8404263317577, 1448.291825181245, 1461.9188082277767, 1488.6415052115908, 1501.7126299798479, 1523.0339516103259, 1544.314678233861, 1553.7201572716228, 1565.2273679554455, 1589.7275122463695, 1608.214843517541, 1633.1767923891537, 1645.7434289276591, 1659.665569341182, 1669.4641629934304, 1689.6308024644845, 1710.6640790939325, 1720.5937642455094, 1733.0368791580192, 1758.0237746238702, 1777.2684324502939, 1803.209281277656, 1816.8115889787668, 1844.53543857336, 1856.5273277997965, 1875.5467200040812, 1896.579994797706, 1905.3635111570352, 1917.8513729989522, 1944.7240713059896, 1961.4022874295706, 1986.3642363011832, 2000.9373573243613, 2014.153499567508, 2024.9656651377672, 2042.10009740591, 2057.936917650699, 2065.0976979613297]</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>[0, 2.53, 4.13, 5.49, 6.82]</t>
+          <t>[0, 0.09, 3.25, 3.74, 11.04, 23.38, 31.12, 31.18, 31.22, 31.28, 37.86, 40.5, 41.38, 43.5, 53.39, 67.27, 76.45, 76.61, 76.69, 76.77, 83.16, 88.35, 100.5, 100.66, 100.85, 111.55, 111.63, 111.74, 111.81, 111.87, 118.49, 125.02, 125.23, 125.43, 125.49, 137.22, 137.29, 137.46, 137.7, 137.75, 139.23, 139.3, 139.4, 139.5, 152.86, 152.92, 152.99, 160.91, 165.84, 165.92, 166.01, 166.06, 176.41, 186.72, 186.81, 193.63, 193.74, 193.83, 197.48, 197.59, 197.76, 198.01, 199.25, 200.63, 200.73, 200.84, 200.94, 201.09, 201.17, 208.98, 209.19, 209.35, 213.84, 213.9, 215.1, 221.31, 221.41, 228.14, 235.78, 235.99, 242.33, 244.34, 247.5, 247.61, 247.89, 255.36, 255.48, 255.61, 255.71, 255.85, 262.12, 262.25, 263.48, 266.74, 266.87, 269.74, 271.04, 271.81, 271.99, 272.09, 274.52, 274.66, 275.52, 275.69, 275.81, 280.7, 280.82, 282.43, 285.9, 286.22, 287.31, 287.45, 293.84, 294.82, 295.12, 296.35, 296.52, 297.71, 297.81, 298.03, 298.31]</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>[0, -10, 0, -10, -10, 0, -10, 0, -20, -10, -20, -20, 0, -20, -10, -20, 0, 0, -10, -20, -10, -10, 0, -20, -10, 0, 0, -20, 0, -20, 0, 0, -10, -10, 0, 0, 0, -10, 0, 0, -20, -10, 0, 0, 0, 0, -20, 0, 0, 0, -20, 0, 0, 0, -10, -10, 0, -10, -20, -20, 0, -20, -20, 0, 0, 0, 0, -20, -10, 0, -10, 0, 0, -10, -20, 0, 0, 0, -20, -20, 0]</t>
+          <t>[0, -10, 0, -10, -20, -20, -20, 0, 0, -10, 0, -20, -10, 0, 0, 0, 0, 0, -10, -20, 0, -10, 0, 0, -10, -20, -10, -10, -20, 0, 0, -10, 0, -20, 0, -20, -10, -10, 0, 0, -20, 0, -20, 0, -20, -10, -20, -20, 0, 0, -10, 0, 0, 0, 0, 0, -20, 0, -20, -20, 0, -20, -10, 0, 0, -10, 0, -10, 0, 0, 0, -20, -20, -10, 0, 0, 0, -10, 0, 0, -10]</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -773,37 +773,37 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1']</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>[81, 93, 103, 108, 110]</t>
+          <t>[81, 93, 95, 102, 105, 155, 177, 177, 177, 177, 199, 208, 212, 212, 232, 280, 291, 291, 291, 291, 339, 382, 382, 384, 384, 410, 447, 499, 500, 514, 514, 514, 514, 529, 529, 557, 557, 558, 559, 594, 594, 594, 603, 603, 603, 603, 603, 603, 603, 603, 603, 632, 688, 688, 688, 725, 725, 740, 750, 750, 775, 775, 775, 775, 775, 783, 788, 793, 809, 809, 809, 814, 819, 823, 823, 855, 855, 866, 866, 866, 878, 878, 880, 880, 882, 882, 882, 882, 886, 886, 886, 886, 886, 889, 889, 894, 894, 894, 898, 923, 923, 923, 923, 923, 930, 930, 930, 946, 964, 964, 964, 966, 968, 979, 1022, 1045, 1045, 1045, 1045, 1045, 1060]</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>[0.342, 0.367, 0.382, 0.38, 0.389]</t>
+          <t>[0.342, 0.368, 0.383, 0.38, 0.389, 0.38, 0.393, 0.393, 0.393, 0.393, 0.393, 0.404, 0.404, 0.404, 0.419, 0.421, 0.419, 0.419, 0.419, 0.419, 0.414, 0.421, 0.421, 0.423, 0.423, 0.419, 0.417, 0.419, 0.423, 0.427, 0.427, 0.427, 0.427, 0.427, 0.427, 0.436, 0.436, 0.436, 0.436, 0.44, 0.44, 0.44, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.444, 0.445, 0.445, 0.445, 0.453, 0.453, 0.453, 0.457, 0.457, 0.455, 0.455, 0.455, 0.455, 0.455, 0.455, 0.455, 0.468, 0.468, 0.468, 0.468, 0.468, 0.483, 0.483, 0.483, 0.487, 0.487, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.492, 0.492, 0.492, 0.492, 0.498, 0.498, 0.498, 0.498, 0.498, 0.498, 0.498, 0.498, 0.498, 0.498, 0.498, 0.5, 0.5, 0.5, 0.5, 0.5, 0.504, 0.504, 0.504, 0.509, 0.517, 0.517, 0.517, 0.517, 0.517, 0.517, 0.517, 0.517, 0.517, 0.517, 0.517, 0.517, 0.519]</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>[0, 30, 60, 90, 120]</t>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>[0, 18.122868633270265, 33.505495166778566, 55.021463298797606, 78.26681461334229]</t>
+          <t>[0, 15.599844038486493, 39.92252010107041, 61.50258282423019, 83.81812008619309, 108.29061897993088, 117.5141192317009, 145.85904606580735, 157.71847506761551, 157.71847506761551, 167.0186748147011, 188.2887612462044, 204.98369106054307, 230.0372363448143, 250.9580525279045, 275.92000139951705, 283.96960161924363, 311.36969755887986, 324.2714017033577, 324.2714017033577, 331.8420206427574, 356.27668274641036, 368.3321212410927, 381.3566658616066, 397.4745683312416, 423.41541715860365, 432.6284672141075, 457.8207701086998, 471.70014315843576, 489.680476295948, 502.3413166761398, 526.772502207756, 541.1727509498596, 552.4990389347076, 568.9317914009094, 594.3831902503968, 603.942090511322, 626.2275892257691, 635.4610296726227, 644.0536835193634, 652.8287088632584, 654.4380086660385, 665.8558737516403, 686.2562942028045, 698.0133459329604, 720.2185351610183, 754.275580906868, 769.7233964681625, 787.8644694924354, 802.287596809864, 809.179055082798, 819.6407567501068, 846.0420042037964, 863.2675858736038, 890.1873346567154, 906.4433183431626, 921.2381395578385, 936.5248727679253, 954.9998687624932, 976.2805958390236, 984.7875034332276, 999.2008367538452, 1020.0522348403931, 1042.0963710546494, 1063.9209389448165, 1083.0756997823714, 1102.7319887578487, 1115.6981870353222, 1135.335101979971, 1141.9467406213282, 1147.0514737188814, 1163.2377247750758, 1173.8293295800684, 1194.7082797706125, 1220.1596786200998, 1233.2879774034022, 1260.7048511207101, 1274.8312523066995, 1296.915480583906, 1318.9385584294794, 1327.1137359321115, 1335.2101352870461, 1336.6378403842446, 1357.607651752233, 1376.3977153003211, 1398.1304530322548, 1431.2584489047524, 1451.830992478132, 1474.7892629086969, 1498.782061141729, 1505.543506711721, 1529.9780500829215, 1544.536490863561, 1557.48352779746, 1573.9162802636617, 1598.3887791573995, 1607.7799794137472, 1633.754094690084, 1647.5024271666998, 1668.7171103417868, 1677.836460155248, 1694.1720224559301, 1713.4451924741263, 1736.054258292913, 1759.716005557775, 1775.8768646180624, 1783.4827425420278, 1797.8301045358176, 1816.893444794416, 1822.0883037269111, 1827.163532298803, 1848.747120851278, 1865.8548022449013, 1887.0878552138802, 1908.9384854495522, 1934.3898842990395, 1941.9363845050332, 1969.3364804446694, 1977.7828969657419, 1977.7828969657419, 1985.8311467468736]</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>[0, 1.7, 2.8, 3.94, 5.02]</t>
+          <t>[0, 3.03, 3.06, 5.41, 6.52, 21.51, 27.26, 27.33, 27.37, 27.41, 31.46, 35.18, 35.22, 35.27, 40.87, 56.37, 60.86, 60.91, 60.97, 61.03, 73.67, 85.75, 85.91, 86.29, 86.49, 94.25, 103.57, 112.63, 112.71, 116.22, 116.39, 116.48, 116.57, 124.12, 124.18, 132.83, 132.95, 133.5, 134.21, 145.98, 146.09, 146.18, 148.98, 149.03, 149.19, 149.4, 149.47, 149.56, 149.63, 149.75, 149.83, 160.01, 174.48, 174.62, 174.69, 188.01, 188.08, 193.57, 195.61, 195.7, 204.93, 204.99, 205.29, 205.36, 205.42, 208.72, 211.42, 212.16, 217.03, 217.14, 217.38, 221.98, 223.27, 225.63, 225.85, 233.15, 233.26, 238.14, 238.4, 238.5, 243.67, 243.95, 245.79, 245.87, 247.13, 247.47, 247.6, 247.68, 248.77, 248.87, 249.01, 249.15, 249.3, 251.38, 251.46, 253.88, 254.15, 254.28, 256.06, 261.46, 261.58, 261.78, 261.91, 262.13, 264.75, 264.9, 265.0, 268.27, 272.66, 272.83, 272.9, 273.87, 274.51, 277.2, 285.57, 290.95, 291.35, 291.46, 291.57, 291.7, 297.41]</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>[0, -10, -10, 0, -10, -10, -10, -10, -10, -10, -10, 0, -10, -10, -10, -10, -10, -10, -20, 0, -20, -20, -20, -20, -20, -20, 0, 0, -20, -20, 0, -20, -20, -20, -20, 0, -20, -20, -20, -20, -10, -20, -10, -20, -10, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -20]</t>
+          <t>[0, -10, 0, 0, -10, -10, -10, -10, 0, -10, -20, 0, -20, -20, 0, 0, 0, -20, -20, 0, 0, 0, 0, 0, 0, -20, 0, 0, 0, 0, 0, -20, -20, -20, -20, 0, -20, -20, 0, -20, -10, -20, -20, 0, 0, -20, -20, -20, 0, 0, -10, -20, 0, -10, 0, 0, -10, 0, -10, -10, 0, -10, 0, -10, -10, -10, 0, 0, -10, 0, 0, 0, 0, -10, -10, 0, -10, 0, 0, 0, -20]</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -842,37 +842,37 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4']</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>[81, 91, 96, 101, 143]</t>
+          <t>[81, 91, 94, 99, 110, 165, 183, 183, 183, 183, 207, 225, 231, 232, 278, 325, 348, 348, 348, 348, 368, 368, 376, 376, 376, 377, 377, 397, 397, 397, 397, 397, 429, 429, 429, 429, 429, 466, 505, 505, 520, 540, 549, 553, 556, 580, 612, 612, 612, 612, 612, 612, 612, 622, 622, 631, 631, 650, 659, 659, 659, 659, 669, 669, 669, 669, 669, 695, 707, 707, 729, 738, 741, 749, 786, 804, 826, 826, 826, 826, 826, 826, 826, 826, 826, 846, 846, 850, 874, 874, 874, 874, 874, 874, 874, 875, 875, 896, 899, 899, 901, 901, 903, 903, 948, 960, 960, 964, 988, 988, 988, 988, 991, 997, 997, 997, 997, 997, 999, 999, 999]</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>[0.342, 0.365, 0.38, 0.378, 0.382]</t>
+          <t>[0.342, 0.365, 0.38, 0.378, 0.395, 0.383, 0.397, 0.397, 0.397, 0.397, 0.393, 0.397, 0.4, 0.398, 0.414, 0.41, 0.406, 0.406, 0.406, 0.406, 0.406, 0.406, 0.417, 0.417, 0.417, 0.417, 0.417, 0.427, 0.427, 0.427, 0.427, 0.427, 0.432, 0.432, 0.432, 0.432, 0.432, 0.457, 0.459, 0.459, 0.464, 0.462, 0.461, 0.462, 0.468, 0.466, 0.461, 0.461, 0.461, 0.461, 0.461, 0.461, 0.461, 0.466, 0.466, 0.47, 0.47, 0.472, 0.47, 0.47, 0.47, 0.47, 0.47, 0.47, 0.47, 0.47, 0.47, 0.474, 0.477, 0.477, 0.477, 0.476, 0.476, 0.476, 0.472, 0.476, 0.476, 0.476, 0.476, 0.476, 0.476, 0.476, 0.476, 0.476, 0.476, 0.474, 0.474, 0.474, 0.474, 0.474, 0.474, 0.474, 0.474, 0.474, 0.474, 0.477, 0.477, 0.479, 0.479, 0.479, 0.481, 0.481, 0.481, 0.481, 0.489, 0.491, 0.491, 0.491, 0.491, 0.491, 0.491, 0.491, 0.489, 0.491, 0.491, 0.491, 0.491, 0.491, 0.502, 0.502, 0.502]</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[0, 30, 60, 90, 120]</t>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>[0, 19.451510810852053, 34.31703748703003, 55.787382173538205, 77.6380124092102]</t>
+          <t>[0, 20.015534210205097, 35.3886614084244, 57.76824424266816, 80.54868853092196, 107.46843731403354, 116.18883755207065, 143.11651804447177, 156.43022680282596, 156.43022680282596, 165.9092765450478, 183.23147112131122, 206.34776228666308, 230.20679539442065, 253.45214670896536, 279.3929955363274, 288.9518957972527, 315.40703657865527, 328.1648222565651, 328.1648222565651, 337.10732201337817, 351.6809093117714, 374.94100073575976, 397.05100311040883, 420.3210754275322, 438.524113714695, 445.8796913743019, 459.8871405959129, 477.97664986848827, 494.03348656892774, 499.33220423460006, 522.3363573908806, 544.0326905131341, 564.523678791523, 589.2302194714547, 613.0189423918725, 632.1332167029382, 647.6325171828271, 658.1534167408944, 658.5731167435647, 675.5479664444924, 689.5232217907907, 712.1072103619576, 736.4347555279733, 754.5661295533181, 778.5491784691811, 787.1018787026406, 812.1398974061013, 822.5433026432992, 822.5433026432992, 832.022352385521, 845.4545464515687, 865.1293964624406, 887.0620051145555, 910.1864345312121, 926.1391150951388, 933.5533900260928, 943.959328556061, 965.9411855697634, 973.9696039199831, 979.6581483483317, 1001.8102958321574, 1024.9456690430643, 1049.7779986262324, 1075.7239241719249, 1098.7258895993236, 1116.0185008168223, 1133.1934013485911, 1148.112177217007, 1148.5318772196772, 1167.89168766737, 1183.7952859520913, 1198.580638039112, 1219.2795005440712, 1241.1301307797432, 1265.1131796956063, 1272.9950799107553, 1296.6158522725107, 1309.4553670287135, 1309.4553670287135, 1319.2921167612078, 1335.700281906128, 1357.6806370496752, 1382.1609096527102, 1404.8624549388887, 1427.385163855553, 1434.9547463178637, 1448.6826773405078, 1467.3942942857745, 1497.3497788667682, 1502.1919903755193, 1524.7701406955723, 1541.8485641956333, 1566.4794296979908, 1590.2185924291614, 1613.2808593988423, 1631.581760334969, 1649.5944608926777, 1665.5480311870579, 1665.967731189728, 1686.1889836311343, 1702.544434332848, 1722.2267539739612, 1746.1018038749698, 1769.8013394832615, 1790.1529243230823, 1797.1311630845073, 1807.920353496075, 1826.1016811251643, 1849.2424163699152, 1854.3705311417582, 1864.3731357932093, 1876.056283938885, 1896.0698530793193, 1909.327805030346, 1932.948840224743, 1966.087435948849, 1986.4345788359644, 2002.4012216210367, 2027.4701989769937, 2034.0789004802705]</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>[0, 2.59, 2.62, 3.52, 21.63]</t>
+          <t>[0, 2.42, 2.46, 3.46, 5.94, 18.96, 23.29, 23.34, 23.39, 23.44, 29.95, 34.78, 35.26, 36.09, 49.55, 66.1, 75.25, 75.32, 75.38, 75.51, 81.18, 81.35, 82.76, 82.82, 82.88, 84.84, 84.91, 91.86, 91.94, 92.0, 92.16, 92.26, 104.99, 105.15, 105.22, 105.37, 105.42, 114.11, 121.1, 121.29, 124.41, 130.49, 133.09, 135.53, 136.85, 142.85, 165.34, 165.46, 165.53, 165.62, 165.7, 165.79, 165.95, 169.43, 169.52, 173.37, 173.48, 179.42, 181.64, 181.73, 181.89, 182.03, 185.82, 185.9, 186.14, 186.22, 186.32, 194.43, 197.54, 197.78, 201.93, 205.98, 207.65, 210.28, 219.05, 223.4, 228.64, 229.03, 229.32, 229.41, 229.54, 229.64, 229.73, 229.82, 229.92, 239.58, 239.69, 241.47, 247.24, 247.36, 247.52, 247.63, 247.73, 247.93, 248.02, 248.19, 248.35, 254.57, 255.86, 256.0, 257.51, 257.76, 258.88, 258.96, 271.18, 274.38, 274.48, 275.8, 281.93, 282.09, 282.17, 282.3, 282.98, 285.68, 285.78, 285.89, 285.99, 286.12, 286.2, 286.32, 286.52]</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>[0, -10, -10, 0, -10, -10, -10, -10, -10, -10, -10, -10, -10, -10, -10, -10, -10, -10, -20, -20, -20, -20, -20, -20, -20, -20, 0, 0, -20, -20, 0, -20, -20, -20, -20, 0, -20, -20, -20, -20, -10, -10, -20, -10, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -20]</t>
+          <t>[0, -10, -10, 0, -10, -10, -10, -10, 0, -10, -10, 0, -10, -20, 0, -20, 0, -20, -20, 0, 0, 0, -20, 0, -20, -20, 0, 0, -20, 0, 0, -20, -20, -20, -20, 0, -20, -20, 0, -20, -10, -20, -20, 0, 0, -20, 0, -10, -20, 0, -10, 0, 0, 0, 0, 0, 0, -10, 0, 0, 0, 0, -10, 0, -10, -10, 0, -10, 0, 0, 0, 0, 0, -10, -10, 0, 0, -10, 0, 0, -20]</t>
         </is>
       </c>
     </row>
@@ -880,58 +880,208 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>clusterStdHigh</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5']</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>[81, 94, 96, 103, 107, 159, 161, 161, 161, 161, 178, 178, 178, 178, 178, 178, 178, 217, 264, 264, 285, 317, 317, 352, 352, 406, 443, 484, 504, 509, 518, 518, 520, 528, 528, 528, 528, 528, 528, 528, 528, 528, 531, 531, 531, 531, 531, 531, 531, 531, 531, 531, 533, 533, 533, 533, 533, 533, 558, 558, 558, 558, 595, 598, 598, 617, 617, 617, 619, 619, 619, 638, 690, 690, 690, 726, 726, 726, 752, 752, 782, 782, 782, 782, 782, 784, 784, 789, 789, 789, 789, 789, 789, 789, 789, 792, 793, 813, 831, 831, 831, 838, 853, 858, 861, 886, 892, 892, 892, 892, 912, 912, 912, 912, 912, 912, 912, 933, 935, 935, 953]</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>[0.342, 0.361, 0.376, 0.372, 0.385, 0.387, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.415, 0.417, 0.417, 0.425, 0.429, 0.429, 0.436, 0.436, 0.438, 0.436, 0.434, 0.444, 0.444, 0.453, 0.453, 0.453, 0.453, 0.453, 0.453, 0.453, 0.453, 0.453, 0.453, 0.453, 0.453, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.464, 0.464, 0.464, 0.464, 0.459, 0.459, 0.459, 0.461, 0.461, 0.461, 0.461, 0.461, 0.461, 0.464, 0.468, 0.468, 0.468, 0.477, 0.477, 0.477, 0.477, 0.477, 0.485, 0.485, 0.485, 0.485, 0.485, 0.485, 0.485, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.494, 0.492, 0.502, 0.502, 0.502, 0.506, 0.511, 0.511, 0.521, 0.515, 0.515, 0.515, 0.515, 0.515, 0.517, 0.517, 0.517, 0.517, 0.517, 0.517, 0.517, 0.519, 0.524, 0.524, 0.524]</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>[0, 18.365378999710085, 42.212937760353086, 64.14384310245514, 86.92428739070894, 112.37568624019625, 120.59298646450046, 147.52066695690158, 160.50351648330692, 160.50351648330692, 174.31592681407932, 194.55589582920075, 212.65902473926545, 233.12175636291505, 258.56231808662415, 280.6962848186493, 289.6433919429779, 305.9804924488068, 321.5386127471924, 321.9583127498627, 340.5591659069062, 360.64719691276554, 373.2572025060654, 380.86385178565985, 397.046566772461, 423.4768655776978, 431.69416580200203, 456.8864686965943, 474.6822892665864, 479.342796945572, 492.4858676314355, 519.2048602461816, 520.6325653433801, 540.4657123923303, 553.121444118023, 576.7439701437951, 610.795965898037, 632.2377037882806, 648.8236104249955, 659.9600732564927, 666.247017645836, 672.9656267881394, 686.2845815420151, 709.0440130233765, 723.6992715120316, 746.3694011926651, 772.7836478471756, 796.7540505170823, 811.1425416231157, 825.065940308571, 831.3528846979143, 837.7746976315977, 839.2664430677893, 859.7949203789236, 871.2669835627081, 895.3619753897192, 921.7325720846655, 946.2802881300452, 970.7066264212134, 985.4324225485327, 992.3238808214667, 996.2607846260073, 1013.8691474914554, 1035.2287237644198, 1049.5962138891223, 1072.273839068413, 1098.565235924721, 1119.9878790616992, 1141.3049690008168, 1165.6971676588062, 1172.990334606171, 1180.9609557449821, 1205.476400357485, 1224.3394468128683, 1249.301395684481, 1262.7153888285163, 1290.1322616636755, 1308.500624328852, 1327.8561866819862, 1349.1369136154653, 1359.1092213094237, 1373.8752153098585, 1394.7551052987578, 1419.941752547026, 1442.2412198722366, 1457.5613935172562, 1464.1657791316513, 1477.6509601533417, 1494.6418372094636, 1498.8921763360504, 1506.3533492743973, 1523.6719919621949, 1545.3552419364457, 1568.76670960784, 1591.0869829595094, 1606.9699019849306, 1614.211590892077, 1627.890040582419, 1645.6817682206636, 1650.0949145734314, 1655.4236483275895, 1675.9634231269365, 1701.2582029283053, 1723.0342855393892, 1744.8849157750612, 1769.357414668799, 1777.7424148976809, 1805.142510837317, 1817.5181947648532, 1817.5181947648532, 1826.6395445168025, 1847.7942317783838, 1865.214223748446, 1887.2011896669871, 1907.550350385905, 1930.5523158133037, 1949.2599034369, 1967.2726039946087, 1983.0894228994855, 1983.5091229021557, 1999.6309368669995]</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>[0, 2.91, 2.97, 6.43, 6.96, 22.0, 22.5, 22.56, 22.6, 22.66, 27.59, 27.72, 27.78, 27.83, 27.91, 27.99, 28.03, 36.31, 43.69, 43.77, 49.94, 56.74, 56.94, 67.42, 67.6, 77.26, 86.7, 96.87, 100.35, 101.95, 104.1, 104.21, 105.57, 109.02, 109.23, 109.31, 109.39, 109.49, 109.56, 109.65, 109.79, 109.91, 110.81, 110.91, 111.0, 111.27, 111.34, 111.44, 111.63, 111.71, 111.82, 111.91, 112.65, 112.73, 112.83, 112.94, 113.02, 113.13, 124.54, 124.67, 124.74, 124.85, 132.24, 133.84, 133.94, 136.33, 136.45, 136.56, 138.1, 138.22, 138.31, 145.23, 156.44, 156.68, 156.8, 165.5, 165.6, 165.69, 172.92, 173.21, 180.38, 180.65, 180.83, 181.07, 181.17, 182.05, 182.33, 182.69, 182.8, 182.95, 183.06, 183.17, 183.31, 183.4, 183.55, 184.27, 184.91, 191.39, 196.1, 196.4, 196.59, 199.81, 202.77, 204.55, 205.55, 212.68, 215.41, 215.53, 215.68, 215.82, 222.75, 222.83, 222.96, 223.09, 223.36, 223.48, 223.6, 231.97, 232.09, 232.18, 235.24]</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, -20, 0, 0, 0, 0, -10, 0, 0, 0, -20, -10, -10, -10, -20, 0, 0, -10, 0, -20, -10, -10, 0, -10, -20, -20, 0, -10, -20, 0, 0, 0, 0, -20, 0, 0, -20, -10, 0, 0, 0, -10, -20, 0, -10, 0, -10, -20, 0, 0, 0, 0, -10, -20, -10, 0, 0, -10, 0, 0, 0, -20, 0, 0, -20, 0, -20, -20, -10, -10, -20, 0, 0, 0, -20, -10, -20, -20, -10]</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5']</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>[81, 89, 95, 104, 133, 185, 212, 212, 212, 212, 227, 227, 262, 291, 291, 291, 291, 291, 291, 291, 291, 313, 353, 353, 353, 386, 386, 394, 405, 405, 409, 413, 415, 420, 423, 465, 469, 469, 469, 469, 493, 503, 514, 516, 538, 566, 567, 567, 567, 567, 575, 590, 617, 617, 617, 620, 620, 621, 629, 629, 661, 665, 670, 689, 713, 734, 734, 734, 734, 734, 738, 749, 754, 757, 796, 823, 841, 841, 841, 841, 841, 851, 854, 856, 873, 884, 884, 884, 884, 884, 894, 894, 930, 944, 945, 965, 965, 965, 992, 992, 992, 992, 1000, 1000, 1000, 1019, 1019, 1020, 1020, 1020, 1027, 1027, 1027, 1027, 1027, 1027, 1027, 1070, 1117, 1117, 1141]</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>[0.336, 0.365, 0.378, 0.368, 0.387, 0.376, 0.391, 0.391, 0.391, 0.391, 0.389, 0.389, 0.38, 0.383, 0.383, 0.383, 0.383, 0.383, 0.383, 0.383, 0.383, 0.374, 0.372, 0.372, 0.372, 0.378, 0.378, 0.385, 0.383, 0.383, 0.389, 0.391, 0.391, 0.391, 0.391, 0.397, 0.398, 0.398, 0.398, 0.398, 0.4, 0.414, 0.419, 0.419, 0.419, 0.414, 0.415, 0.415, 0.415, 0.415, 0.415, 0.414, 0.434, 0.434, 0.434, 0.434, 0.434, 0.43, 0.442, 0.442, 0.438, 0.444, 0.442, 0.445, 0.438, 0.43, 0.43, 0.43, 0.43, 0.43, 0.43, 0.442, 0.442, 0.44, 0.429, 0.43, 0.43, 0.43, 0.43, 0.43, 0.43, 0.442, 0.445, 0.447, 0.451, 0.453, 0.453, 0.453, 0.453, 0.453, 0.451, 0.451, 0.451, 0.451, 0.451, 0.453, 0.453, 0.453, 0.457, 0.457, 0.457, 0.457, 0.459, 0.459, 0.459, 0.468, 0.468, 0.468, 0.468, 0.468, 0.476, 0.476, 0.476, 0.476, 0.476, 0.476, 0.476, 0.479, 0.489, 0.489, 0.508]</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>[0, 17.680564260482797, 37.32974722385407, 62.21284482479095, 86.38801019191743, 111.83940904140474, 122.34273371696473, 150.21524510383608, 161.98343009948732, 161.98343009948732, 171.46247984170915, 179.58493937253954, 196.2414988398552, 219.67289487123492, 233.96053255796434, 257.58307470083236, 291.17307051420215, 311.50273960828787, 331.5046384930611, 363.04841157197956, 369.8124608755112, 376.8198463439942, 396.6207824230195, 407.1172011852265, 429.14245018959053, 442.30734548568734, 468.66193704009066, 481.1683201491834, 502.60417684912693, 524.3798014104367, 547.1060778796674, 561.9252231419088, 576.9997033655644, 594.7257574141026, 615.6465735971929, 636.2034726679326, 642.0333724439145, 668.9610529363156, 681.4867883861066, 681.4867883861066, 691.0100165188313, 708.9327596962453, 726.4710615217687, 739.1874226629735, 760.1082388460637, 786.5385376513005, 794.5881378710271, 818.6813256800176, 832.0190249741079, 832.0190249741079, 840.0672747552396, 851.6612129032613, 878.0624609291556, 897.4270364105704, 923.8573352158072, 931.4041316807272, 947.5067859530451, 961.1634786725047, 978.919037640095, 1001.4370160937311, 1011.0152502298357, 1025.2089368104937, 1044.0292961120608, 1065.9844555377963, 1087.8350857734683, 1108.391984844208, 1113.0875849723818, 1135.7634255409243, 1149.1387240648273, 1149.1387240648273, 1158.0464756369595, 1177.5512685179715, 1193.9960484623914, 1217.6724532246594, 1239.9879904866223, 1266.418289291859, 1274.9709895253186, 1302.3710854649548, 1313.1090111613278, 1313.1090111613278, 1329.4087748646741, 1342.0743093609815, 1358.7400564551358, 1382.245144975186, 1403.630868184567, 1428.5928170561795, 1437.070568776131, 1463.053418374062, 1476.1766992092137, 1476.1766992092137, 1484.4217570424084, 1488.0701646924024, 1505.2026258587841, 1523.747073423863, 1540.455092799664, 1564.0776164889342, 1596.2922123312956, 1616.7272186160094, 1638.35792452097, 1661.951322329045, 1668.2545163869866, 1676.393397837878, 1683.8436620533473, 1703.8521426975733, 1730.7718914806849, 1746.3085510075098, 1771.1950368464, 1785.2548207819468, 1811.085992389918, 1831.3769153893, 1841.3665612399584, 1861.388694542647, 1872.318885582686, 1898.4476539552218, 1921.0266762435442, 1945.3306397140032, 1962.9801316916949, 1980.9928322494036, 1993.9639664828783, 1994.3836664855485, 2017.0030824840073]</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>[0, 0.1, 0.14, 0.18, 0.24, 0.31, 0.39, 0.47, 0.55, 0.67, 0.78, 0.91, 1.01, 1.1, 1.24, 1.37, 1.45, 1.57, 1.68, 1.81, 1.93, 2.08, 2.21, 2.34, 2.75, 2.87, 3.01, 3.16, 3.32, 3.47, 3.61, 3.78, 3.95, 4.14, 4.3, 4.46, 4.64, 5.17, 5.33, 5.52, 5.73, 5.97, 6.23, 6.43, 6.99, 7.23, 7.46, 7.71, 7.91, 8.13, 8.45, 8.66, 8.94, 9.17, 9.48, 9.81, 10.29, 10.5, 10.8, 11.08, 11.42, 11.67, 11.98, 12.27, 12.54, 12.84, 13.14, 13.82, 14.12, 14.56, 15.03, 15.31, 15.68, 15.97, 16.31, 16.65, 17.07, 17.45, 17.83, 18.24, 18.58, 19.03, 19.38, 19.93, 20.26, 21.21, 22.09, 22.95, 23.33, 23.69, 24.18, 24.54, 24.98, 25.4, 25.88, 26.22, 26.68, 27.08, 27.79, 28.51, 29.44, 29.88, 30.43, 30.88, 31.27, 32.01, 32.79, 33.27, 33.74, 34.4, 35.0, 35.42, 36.24, 36.61, 37.26, 38.42, 38.97, 39.49, 39.97, 40.5, 41.06]</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>[-10, 0, -10, -10, 0, -10, 0, -10, 0, -20, 0, -20, -20, 0, 0, 0, 0, -20, 0, 0, 0, 0, 0, -20, 0, 0, 0, 0, -20, 0, -10, -20, 0, -10, -20, 0, 0, -20, 0, -10, 0, -20, -10, 0, -10, -20, 0, -10, 0, -20, 0, -10, 0, -10, 0, 0, 0, -20, 0, -10, -20, 0, -10, -10, 0, -20, 0, 0, -20, -10, -20, -10, -10, 0, -20, 0, -20, 0, -20, -10, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>redistrict</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1']</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>[81, 81, 95, 116, 137, 188, 214, 214, 214, 214, 237, 237, 283, 283, 283, 321, 321, 321, 336, 336, 347, 347, 347, 347, 347, 347, 347, 374, 401, 401, 401, 401, 401]</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>[0.336, 0.336, 0.385, 0.372, 0.398, 0.393, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.393, 0.393, 0.393, 0.389, 0.389, 0.389, 0.393, 0.393, 0.4, 0.4, 0.4, 0.4, 0.4, 0.4, 0.4, 0.412, 0.419, 0.419, 0.419, 0.419, 0.419]</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960]</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>[0, 20.71788024902342, 38.753924107551555, 65.48375976085663, 85.93966891765595, 110.9016177892685, 119.95741803646088, 146.88497126102448, 154.4052145957947, 154.4052145957947, 163.62591395378115, 180.37350366115572, 208.18910424709324, 230.62357096672062, 255.86722307205204, 270.00474715232855, 293.0375232160092, 304.182018083334, 328.80468079447746, 350.8277580440044, 364.5980957448482, 376.0378918111324, 387.2849316060543, 408.10341877341267, 429.8655682981014, 444.94796532988545, 452.7713741242885, 466.603038829565, 485.9531664311885, 510.98294128775586, 516.549529403448, 535.082922309637, 550.1574024856089]</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>[0, 0.0, 0.3, 0.68, 1.15, 1.88, 2.76, 2.76, 2.76, 2.76, 3.64, 3.64, 4.9, 4.9, 4.9, 6.52, 6.52, 6.53, 7.9, 7.9, 9.38, 9.38, 9.39, 9.39, 9.39, 9.39, 9.39, 11.16, 12.74, 12.74, 12.74, 12.74, 12.74]</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, -10, -20, 0, 0, -10, -10, 0, -10, -10, 0, -20, -10, 0, 0, -20, 0, 0, 0, 0, -20, -20, 0, -20, 0, -10, 0, 0, -20, -20, 0, 0, -10, -20, 0, -20, 0, 0, 0, -20, -20, -10, -10, 0, -20, 0, -10, -10, -10, 0, -20, 0, 0, -10, -10, 0, 0, 0, -10, -20, 0, -20, -10, 0, -10, -20, -20, 0, -10, 0, -20, 0, -20, 0, 0, 0, -10, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1032,134 +1182,484 @@
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>classWt</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4']</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>[100, 102, 104, 104, 145, 188, 211, 211, 211, 211, 236, 256, 256, 256, 256, 273, 273, 311, 370, 370, 392, 415, 436, 436, 436, 469, 469, 470, 481, 481, 495, 495, 529, 555, 555, 555, 555, 555, 572, 572, 572, 580, 622, 622, 622, 658, 658, 662, 666, 666, 693, 716, 716, 716, 716, 716, 717, 761, 821, 821, 835, 845, 852, 855, 858, 903, 914, 914, 914, 914, 926, 935, 935, 935, 935, 935, 935, 977, 1036, 1036, 1061, 1061, 1061, 1061, 1061, 1063, 1063, 1096, 1120, 1120, 1120, 1148, 1148, 1151, 1151, 1168, 1168, 1210, 1259, 1259, 1276, 1276, 1311, 1320, 1320, 1320, 1320, 1320, 1353, 1353, 1353, 1386, 1386, 1396, 1398, 1441, 1486, 1536, 1575, 1607, 1614, 1614, 1614, 1614, 1614, 1614, 1614, 1642, 1668, 1668, 1668, 1668, 1668, 1683, 1718, 1718, 1718, 1732, 1756, 1756, 1756, 1756, 1759, 1785, 1785, 1785, 1785, 1785, 1789, 1789, 1789, 1801, 1816, 1816, 1819, 1864, 1873, 1873, 1873, 1873, 1898, 1898, 1898, 1909, 1909, 1910, 1910, 1941, 1967, 1967, 1968, 1973, 1998, 2002, 2013, 2056, 2079, 2079, 2079, 2079, 2102, 2102, 2106, 2131, 2131, 2154, 2154, 2154, 2198, 2198, 2198, 2198, 2233, 2241, 2241, 2257, 2257, 2257, 2284, 2284, 2284, 2295, 2298, 2298, 2340, 2387, 2407, 2407, 2407, 2407, 2411, 2424, 2479, 2488, 2488, 2522, 2524, 2526, 2529, 2529, 2569, 2571, 2628, 2628, 2628, 2656, 2656, 2668, 2694, 2694, 2713, 2713, 2715, 2738, 2738, 2742, 2742, 2742, 2742, 2742, 2742]</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>[0.198, 0.197, 0.197, 0.197, 0.168, 0.174, 0.182, 0.182, 0.182, 0.182, 0.19, 0.192, 0.192, 0.192, 0.192, 0.196, 0.196, 0.198, 0.201, 0.201, 0.206, 0.209, 0.214, 0.214, 0.214, 0.226, 0.226, 0.227, 0.23, 0.23, 0.229, 0.229, 0.228, 0.23, 0.23, 0.23, 0.23, 0.23, 0.233, 0.233, 0.233, 0.232, 0.232, 0.232, 0.232, 0.232, 0.232, 0.234, 0.234, 0.234, 0.234, 0.235, 0.235, 0.235, 0.235, 0.235, 0.235, 0.237, 0.239, 0.239, 0.239, 0.244, 0.247, 0.248, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.251, 0.251, 0.252, 0.252, 0.252, 0.252, 0.252, 0.252, 0.252, 0.265, 0.266, 0.266, 0.266, 0.266, 0.266, 0.268, 0.268, 0.267, 0.267, 0.267, 0.268, 0.268, 0.269, 0.269, 0.268, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.266, 0.267, 0.266, 0.266, 0.268, 0.275, 0.274, 0.274, 0.274, 0.274, 0.274, 0.274, 0.274, 0.274, 0.284, 0.284, 0.284, 0.284, 0.284, 0.284, 0.284, 0.291, 0.291, 0.291, 0.291, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.293, 0.294, 0.294, 0.294, 0.295, 0.295, 0.295, 0.295, 0.295, 0.295, 0.295, 0.295, 0.294, 0.294, 0.294, 0.294, 0.3, 0.303, 0.303, 0.303, 0.304, 0.303, 0.306, 0.31, 0.309, 0.309, 0.309, 0.309, 0.309, 0.311, 0.311, 0.311, 0.312, 0.312, 0.312, 0.312, 0.312, 0.313, 0.313, 0.313, 0.313, 0.313, 0.313, 0.313, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.313, 0.313, 0.313, 0.313, 0.313, 0.313, 0.313, 0.314, 0.314, 0.32, 0.32, 0.32, 0.323, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.323, 0.323, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324, 0.324]</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600, 3630, 3660, 3690, 3720, 3750, 3780, 3810, 3840, 3870, 3900, 3930, 3960, 3990, 4020, 4050, 4080, 4110, 4140, 4170, 4200, 4230, 4260, 4290, 4320, 4350, 4380, 4410, 4440, 4470, 4500, 4530, 4560, 4590, 4620, 4650, 4680, 4710, 4740, 4770, 4800, 4830, 4860, 4890, 4920, 4950, 4980, 5010, 5040, 5070, 5100, 5130, 5160, 5190, 5220, 5250, 5280, 5310, 5340, 5370, 5400, 5430, 5460, 5490, 5520, 5550, 5580, 5610, 5640, 5670, 5700, 5730, 5760, 5790, 5820, 5850, 5880, 5910, 5940, 5970, 6000, 6030, 6060, 6090, 6120, 6150, 6180, 6210, 6240, 6270, 6300, 6330, 6360, 6390, 6420, 6450, 6480, 6510, 6540, 6570, 6600, 6630, 6660, 6690, 6720, 6750, 6780, 6810, 6840, 6870, 6900, 6930, 6960, 6990, 7020, 7050, 7080, 7110, 7140, 7170, 7200]</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>[0, 22.340562248230004, 36.88287279605868, 61.634798574447636, 83.02052178382874, 104.06687083244324, 111.78107104301453, 139.65345063209534, 152.65334823131562, 152.65334823131562, 162.13239797353745, 183.38027542829516, 192.23498999476436, 212.09224068522457, 236.9352372825146, 261.2558628737927, 280.3701371848584, 296.28833767771727, 311.9832093656064, 312.4029093682767, 333.41916341185583, 343.90867324471486, 362.62493992447867, 378.47864027619374, 402.95113916993154, 415.8422214090825, 441.403221744299, 452.12646363377576, 470.6853236496449, 492.70840149521825, 500.86936870217323, 508.29462920427324, 524.4752869725228, 546.5006130337715, 560.2961890339851, 582.0289189934731, 610.0696648001672, 634.3554116129876, 653.8076899647714, 670.1253862023354, 677.3795420765878, 691.6509842276574, 711.2521261572839, 728.8122861504556, 754.7531349778177, 768.9133387923242, 782.6122555196287, 791.2552079856397, 806.7836994588376, 828.0644234120847, 836.3806077063085, 856.6221762716772, 873.359031301737, 895.9157562077047, 919.8268078386785, 943.262772613764, 962.3770469248296, 980.8086474955084, 996.7622177898886, 997.1819177925589, 1016.1694716751578, 1035.2048420727256, 1054.8214446127417, 1073.8998951494696, 1095.2856183588506, 1117.3108673632146, 1126.0312676012518, 1152.4864077150824, 1164.7084574043752, 1164.7084574043752, 1173.6509571611882, 1193.6932872831821, 1209.545349341631, 1232.0239489614964, 1257.7578408539296, 1281.193805629015, 1299.4947065651418, 1317.0885071098805, 1332.646627408266, 1333.0663274109363, 1354.4727754890919, 1369.4083820164203, 1388.599386101961, 1413.6445343792439, 1435.9335986435412, 1450.6585297405718, 1458.222988885641, 1471.4669054687022, 1489.8267991006373, 1510.1339749276638, 1515.3323336422443, 1537.5753668129444, 1552.7537172019481, 1576.1677598416804, 1596.8991801917552, 1620.5205580890179, 1639.2281457126142, 1656.821946257353, 1672.4854339659214, 1672.9051339685916, 1687.8314926683902, 1689.06034258008, 1705.7169020473957, 1726.794499951601, 1740.5527519762516, 1764.6477419435978, 1788.5132887423038, 1809.9140896379947, 1832.9538667976856, 1849.1040598690508, 1855.6328143179414, 1879.1056991159915, 1889.7278056442735, 1900.4854567646978, 1914.2027798891065, 1935.249128937721, 1942.7956291437147, 1967.0189973115919, 1986.2868658065793, 2004.286597204208, 2016.4785267353054, 2033.841014051437, 2051.916613721847, 2074.5612998962397, 2095.7757285118096, 2109.7682589292517, 2115.0130812406533, 2129.2516765594473, 2144.240450906753, 2165.019886636733, 2169.9822614192954, 2188.9408147096624, 2205.3798158884038, 2225.922352409362, 2249.133574056624, 2262.5792524576177, 2267.3992193460454, 2281.623173999785, 2298.706046319007, 2322.319041466712, 2327.352825295924, 2334.7006253123272, 2336.604232108592, 2351.452499735354, 2359.6870551943766, 2380.9398415446267, 2413.6164373278602, 2435.524161994456, 2455.303991568087, 2479.4825859665857, 2486.132228851317, 2504.667218327521, 2524.305078792571, 2546.328121089934, 2567.713844299315, 2589.739093303679, 2598.4594935417163, 2623.969927692412, 2636.234183382987, 2636.234183382987, 2646.4286331057538, 2663.689525210856, 2682.9701648592936, 2704.1947378993023, 2725.821647632121, 2742.7318259358394, 2749.470945179461, 2762.708732450007, 2780.251622855662, 2797.2529793620097, 2801.6915534615505, 2823.775048983096, 2849.0051090836514, 2869.342544233798, 2890.728267443179, 2911.7746164917935, 2920.662716734408, 2946.6454619050014, 2956.2374869942655, 2956.2374869942655, 2967.0919850826253, 2974.868290233611, 2977.2477987289417, 2999.3909442186346, 3011.898446059226, 3033.6311712503425, 3063.987167477607, 3085.424536919593, 3109.3809011220924, 3130.574299788474, 3137.103040075301, 3143.151052325963, 3159.8076117932787, 3180.7800786674015, 3190.9983442485327, 3214.1484189212315, 3247.738414734601, 3267.7996660888184, 3288.91617950797, 3312.5095773160447, 3319.0383176028718, 3339.280294984578, 3356.843862527608, 3375.161327713727, 3397.47686497569, 3420.4810139358037, 3427.5244141280646, 3453.9796791732306, 3466.5362333953376, 3466.5362333953376, 3474.5844831764693, 3485.91231021285, 3506.915775054693, 3523.0137065589424, 3549.4440053641792, 3563.029429119825, 3577.1392311334607, 3589.1018335223193, 3609.2146462321275, 3629.7530219435685, 3637.8908656358713, 3654.629230475425, 3676.3630701303478, 3690.3318372726435, 3716.2726861000056, 3730.235582661628, 3755.596855425834, 3771.390786767005, 3790.084251546859, 3811.1175281763067, 3819.4465435504903, 3825.1949569225303, 3826.686702358722, 3847.7315793156617, 3858.0545295357697, 3880.2597203373903, 3911.077716505527, 3931.119873106479, 3950.5780201792713, 3963.8112184405322, 3971.307190597057]</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>[0, 0.49, 0.94, 1.36, 28.46, 40.18, 46.5, 46.86, 47.31, 47.72, 53.62, 58.31, 58.7, 59.12, 59.55, 65.46, 65.92, 86.26, 105.03, 105.46, 110.44, 117.12, 122.27, 122.75, 123.69, 133.81, 134.43, 135.1, 140.51, 141.1, 146.41, 147.08, 158.45, 165.31, 166.28, 167.49, 168.04, 168.6, 175.82, 176.8, 177.33, 183.2, 201.78, 202.3, 202.79, 215.72, 216.26, 219.58, 222.69, 223.39, 231.59, 239.83, 240.49, 241.14, 241.61, 242.14, 243.46, 263.38, 280.0, 280.46, 283.99, 287.88, 289.04, 289.61, 291.6, 302.88, 307.61, 308.47, 309.18, 309.77, 316.2, 321.29, 321.97, 322.54, 323.27, 323.92, 324.6, 344.91, 370.51, 372.0, 388.24, 388.74, 389.34, 389.97, 390.73, 392.72, 393.41, 405.56, 412.45, 413.87, 414.55, 422.4, 424.6, 426.34, 427.45, 435.43, 436.21, 452.32, 477.77, 478.41, 485.65, 486.33, 498.14, 501.38, 502.07, 502.77, 503.41, 504.04, 517.02, 517.63, 518.31, 531.36, 532.67, 538.74, 541.82, 572.4, 593.74, 614.38, 631.71, 656.96, 664.67, 665.64, 666.51, 667.2, 667.92, 668.69, 670.01, 679.96, 690.01, 691.29, 692.87, 693.81, 694.73, 702.41, 716.05, 716.68, 718.3, 723.82, 731.81, 733.31, 734.09, 735.05, 737.84, 746.2, 747.46, 751.25, 752.78, 753.59, 757.86, 759.16, 760.28, 766.0, 771.87, 772.52, 775.22, 794.2, 797.88, 799.41, 800.17, 802.06, 810.27, 810.99, 811.81, 817.95, 819.38, 821.2, 822.04, 842.82, 854.13, 855.58, 857.59, 863.74, 871.19, 876.01, 878.98, 895.26, 901.86, 902.9, 904.18, 905.04, 912.49, 914.1, 917.17, 923.77, 925.18, 933.53, 935.75, 937.36, 952.19, 952.9, 953.61, 955.56, 970.45, 973.85, 974.84, 981.51, 982.56, 985.06, 995.71, 996.4, 997.16, 1005.67, 1009.75, 1010.58, 1024.36, 1038.84, 1045.9, 1048.31, 1050.29, 1052.77, 1057.08, 1065.05, 1089.3, 1091.42, 1092.28, 1103.0, 1105.8, 1107.56, 1110.74, 1113.59, 1128.61, 1130.21, 1148.22, 1149.97, 1152.44, 1161.32, 1162.92, 1170.04, 1178.76, 1180.37, 1188.5, 1189.33, 1191.23, 1198.34, 1199.58, 1201.03, 1202.83, 1205.94, 1206.95, 1209.07, 1210.17]</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 0, 0, -10, 0, -10, 0, -10, -20, 0, 0, 0, 0, 0, 0, -10, -10, -10, -10, -10, 0, -10, 0, -20, -20, 0, -20, 0, 0, 0, -20, 0, 0, -20, -20, -20, 0, -20, -10, -10, -10, -10, -20, 0, 0, 0, 0, 0, 0, 0, 0, -20, -20, 0, -20, 0, 0, 0, 0, 0, -20, -20, 0, -20, -10, 0, -20, -20, -20, -20, -20, -20, -20, -20, -20, 0, 0, -10, -10, 0, -10, -10, 0, -10, 0, 0, -10, 0, 0, 0, -10, -10, 0, 0, -10, -10, -10]</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5']</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>[100, 113, 115, 125, 128, 175, 205, 205, 205, 205, 216, 249, 249, 266, 266, 307, 369, 404, 422, 425, 429, 433, 449, 452, 485, 530, 570, 570, 570, 570, 594, 596, 651, 651, 651, 682, 682, 688, 702, 702, 724, 724, 731, 755, 755, 755, 755, 755, 783, 783, 783, 794, 794, 794, 794, 794, 808, 850, 882, 882, 903, 903, 903, 903, 903, 903, 903, 907, 941, 941, 941, 968, 968, 970, 970, 1015, 1069, 1114, 1117, 1136, 1144, 1144, 1180, 1201, 1201, 1201, 1201, 1201, 1201, 1201, 1201, 1217, 1232, 1232, 1276, 1318, 1320, 1320, 1320, 1320, 1345, 1345, 1380, 1406, 1406, 1406, 1406, 1406, 1414, 1414, 1414, 1416, 1422, 1426, 1428, 1472, 1494, 1494, 1494, 1494, 1508, 1531, 1531, 1531, 1531, 1531, 1531, 1562, 1617, 1617, 1638, 1649, 1659, 1666, 1679, 1722, 1741, 1741, 1741, 1741, 1758, 1793, 1794, 1832, 1839, 1872, 1927, 1976, 1977, 1984, 1987, 2001, 2042, 2059, 2059, 2095, 2095, 2100, 2107, 2107, 2109, 2109, 2109, 2109, 2120, 2120, 2120, 2141, 2160, 2160, 2160, 2160, 2162, 2171, 2172, 2172, 2172, 2172, 2172, 2194, 2194, 2194, 2194, 2194, 2194, 2196, 2196, 2208, 2233, 2233, 2233, 2233, 2269, 2306, 2306, 2306, 2306, 2306, 2354, 2354, 2354, 2354, 2356, 2365, 2365, 2365, 2365, 2365, 2410, 2417, 2417, 2442, 2456, 2490, 2490, 2524, 2524, 2525, 2542, 2542, 2571, 2579, 2633, 2636, 2636, 2673, 2673, 2676, 2684, 2684, 2688, 2735, 2735, 2735, 2735, 2753, 2753, 2791, 2845, 2845, 2870]</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>[0.198, 0.194, 0.194, 0.191, 0.195, 0.196, 0.196, 0.196, 0.196, 0.196, 0.204, 0.203, 0.203, 0.201, 0.201, 0.2, 0.193, 0.196, 0.204, 0.204, 0.204, 0.204, 0.209, 0.21, 0.212, 0.212, 0.214, 0.214, 0.214, 0.214, 0.214, 0.216, 0.215, 0.215, 0.215, 0.225, 0.225, 0.227, 0.227, 0.227, 0.229, 0.229, 0.236, 0.236, 0.236, 0.236, 0.236, 0.236, 0.238, 0.238, 0.238, 0.24, 0.24, 0.24, 0.24, 0.24, 0.24, 0.245, 0.25, 0.25, 0.254, 0.254, 0.254, 0.254, 0.254, 0.254, 0.254, 0.259, 0.262, 0.262, 0.262, 0.263, 0.263, 0.263, 0.263, 0.262, 0.262, 0.262, 0.262, 0.261, 0.261, 0.261, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.263, 0.263, 0.263, 0.266, 0.267, 0.267, 0.267, 0.267, 0.267, 0.268, 0.268, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.267, 0.265, 0.266, 0.266, 0.265, 0.265, 0.265, 0.265, 0.265, 0.265, 0.266, 0.266, 0.266, 0.266, 0.266, 0.266, 0.265, 0.265, 0.265, 0.266, 0.266, 0.267, 0.266, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.272, 0.273, 0.274, 0.273, 0.273, 0.276, 0.276, 0.278, 0.277, 0.277, 0.277, 0.277, 0.277, 0.277, 0.277, 0.277, 0.277, 0.287, 0.288, 0.288, 0.288, 0.288, 0.288, 0.288, 0.288, 0.288, 0.288, 0.288, 0.288, 0.287, 0.287, 0.287, 0.287, 0.287, 0.287, 0.287, 0.287, 0.29, 0.292, 0.292, 0.292, 0.292, 0.292, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.291, 0.29, 0.291, 0.291, 0.291, 0.291, 0.291, 0.29, 0.29, 0.29, 0.29, 0.29, 0.291, 0.291, 0.291, 0.292, 0.292, 0.294, 0.294, 0.294, 0.297, 0.297, 0.297, 0.297, 0.297, 0.297, 0.297, 0.299, 0.3, 0.3, 0.3]</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600, 3630, 3660, 3690, 3720, 3750, 3780, 3810, 3840, 3870, 3900, 3930, 3960, 3990, 4020, 4050, 4080, 4110, 4140, 4170, 4200, 4230, 4260, 4290, 4320, 4350, 4380, 4410, 4440, 4470, 4500, 4530, 4560, 4590, 4620, 4650, 4680, 4710, 4740, 4770, 4800, 4830, 4860, 4890, 4920, 4950, 4980, 5010, 5040, 5070, 5100, 5130, 5160, 5190, 5220, 5250, 5280, 5310, 5340, 5370, 5400, 5430, 5460, 5490, 5520, 5550, 5580, 5610, 5640, 5670, 5700, 5730, 5760, 5790, 5820, 5850, 5880, 5910, 5940, 5970, 6000, 6030, 6060, 6090, 6120, 6150, 6180, 6210, 6240, 6270, 6300, 6330, 6360, 6390, 6420, 6450, 6480, 6510, 6540, 6570, 6600, 6630, 6660, 6690, 6720, 6750, 6780, 6810, 6840, 6870, 6900, 6930, 6960, 6990, 7020, 7050, 7080, 7110, 7140, 7170, 7200]</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>[0, 18.774275875091554, 33.893252921104434, 56.75506417751312, 68.84264686107635, 91.84679582118987, 100.60479620695114, 128.00489214658737, 141.07994428873062, 141.07994428873062, 150.02244404554366, 172.5163025736809, 185.9257399439812, 195.6975139856339, 212.380441403389, 232.447890496254, 242.84529078006747, 259.80149662494665, 277.37263660430915, 279.70289044380195, 295.9526650071145, 318.2058214306832, 340.9993288159371, 366.08059741258626, 387.93122764825824, 409.95647665262226, 420.50575193166736, 447.9058478713036, 458.03635426759723, 458.03635426759723, 467.15770401954654, 482.76613318920135, 503.7536221265793, 520.0203052043914, 545.9611540317535, 560.0020063877105, 576.3549344837664, 588.0178556740283, 606.2737878382205, 624.8325614273547, 633.764834743738, 638.8624914824961, 647.4788032233714, 668.2390016973018, 679.6617474496363, 701.3944848477839, 728.8218321740626, 742.1400303781031, 759.8768053948878, 782.5978032052516, 789.005650371313, 810.0318201959133, 820.4300871193409, 840.6479471981526, 865.744800144434, 889.1807649195194, 906.3156596720219, 923.9094602167606, 935.4235038280488, 935.8432038307191, 956.0416058540345, 975.0392582654954, 981.0644581556321, 1004.7455683469773, 1026.1160429239274, 1043.4240046262742, 1050.536977016926, 1063.9886752963066, 1083.3712708830833, 1105.2627251982688, 1110.3926673412323, 1132.41098279953, 1147.2484227597713, 1160.2745661914348, 1177.1847930967808, 1199.2100421011448, 1208.2658423483372, 1230.0668736994267, 1245.1739836275578, 1261.2946137964727, 1272.209213680029, 1297.456958526373, 1314.5894196927547, 1337.1297148406506, 1352.4690960586072, 1374.201832598448, 1400.328429669142, 1419.5204867064956, 1442.7911889374259, 1459.188185912371, 1465.5960236012938, 1484.686961358786, 1510.114457291365, 1528.5499233663086, 1550.8654606282714, 1571.4223596990112, 1578.8375367701058, 1605.2928018152718, 1617.5148196518426, 1617.5148196518426, 1626.9938693940644, 1633.2606300413613, 1649.917189508677, 1669.941518503428, 1682.6991703808312, 1706.3217094719414, 1731.60630620122, 1753.4878201782708, 1771.6399697005754, 1797.37756792903, 1804.389928978682, 1825.9693287074572, 1845.5311641395099, 1867.894434136153, 1888.8152503192432, 1910.3510493457325, 1918.0652495563038, 1944.992930048705, 1956.1542635142812, 1956.1542635142812, 1961.6986133635053, 1980.533623844386, 1990.5031298577794, 2011.7585698783407, 2033.9163988053808, 2055.1823668420325, 2070.6364609658726, 2083.6223613679417, 2098.145687240363, 2098.565387243033, 2116.718445962668, 2133.037854474783, 2151.250371617079, 2173.285902088881, 2195.601439350844, 2216.6477883994585, 2223.1478138864045, 2242.989262670279, 2255.6275300443176, 2255.6275300443176, 2264.5700298011307, 2288.042941445113, 2301.529947495461, 2307.8360608637336, 2324.4160609900955, 2340.5679102599624, 2349.7914105117325, 2373.530311316252, 2386.001078265906, 2390.4115740716466, 2414.8034792006024, 2423.6142072618018, 2445.4529760301125, 2458.652053350211, 2482.1456522881995, 2496.780249327422, 2520.0555881261835, 2532.249125611783, 2552.739950859547, 2573.7732268929485, 2590.7451765537267, 2608.8400372266774, 2626.9081672668462, 2650.6902949571613, 2675.7975466489797, 2692.7516036272054, 2700.2522018671043, 2721.380362796784, 2734.5997031927113, 2746.406200766564, 2751.7067114710812, 2758.633572751284, 2760.061277848483, 2777.3770094692713, 2794.6084351122386, 2815.868704038859, 2848.9966999113567, 2869.5605065882214, 2889.3708496868617, 2903.0554443657406, 2908.7378664672383, 2924.9450654685506, 2940.2089051902303, 2964.448226970435, 2987.2121906697757, 3002.503522247077, 3009.5234579980383, 3022.8026572167882, 3040.2751295268545, 3053.0261469066154, 3058.4498005568994, 3068.504958444835, 3085.637419611217, 3108.7455983221544, 3122.4624635040773, 3145.1401027023803, 3177.8111486256134, 3199.306928855182, 3223.587328964473, 3245.730323368312, 3252.2590733110915, 3264.226976662875, 3265.654681760074, 3284.6303136885176, 3298.2349824726593, 3321.8575128376497, 3353.9848087608825, 3378.865342742206, 3403.6076705515397, 3419.6647957861437, 3425.830828279258, 3438.2903273642078, 3460.4619226515306, 3471.265498739482, 3498.6746975004685, 3511.844640642406, 3524.18887358308, 3538.1400706827653, 3559.636635619403, 3580.1750116407884, 3589.1735187232507, 3603.1211391627803, 3623.6236167609704, 3637.4719803512107, 3662.4339292228233, 3678.6899129092703, 3692.805960816146, 3703.452776390315, 3726.0433152735245, 3745.839339786769, 3757.7054207384595, 3779.096448236705, 3787.6037993788727, 3808.252769291402, 3832.893620097638, 3857.2142456889164, 3873.075026500226, 3888.993226993085, 3903.405305516721, 3903.825005519391, 3925.202866780759]</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>[0, 4.38, 4.75, 8.76, 10.21, 21.87, 28.23, 28.63, 29.06, 29.49, 31.59, 40.52, 40.97, 46.15, 46.56, 57.02, 80.89, 92.2, 97.96, 99.49, 101.92, 104.81, 110.05, 111.39, 121.56, 136.38, 149.99, 150.47, 150.92, 151.45, 160.46, 162.11, 178.78, 180.23, 181.84, 197.38, 197.96, 200.64, 209.18, 209.68, 217.86, 218.86, 220.97, 227.12, 227.6, 228.56, 229.08, 229.64, 237.86, 238.36, 238.78, 242.92, 244.01, 244.57, 245.13, 245.68, 252.05, 266.8, 277.38, 278.04, 283.5, 286.19, 287.21, 287.93, 288.48, 290.1, 291.04, 292.39, 306.53, 307.13, 308.12, 317.83, 318.42, 320.58, 321.16, 334.21, 350.83, 369.05, 372.55, 381.72, 386.71, 387.32, 405.9, 413.73, 414.46, 414.95, 416.31, 418.42, 419.32, 420.02, 420.67, 426.68, 433.67, 434.9, 446.78, 461.2, 462.87, 464.41, 465.68, 466.37, 485.48, 487.0, 497.18, 507.15, 507.82, 508.47, 509.22, 509.85, 515.9, 516.6, 517.36, 520.26, 524.21, 527.91, 530.33, 557.29, 573.2, 575.08, 575.88, 576.99, 583.73, 590.61, 591.3, 591.91, 592.67, 594.19, 595.19, 610.0, 626.45, 628.39, 635.66, 639.37, 642.88, 645.99, 653.64, 671.27, 675.51, 676.69, 678.2, 679.38, 686.64, 694.81, 695.99, 710.09, 713.95, 721.09, 740.82, 753.15, 754.31, 762.16, 764.53, 768.02, 780.73, 785.42, 786.11, 793.9, 796.75, 801.19, 804.26, 805.04, 807.75, 808.99, 811.57, 812.4, 818.5, 820.4, 821.23, 828.18, 836.36, 839.01, 840.5, 841.33, 843.19, 847.11, 848.87, 850.08, 851.23, 852.09, 852.83, 864.26, 865.04, 865.99, 867.83, 869.17, 870.35, 873.0, 874.5, 881.72, 892.05, 893.45, 895.57, 896.38, 910.49, 924.19, 925.65, 927.23, 929.21, 930.04, 949.97, 951.4, 952.52, 953.35, 955.61, 961.45, 962.76, 964.27, 965.13, 966.81, 982.06, 988.89, 990.83, 997.45, 1007.0, 1020.89, 1021.61, 1032.26, 1033.04, 1034.73, 1039.57, 1040.82, 1052.49, 1057.48, 1070.89, 1073.51, 1074.81, 1087.39, 1088.09, 1090.43, 1094.04, 1095.42, 1099.88, 1115.7, 1116.43, 1117.68, 1118.92, 1123.93, 1125.36, 1136.0, 1151.92, 1153.63, 1163.48]</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>[-20, -20, -10, -10, 0, -10, -10, 0, -10, -20, 0, -20, 0, 0, 0, 0, 0, 0, 0, -10, 0, -10, 0, 0, 0, -20, -20, 0, -10, 0, -20, 0, 0, 0, -20, 0, -10, -10, -10, -20, -10, 0, 0, -20, 0, -20, -10, -20, -10, -10, 0, -20, 0, 0, 0, 0, -10, 0, 0, -20, 0, -10, 0, -10, 0, -20, 0, -10, 0, 0, -10, -20, -20, -20, -20, -20, 0, 0, 0, 0, 0, -10, 0, -10, -10, -10, 0, -20, -20, -20, 0, -20, 0, -10, 0, 0, 0, 0, -20, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>clusterWt</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5']</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>[100, 108, 110, 110, 118, 166, 189, 189, 189, 189, 196, 240, 240, 240, 240, 240, 241, 279, 340, 340, 346, 346, 362, 362, 402, 403, 403, 417, 446, 446, 449, 487, 487, 495, 500, 547, 605, 657, 658, 675, 680, 711, 711, 718, 721, 764, 822, 870, 872, 880, 890, 892, 923, 925, 925, 948, 948, 956, 966, 966, 971, 985, 987, 987, 990, 1033, 1054, 1054, 1054, 1054, 1079, 1082, 1137, 1137, 1137, 1170, 1170, 1171, 1181, 1181, 1191, 1191, 1191, 1191, 1191, 1194, 1197, 1225, 1251, 1251, 1251, 1251, 1286, 1314, 1314, 1314, 1314, 1314, 1322, 1322, 1322, 1329, 1331, 1348, 1389, 1433, 1455, 1455, 1455, 1455, 1464, 1498, 1498, 1516, 1517, 1556, 1606, 1649, 1650, 1655, 1660, 1660, 1660, 1660, 1660, 1660, 1670, 1698, 1719, 1719, 1719, 1726, 1762, 1764, 1764, 1799, 1799, 1803, 1840, 1840, 1853, 1896, 1896, 1896, 1896, 1896, 1900, 1942, 2001, 2001, 2017, 2017, 2017, 2017, 2017, 2019, 2019, 2035, 2074, 2074, 2074, 2110, 2110, 2120, 2121, 2163, 2213, 2260, 2261, 2275, 2280, 2321, 2323, 2336, 2336, 2378, 2436, 2488, 2523, 2576, 2589, 2602, 2649, 2658, 2658, 2673, 2685, 2690, 2696, 2696, 2707, 2707, 2741, 2767, 2767, 2767, 2767, 2767, 2789, 2789, 2794, 2794, 2828, 2850, 2851, 2851, 2851, 2851, 2856, 2856, 2856, 2856, 2860, 2874, 2874, 2874, 2874, 2875, 2905, 2924, 2925, 2937, 2937, 2937, 2937, 2937, 2937, 2980, 3034, 3034, 3057, 3060, 3060, 3060, 3060, 3060, 3060, 3105, 3165, 3165, 3186]</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>[0.198, 0.193, 0.193, 0.193, 0.192, 0.191, 0.195, 0.195, 0.195, 0.195, 0.204, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.209, 0.209, 0.217, 0.217, 0.218, 0.22, 0.22, 0.229, 0.233, 0.233, 0.236, 0.237, 0.237, 0.238, 0.237, 0.236, 0.234, 0.235, 0.235, 0.234, 0.234, 0.234, 0.234, 0.234, 0.235, 0.236, 0.234, 0.234, 0.234, 0.234, 0.235, 0.238, 0.24, 0.242, 0.242, 0.25, 0.25, 0.253, 0.253, 0.253, 0.256, 0.257, 0.258, 0.258, 0.258, 0.258, 0.258, 0.258, 0.258, 0.258, 0.258, 0.257, 0.257, 0.257, 0.257, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.262, 0.265, 0.265, 0.265, 0.265, 0.265, 0.269, 0.269, 0.269, 0.269, 0.269, 0.269, 0.271, 0.271, 0.271, 0.271, 0.272, 0.28, 0.286, 0.286, 0.286, 0.286, 0.286, 0.286, 0.286, 0.286, 0.286, 0.286, 0.286, 0.286, 0.287, 0.287, 0.287, 0.287, 0.287, 0.287, 0.287, 0.287, 0.287, 0.287, 0.286, 0.291, 0.292, 0.292, 0.292, 0.293, 0.292, 0.296, 0.296, 0.295, 0.295, 0.296, 0.297, 0.297, 0.297, 0.297, 0.297, 0.297, 0.297, 0.297, 0.297, 0.298, 0.298, 0.298, 0.301, 0.301, 0.301, 0.301, 0.301, 0.301, 0.301, 0.306, 0.31, 0.31, 0.31, 0.31, 0.31, 0.31, 0.31, 0.31, 0.31, 0.308, 0.309, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.307, 0.308, 0.31, 0.31, 0.31, 0.315, 0.315, 0.315, 0.315, 0.315, 0.315, 0.315, 0.315, 0.315, 0.315, 0.315, 0.315, 0.316, 0.316, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.317, 0.317, 0.318, 0.319, 0.319, 0.319, 0.319, 0.319, 0.319, 0.319, 0.319, 0.321, 0.321, 0.321, 0.321, 0.321, 0.321, 0.321, 0.321, 0.321, 0.321, 0.322, 0.322, 0.322]</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600, 3630, 3660, 3690, 3720, 3750, 3780, 3810, 3840, 3870, 3900, 3930, 3960, 3990, 4020, 4050, 4080, 4110, 4140, 4170, 4200, 4230, 4260, 4290, 4320, 4350, 4380, 4410, 4440, 4470, 4500, 4530, 4560, 4590, 4620, 4650, 4680, 4710, 4740, 4770, 4800, 4830, 4860, 4890, 4920, 4950, 4980, 5010, 5040, 5070, 5100, 5130, 5160, 5190, 5220, 5250, 5280, 5310, 5340, 5370, 5400, 5430, 5460, 5490, 5520, 5550, 5580, 5610, 5640, 5670, 5700, 5730, 5760, 5790, 5820, 5850, 5880, 5910, 5940, 5970, 6000, 6030, 6060, 6090, 6120, 6150, 6180, 6210, 6240, 6270, 6300, 6330, 6360, 6390, 6420, 6450, 6480, 6510, 6540, 6570, 6600, 6630, 6660, 6690, 6720, 6750, 6780, 6810, 6840, 6870, 6900, 6930, 6960, 6990, 7020, 7050, 7080, 7110, 7140, 7170, 7200]</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>[0, 21.079954481124897, 42.39731462001802, 65.5722112417221, 78.58960797786712, 102.0832069158554, 110.97130715847015, 137.42649095058442, 150.20809309482576, 150.20809309482576, 158.931992661953, 180.7793182253838, 198.19931019544606, 218.32850269079213, 243.12100256681447, 264.4766212821007, 280.9037280917168, 296.8219285845757, 312.8974460959435, 313.3171460986138, 334.7520487666131, 355.335753619671, 376.20817397832883, 398.2372458577157, 421.99919973611844, 437.65969942808164, 445.2665114641191, 457.3654434204103, 476.077060365677, 482.6886990070345, 488.0555523872377, 509.98046097755446, 524.6065307557584, 536.8017443418504, 553.6195619225504, 576.6237108826639, 586.3503111481668, 611.5426140427592, 621.8477768778803, 630.4520912289621, 640.3468912601472, 659.9869166374208, 668.7198455095293, 680.748482656479, 695.7299294352533, 716.7762784838678, 726.5028787493708, 749.757312190533, 765.4230634093287, 798.0466171622279, 818.5310253381732, 833.8546643733981, 856.5966079711917, 871.7911934852604, 898.2214922904972, 910.2676566600803, 922.4618760406975, 937.5875424444679, 959.03028061986, 978.0839542210106, 987.1602814257149, 1005.8924244225029, 1020.5362842142586, 1044.306419283152, 1065.2272354662423, 1086.2735845148568, 1093.6523847162728, 1119.6351168692115, 1131.3011012613777, 1131.3011012613777, 1140.9590009987357, 1157.5366815268997, 1178.5401469886306, 1195.276138132811, 1218.7697370707992, 1233.3327922523026, 1258.1345509469513, 1272.1028129518036, 1290.4870431602005, 1311.2728667676452, 1316.1989547193052, 1331.5062545239928, 1346.338535732031, 1368.0356618106366, 1391.30573412776, 1407.054953712225, 1414.2850899875164, 1425.2627780497073, 1443.8337056696414, 1454.6956834375858, 1459.9138767302036, 1466.3965875208378, 1483.0531469881535, 1506.0710031807423, 1515.3499368727207, 1538.5000268042088, 1572.0900226175786, 1592.460628706217, 1612.4849562942984, 1623.266632896662, 1629.544477015734, 1640.2557363569738, 1653.88299549222, 1675.7500854790212, 1696.6709016621114, 1718.2067006886007, 1726.9549005806448, 1755.7722428619863, 1769.5600978434088, 1769.5600978434088, 1779.217997580767, 1802.6875027477743, 1813.568749266863, 1819.9284924447538, 1835.6395227372648, 1854.7280718743802, 1863.113072103262, 1883.9449821412566, 1896.4978806197646, 1899.294185227156, 1906.7831352531914, 1915.54890075326, 1932.3763049185281, 1952.3106921255594, 1972.2564683973794, 1989.599335199595, 1996.3157210648067, 2006.623753803969, 2019.9837835252292, 2040.7632192552096, 2044.5303157508379, 2057.29478211999, 2081.3387758791455, 2098.352481681109, 2124.293330508471, 2138.932312303782, 2152.1249073505405, 2161.687568569184, 2176.2728327274326, 2196.3163075447087, 2208.659586322308, 2229.6246109843255, 2242.9896119236946, 2264.1837740540504, 2288.616137063503, 2311.7524039149284, 2328.0222408652307, 2345.6160414099695, 2361.1741617083553, 2361.5938617110255, 2382.2159134268763, 2402.1904002308847, 2421.0693598866465, 2444.26282273531, 2467.532895052433, 2483.4304116845133, 2490.637402379513, 2512.572845995426, 2531.8796882271768, 2554.0759036660197, 2579.521915853024, 2602.49844044447, 2615.464899384976, 2630.416660368443, 2642.0945978164677, 2662.6514968872075, 2670.9842461347585, 2693.754212212563, 2707.1934182405475, 2719.7027427434923, 2730.9943875908853, 2754.4707483887673, 2767.7848949313166, 2776.877487021685, 2791.834887725115, 2812.391786795855, 2822.1183870613577, 2847.31068995595, 2867.5534023821356, 2892.254093080759, 2904.6395654022695, 2911.0653937339785, 2930.505197858811, 2949.8255323648455, 2973.8085812807085, 2984.7805278062824, 2996.376355415583, 3009.930697768927, 3031.886628001929, 3052.672452491522, 3061.3208623468877, 3067.012224954367, 3083.1928827226166, 3100.928763765097, 3111.0297893226148, 3134.1798801124096, 3167.7804757773874, 3189.162181919813, 3213.597966235876, 3244.8159380376337, 3251.132782500982, 3256.7936956346034, 3272.974353402853, 3294.4138523995875, 3307.9074005782604, 3328.6817352473736, 3356.1353309333326, 3376.1130873382094, 3396.84035038352, 3410.4597458302974, 3417.2302812993526, 3427.5213375747203, 3438.4094441115853, 3456.878958123922, 3470.071010273695, 3493.221092575788, 3523.608638876676, 3547.774322193861, 3571.591941708326, 3588.786132782697, 3594.3957555830475, 3614.3861726582045, 3629.4590159475797, 3654.470008569955, 3678.866564637422, 3701.868530064821, 3720.576117688417, 3738.588818246126, 3752.853445512056, 3753.2731455147264, 3773.4677967369553, 3794.421501690149, 3811.841493660211, 3835.426172453165, 3858.8623326122756, 3883.166296082735, 3900.2470768749713, 3919.09757745862, 3934.9143963634965, 3935.3340963661667, 3956.3556970894333]</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>[0, 2.74, 3.18, 3.63, 6.18, 17.26, 21.35, 21.72, 22.15, 22.52, 24.14, 34.93, 35.37, 35.76, 36.21, 37.19, 38.61, 54.13, 72.67, 73.44, 75.46, 75.95, 81.24, 81.66, 95.02, 96.13, 96.64, 102.38, 116.97, 117.57, 119.26, 129.1, 130.07, 133.47, 135.98, 157.22, 166.62, 182.89, 184.25, 189.16, 191.73, 202.93, 203.9, 208.04, 209.04, 224.2, 262.85, 278.6, 280.49, 284.64, 288.86, 290.97, 298.64, 300.06, 300.78, 310.49, 312.44, 316.46, 320.69, 322.25, 325.48, 328.77, 329.73, 331.11, 333.94, 344.36, 350.27, 351.47, 352.12, 353.19, 367.94, 370.32, 385.96, 386.57, 387.84, 397.37, 398.8, 400.39, 410.62, 411.26, 417.58, 418.23, 418.84, 419.88, 420.49, 423.68, 425.7, 435.55, 443.21, 443.77, 444.39, 445.75, 458.66, 468.47, 469.86, 470.66, 471.44, 472.07, 476.21, 476.9, 477.58, 479.4, 480.29, 483.82, 495.26, 508.64, 521.08, 521.85, 522.6, 523.17, 528.08, 537.02, 537.83, 543.69, 547.23, 568.84, 597.82, 613.3, 615.23, 619.18, 623.18, 624.63, 626.16, 627.44, 628.83, 629.63, 634.21, 643.75, 653.93, 655.64, 657.63, 661.66, 670.25, 671.03, 672.4, 685.96, 687.78, 691.08, 700.66, 702.32, 709.39, 720.17, 720.81, 721.97, 722.79, 723.73, 727.23, 746.01, 763.69, 764.92, 774.8, 776.0, 777.17, 778.0, 778.96, 781.28, 782.18, 791.64, 803.59, 805.5, 806.28, 817.98, 819.72, 824.25, 824.99, 837.0, 851.7, 867.63, 869.0, 874.0, 877.64, 890.04, 892.02, 896.37, 897.65, 913.46, 933.92, 949.21, 957.27, 978.21, 989.46, 997.82, 1021.02, 1025.91, 1027.36, 1032.99, 1039.18, 1045.02, 1049.08, 1050.89, 1055.54, 1056.56, 1066.53, 1077.75, 1080.16, 1081.49, 1083.03, 1083.9, 1095.68, 1097.71, 1099.32, 1100.11, 1111.19, 1118.15, 1119.49, 1122.65, 1124.11, 1125.54, 1128.64, 1130.08, 1131.1, 1132.77, 1136.14, 1143.25, 1144.14, 1145.19, 1146.46, 1148.07, 1162.71, 1173.7, 1175.45, 1184.48, 1186.27, 1189.3, 1191.35, 1192.36, 1195.38, 1209.34, 1224.22, 1224.99, 1234.75, 1238.55, 1240.35, 1241.49, 1242.43, 1243.48, 1244.46, 1260.08, 1280.79, 1282.25, 1288.47]</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, -10, 0, 0, -10, 0, -10, 0, -10, -20, 0, 0, 0, -20, 0, 0, -20, 0, -20, 0, 0, 0, 0, 0, -20, -10, -10, -20, 0, 0, 0, -10, 0, 0, -10, -20, -20, 0, -20, 0, -20, -20, -20, -20, -20, 0, 0, 0, -20, 0, 0, -20, -20, -20, 0, -20, 0, 0, 0, 0, 0, -20, -20, 0, -10, -20, 0, -10, -20, -10, -10, 0, 0, -10, -10, 0, 0, -10, -10, -10, 0, -10, -10, 0, -10, 0, 0, -10, 0, 0, 0, -10, -10, -10, 0, -10, -20, -20]</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>clusterStdLow</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4']</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>[100, 109, 117, 123, 167, 216, 236, 236, 236, 236, 254, 254, 276, 289, 289, 289, 289, 289, 289, 314, 314, 314, 320, 349, 349, 388, 388, 388, 388, 388, 388, 394, 420, 427, 427, 463, 463, 465, 470, 470, 477, 479, 525, 525, 525, 529, 529, 529, 532, 532, 544, 550, 603, 605, 605, 646, 646, 646, 649, 649, 652, 689, 689, 711, 711, 753, 807, 859, 862, 865, 868, 879, 888, 900, 923, 966, 980, 980, 980, 980, 998, 998, 998, 998, 1015, 1022, 1022, 1042, 1064, 1064, 1064, 1067, 1067, 1067, 1067, 1067, 1067, 1110, 1132, 1132, 1132, 1135, 1152, 1156, 1156, 1191, 1191, 1199, 1202, 1202, 1204, 1224, 1224, 1224, 1224, 1224, 1224, 1264, 1325, 1325, 1349, 1376, 1376, 1376, 1376, 1376, 1390, 1433, 1489, 1489, 1513, 1513, 1513, 1513, 1513, 1513, 1513, 1564, 1589, 1589, 1589, 1629, 1629, 1684, 1686, 1725, 1774, 1822, 1825, 1836, 1842, 1860, 1860, 1860, 1860, 1860, 1860, 1903, 1958, 1958, 1978, 1993, 1993, 1993, 1993, 1993, 2004, 2047, 2106, 2106, 2126, 2167, 2167, 2167, 2167, 2167, 2167, 2209, 2265, 2265, 2271, 2294, 2299, 2299, 2340, 2380, 2382, 2382, 2382, 2382, 2401, 2406, 2435, 2460, 2460, 2487, 2487, 2507, 2516, 2516, 2535, 2567, 2620, 2620, 2620, 2656, 2656, 2661, 2672, 2672, 2705, 2705, 2707, 2743, 2743, 2743, 2743, 2743, 2747, 2747, 2747, 2781, 2781, 2800, 2821, 2866, 2916, 2968, 2969, 2994, 2997, 2997, 3031, 3059, 3059, 3059, 3059, 3059, 3105, 3105, 3105]</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>[0.198, 0.188, 0.189, 0.187, 0.179, 0.189, 0.195, 0.195, 0.195, 0.195, 0.204, 0.204, 0.209, 0.21, 0.21, 0.21, 0.21, 0.21, 0.21, 0.207, 0.207, 0.207, 0.21, 0.209, 0.209, 0.218, 0.218, 0.218, 0.218, 0.218, 0.218, 0.222, 0.224, 0.231, 0.231, 0.244, 0.244, 0.244, 0.244, 0.244, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.25, 0.249, 0.249, 0.249, 0.25, 0.249, 0.248, 0.248, 0.247, 0.247, 0.247, 0.247, 0.247, 0.247, 0.247, 0.247, 0.247, 0.247, 0.248, 0.246, 0.252, 0.255, 0.258, 0.258, 0.26, 0.26, 0.263, 0.27, 0.27, 0.269, 0.269, 0.269, 0.269, 0.27, 0.27, 0.27, 0.27, 0.27, 0.27, 0.27, 0.277, 0.282, 0.282, 0.282, 0.283, 0.283, 0.283, 0.283, 0.283, 0.283, 0.297, 0.298, 0.298, 0.298, 0.298, 0.299, 0.3, 0.3, 0.299, 0.299, 0.3, 0.3, 0.3, 0.3, 0.303, 0.303, 0.303, 0.303, 0.303, 0.303, 0.306, 0.307, 0.307, 0.311, 0.311, 0.311, 0.311, 0.311, 0.311, 0.312, 0.312, 0.313, 0.313, 0.314, 0.314, 0.314, 0.314, 0.314, 0.314, 0.314, 0.316, 0.317, 0.317, 0.317, 0.317, 0.317, 0.317, 0.317, 0.317, 0.316, 0.316, 0.317, 0.317, 0.317, 0.316, 0.316, 0.316, 0.316, 0.316, 0.316, 0.317, 0.317, 0.317, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.318, 0.317, 0.317, 0.317, 0.317, 0.317, 0.317, 0.317, 0.317, 0.317, 0.317, 0.317, 0.318, 0.319, 0.319, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.319, 0.319, 0.319, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.319, 0.319, 0.319, 0.319, 0.319, 0.319, 0.319, 0.319, 0.319, 0.319, 0.322, 0.322, 0.322, 0.323, 0.323, 0.323, 0.324, 0.323, 0.323, 0.322, 0.322, 0.322, 0.322, 0.322, 0.322, 0.321, 0.321, 0.321, 0.321, 0.321, 0.323, 0.323, 0.323]</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600, 3630, 3660, 3690, 3720, 3750, 3780, 3810, 3840, 3870, 3900, 3930, 3960, 3990, 4020, 4050, 4080, 4110, 4140, 4170, 4200, 4230, 4260, 4290, 4320, 4350, 4380, 4410, 4440, 4470, 4500, 4530, 4560, 4590, 4620, 4650, 4680, 4710, 4740, 4770, 4800, 4830, 4860, 4890, 4920, 4950, 4980, 5010, 5040, 5070, 5100, 5130, 5160, 5190, 5220, 5250, 5280, 5310, 5340, 5370, 5400, 5430, 5460, 5490, 5520, 5550, 5580, 5610, 5640, 5670, 5700, 5730, 5760, 5790, 5820, 5850, 5880, 5910, 5940, 5970, 6000, 6030, 6060, 6090, 6120, 6150, 6180, 6210, 6240, 6270, 6300, 6330, 6360, 6390, 6420, 6450, 6480, 6510, 6540, 6570, 6600, 6630, 6660, 6690, 6720, 6750, 6780, 6810, 6840, 6870, 6900, 6930, 6960, 6990, 7020, 7050, 7080, 7110, 7140, 7170, 7200]</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>[0, 17.52793416976929, 38.7789392709732, 62.58059532642363, 84.89613258838654, 108.87918150424957, 115.41948168277742, 137.76446869373325, 150.5118126869202, 150.5118126869202, 159.09661245346072, 177.91365759372712, 189.81120007038118, 210.32214829921725, 228.76914179325104, 252.86413037776947, 280.9207267522812, 300.9088410139084, 312.83593409061433, 329.90732657909393, 336.436066865921, 342.9824781358242, 354.54200977683064, 377.3715014636516, 389.99735373854634, 413.1474252164363, 447.1121210515499, 466.29107274413104, 484.02367038130757, 507.2526690423488, 514.1694772541523, 529.0264484226703, 544.5860427081585, 561.047990077734, 587.4782888829708, 602.8189172923564, 622.7874913275241, 637.79313172698, 660.7685646235941, 682.5441915690897, 689.524436920881, 705.6697045505044, 726.9214303672311, 741.9056848704812, 767.8465336978433, 780.7718532025812, 797.1853027582166, 808.3614051222798, 828.4742178559301, 843.816136229038, 850.2433691859243, 861.7483902573583, 884.014494526386, 900.3498630166051, 924.8223619103429, 942.5262917637823, 969.6005645394323, 978.2200222969053, 998.7784373044966, 1018.0795618057249, 1026.906996643543, 1049.425167429447, 1061.6180006325242, 1071.627299290895, 1086.808674794435, 1107.3655738651748, 1116.4213741123672, 1141.6136770069595, 1158.2329282343383, 1170.8162989675993, 1182.323849111795, 1199.5817208707329, 1219.3448289096352, 1243.4611829459664, 1265.3118131816384, 1286.358162230253, 1294.9108624637124, 1322.7833738505838, 1335.814122074842, 1335.814122074842, 1342.7892718851563, 1361.8519820511337, 1380.3217920839784, 1399.885567575693, 1421.5436864912508, 1435.6558796703814, 1442.5885307252406, 1466.6762978971003, 1481.7029489219187, 1499.1765653312204, 1503.7677525699137, 1516.1315676152703, 1527.3778009831904, 1546.4282857835292, 1567.798760265112, 1583.0771274983883, 1589.3437117278577, 1603.0760107457638, 1618.741172426939, 1635.1696043193342, 1640.3938686788083, 1653.4571123063565, 1671.762788718939, 1688.583626765013, 1714.0350256145002, 1729.180449742079, 1754.1991224944593, 1767.409490913153, 1787.5223035991194, 1804.1014747560025, 1823.943976455927, 1845.112312680483, 1862.190736180544, 1884.0320534527302, 1907.662737327814, 1931.0987021028996, 1947.7728015482426, 1964.5288020670414, 1980.604319578409, 1981.0240195810793, 2001.5940310060976, 2022.4418579399583, 2039.178712970018, 2062.204023057222, 2084.9293885290617, 2107.9313539564605, 2124.209454590082, 2142.2221551477905, 2157.004179626703, 2157.423879629373, 2178.0026869833464, 2195.044585639238, 2210.642878681421, 2231.0924203217023, 2254.608524733781, 2269.8102757751935, 2277.2595401704307, 2291.60345301032, 2310.2156250894063, 2338.1385432660572, 2342.022157019376, 2365.977642267942, 2380.553641670942, 2386.694473737478, 2400.893409675359, 2419.9819588124747, 2428.199259036779, 2451.4536924779413, 2466.0861933171745, 2481.5400681674478, 2502.4021008312698, 2518.451592761278, 2526.311221015453, 2546.7066475510596, 2561.6432428240773, 2582.9092108607288, 2600.3967384219163, 2618.409438979625, 2632.932764852046, 2633.3524648547163, 2653.5662156939497, 2672.739631474017, 2686.350319892167, 2711.7060074388974, 2737.0292019903654, 2759.5971680700773, 2776.989160305261, 2795.00186086297, 2812.9085014164443, 2813.3282014191145, 2833.1336513817305, 2854.8900912582867, 2865.4155461966984, 2886.676930779218, 2909.745595687627, 2932.7475611150257, 2951.455148738622, 2969.048949283361, 2984.1151764094825, 2984.5348764121527, 3006.373078888654, 3022.255419129133, 3037.5273890197273, 3060.248821943998, 3082.0994521796697, 3101.67745129466, 3109.391651505231, 3136.319331997632, 3147.7024480760087, 3147.7024480760087, 3156.7840476334086, 3172.8813685357563, 3190.075423407554, 3202.380906772613, 3227.8323056221, 3241.0270672321312, 3258.389540755748, 3274.834041392802, 3295.5138729691494, 3316.5471497416484, 3325.012826120852, 3333.1412876605973, 3353.3877490520463, 3365.53439016342, 3390.9857890129074, 3405.038238763808, 3418.656529438494, 3430.9068300843223, 3453.747083485125, 3473.543108594416, 3481.1282945990547, 3482.3571445107445, 3483.784849607943, 3510.517313778399, 3520.9268810152994, 3543.1320698618874, 3570.33236709833, 3591.252454912661, 3608.5069717288, 3632.4997699618325, 3639.270315444468, 3662.718966424464, 3675.612739765643, 3685.1158241152752, 3707.338210189341, 3729.3634591937052, 3737.738009226321, 3762.930312120913, 3775.9961314320553, 3798.8326190590847, 3810.3704192519176, 3816.5335780262935, 3832.714235794543, 3854.8565484404553, 3866.5867018342005, 3884.0673681378353, 3911.605714857577, 3932.9655787587153, 3957.1455152630792, 3970.2730605483043, 3975.7136774539936]</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>[0, 3.27, 3.91, 4.51, 15.5, 30.78, 37.94, 38.47, 39.01, 39.47, 47.46, 47.88, 55.97, 60.01, 60.49, 61.0, 61.6, 62.23, 63.5, 78.6, 79.23, 79.89, 82.64, 91.74, 92.09, 99.88, 100.35, 101.51, 103.4, 103.95, 104.51, 109.62, 118.06, 118.97, 119.51, 128.72, 129.59, 131.91, 133.92, 134.64, 141.94, 144.44, 159.98, 161.05, 161.82, 164.52, 165.21, 165.83, 167.07, 167.7, 175.25, 178.97, 196.36, 197.62, 198.44, 212.85, 213.37, 213.97, 216.26, 218.17, 219.53, 229.44, 230.01, 238.64, 239.11, 250.47, 260.65, 277.81, 278.36, 280.25, 282.41, 289.2, 293.72, 299.17, 306.13, 323.2, 328.27, 328.94, 329.71, 330.46, 336.05, 337.49, 338.18, 339.15, 344.61, 347.18, 348.81, 363.21, 370.97, 371.99, 372.82, 376.36, 378.1, 379.37, 380.85, 381.67, 382.4, 394.45, 402.48, 404.14, 405.69, 411.79, 419.1, 421.47, 422.17, 433.96, 437.78, 441.99, 445.05, 446.99, 449.16, 455.79, 457.18, 458.43, 459.32, 460.12, 460.9, 478.03, 498.61, 501.16, 508.28, 519.91, 520.69, 522.56, 523.71, 524.7, 528.96, 537.19, 556.0, 557.69, 563.89, 564.75, 565.89, 567.59, 568.8, 569.62, 572.29, 586.75, 595.49, 596.99, 598.33, 612.4, 613.71, 627.52, 628.65, 636.11, 649.0, 662.99, 665.69, 669.62, 673.78, 680.1, 680.8, 681.63, 682.41, 684.16, 686.02, 697.1, 708.38, 709.19, 715.42, 722.59, 724.0, 724.95, 725.85, 727.2, 734.22, 746.85, 762.28, 763.12, 771.28, 782.81, 783.65, 784.44, 787.05, 788.66, 790.34, 802.05, 814.99, 816.58, 819.96, 828.5, 833.54, 835.58, 851.22, 863.59, 865.63, 867.04, 870.18, 871.1, 879.6, 884.18, 894.72, 903.64, 904.63, 914.03, 915.66, 924.31, 929.14, 930.69, 938.03, 943.95, 959.44, 961.06, 961.99, 973.24, 974.77, 978.9, 984.39, 986.59, 999.66, 1001.78, 1004.82, 1023.56, 1024.51, 1025.41, 1026.37, 1027.28, 1029.57, 1031.1, 1032.09, 1045.37, 1046.16, 1055.06, 1062.47, 1077.43, 1094.15, 1116.06, 1117.9, 1128.04, 1132.02, 1133.98, 1146.84, 1162.76, 1163.71, 1164.54, 1165.99, 1167.04, 1185.85, 1187.39, 1188.37]</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, -10, 0, 0, -10, 0, -10, 0, -10, -10, 0, 0, 0, 0, -10, 0, -20, -20, -20, 0, -20, 0, 0, 0, -20, -20, 0, -20, 0, 0, 0, -20, 0, -20, -10, -10, -10, -20, -20, 0, -20, -20, -20, -20, 0, 0, 0, 0, 0, 0, 0, 0, -20, -20, 0, 0, 0, 0, 0, 0, 0, -20, -20, 0, -20, -10, -20, -20, -10, -20, -10, -10, 0, -10, -10, -10, 0, 0, -10, -10, 0, -10, -10, 0, -10, 0, 0, -10, 0, 0, 0, 0, -10, -10, 0, -10, -20, -20]</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>clusterStdHigh</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5']</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>[100, 104, 106, 108, 147, 184, 204, 204, 204, 204, 219, 219, 224, 234, 235, 235, 235, 235, 235, 235, 235, 235, 235, 236, 236, 237, 237, 261, 288, 288, 288, 288, 293, 304, 304, 304, 304, 304, 349, 368, 368, 368, 403, 415, 415, 415, 415, 415, 434, 434, 434, 474, 474, 489, 489, 534, 578, 631, 654, 667, 673, 679, 686, 687, 690, 733, 761, 761, 761, 761, 767, 767, 767, 767, 787, 799, 803, 815, 842, 842, 852, 867, 867, 887, 887, 936, 993, 1039, 1054, 1066, 1069, 1089, 1089, 1089, 1089, 1104, 1104, 1146, 1209, 1209, 1231, 1256, 1256, 1256, 1256, 1256, 1256, 1300, 1360, 1360, 1383, 1388, 1434, 1434, 1434, 1468, 1468, 1475, 1483, 1483, 1496, 1498, 1529, 1546, 1546, 1567, 1567, 1583, 1593, 1593, 1603, 1640, 1689, 1689, 1689, 1723, 1723, 1727, 1734, 1734, 1734, 1736, 1788, 1795, 1795, 1826, 1828, 1831, 1846, 1846, 1877, 1879, 1885, 1896, 1896, 1931, 1935, 1938, 1947, 1947, 1953, 1988, 1988, 2002, 2004, 2046, 2085, 2120, 2136, 2144, 2152, 2152, 2152, 2152, 2182, 2182, 2182, 2209, 2234, 2234, 2235, 2265, 2265, 2265, 2265, 2265, 2272, 2314, 2371, 2371, 2392, 2403, 2405, 2405, 2408, 2448, 2465, 2465, 2465, 2465, 2471, 2504, 2504, 2516, 2516, 2559, 2602, 2653, 2703, 2708, 2714, 2714, 2714, 2714, 2714, 2716, 2716, 2744, 2755, 2755, 2755, 2764, 2764, 2779, 2782, 2830, 2889, 2939, 2941, 2945, 2948, 2972, 2972, 2972, 2972, 2972, 2972, 3014, 3060, 3060, 3077]</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>[0.198, 0.201, 0.202, 0.202, 0.184, 0.182, 0.187, 0.187, 0.187, 0.187, 0.196, 0.196, 0.202, 0.201, 0.201, 0.201, 0.201, 0.201, 0.201, 0.201, 0.201, 0.201, 0.201, 0.201, 0.201, 0.2, 0.2, 0.208, 0.211, 0.211, 0.211, 0.211, 0.208, 0.208, 0.208, 0.208, 0.208, 0.208, 0.212, 0.213, 0.213, 0.213, 0.213, 0.213, 0.213, 0.213, 0.213, 0.213, 0.211, 0.211, 0.211, 0.21, 0.21, 0.213, 0.213, 0.217, 0.215, 0.22, 0.227, 0.228, 0.228, 0.235, 0.235, 0.235, 0.235, 0.234, 0.234, 0.234, 0.234, 0.234, 0.234, 0.234, 0.234, 0.234, 0.24, 0.245, 0.244, 0.246, 0.246, 0.246, 0.246, 0.246, 0.246, 0.246, 0.246, 0.247, 0.246, 0.247, 0.247, 0.247, 0.247, 0.25, 0.25, 0.25, 0.25, 0.253, 0.253, 0.258, 0.261, 0.261, 0.26, 0.26, 0.26, 0.26, 0.26, 0.26, 0.26, 0.261, 0.26, 0.26, 0.262, 0.266, 0.266, 0.266, 0.266, 0.276, 0.276, 0.279, 0.279, 0.279, 0.281, 0.282, 0.282, 0.284, 0.284, 0.285, 0.285, 0.287, 0.287, 0.287, 0.288, 0.288, 0.29, 0.29, 0.29, 0.29, 0.29, 0.29, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.293, 0.293, 0.292, 0.292, 0.292, 0.292, 0.294, 0.294, 0.294, 0.295, 0.295, 0.295, 0.295, 0.295, 0.297, 0.297, 0.297, 0.297, 0.298, 0.298, 0.297, 0.298, 0.298, 0.301, 0.301, 0.301, 0.301, 0.301, 0.301, 0.301, 0.301, 0.309, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.308, 0.31, 0.31, 0.311, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.314, 0.313, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.312, 0.314, 0.314, 0.313, 0.313, 0.313, 0.314, 0.313, 0.313, 0.313, 0.313, 0.313, 0.313, 0.313, 0.314, 0.314, 0.314]</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600, 3630, 3660, 3690, 3720, 3750, 3780, 3810, 3840, 3870, 3900, 3930, 3960, 3990, 4020, 4050, 4080, 4110, 4140, 4170, 4200, 4230, 4260, 4290, 4320, 4350, 4380, 4410, 4440, 4470, 4500, 4530, 4560, 4590, 4620, 4650, 4680, 4710, 4740, 4770, 4800, 4830, 4860, 4890, 4920, 4950, 4980, 5010, 5040, 5070, 5100, 5130, 5160, 5190, 5220, 5250, 5280, 5310, 5340, 5370, 5400, 5430, 5460, 5490, 5520, 5550, 5580, 5610, 5640, 5670, 5700, 5730, 5760, 5790, 5820, 5850, 5880, 5910, 5940, 5970, 6000, 6030, 6060, 6090, 6120, 6150, 6180, 6210, 6240, 6270, 6300, 6330, 6360, 6390, 6420, 6450, 6480, 6510, 6540, 6570, 6600, 6630, 6660, 6690, 6720, 6750, 6780, 6810, 6840, 6870, 6900, 6930, 6960, 6990, 7020, 7050, 7080, 7110, 7140, 7170, 7200]</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>[0, 14.390010166168217, 34.40344750881195, 53.57026708126068, 74.49108326435089, 92.60073244571686, 100.81803267002107, 124.91122047901155, 136.983123087883, 136.983123087883, 143.77942290306092, 155.75612530708312, 166.8244977712631, 184.02682273387907, 197.78010656833646, 219.040393948555, 244.42014119625094, 266.0589890241623, 280.89394962787634, 311.16592228412634, 317.02600709199913, 336.41321333646783, 354.4439952254296, 380.02125962972644, 402.80602945089345, 419.21997588872915, 426.34450091123585, 435.5846852064133, 452.5593361854554, 474.283291721344, 479.46007460355764, 485.06393643617633, 496.16369467973715, 513.6445256114007, 524.370590388775, 548.4655875563623, 572.287234914303, 592.7457044005396, 617.8980043768885, 635.5936148285867, 642.3641603112222, 647.618021297455, 664.2745807647707, 685.7455782890322, 696.4716430664065, 718.6768273830417, 740.6303272724155, 761.5416781902317, 783.7087923765185, 814.9267641782764, 821.3346113443378, 845.2866215944293, 860.3355214953426, 872.0031704783444, 889.307499969006, 911.33274897337, 921.6562402129177, 947.3330104708676, 964.93271945715, 975.2976282000546, 997.4111786842351, 1017.3282061576848, 1034.435887598992, 1056.7154808759694, 1079.960832190514, 1101.0071812391286, 1109.3706722021109, 1137.2431835889822, 1150.3079681158072, 1150.3079681158072, 1166.3514371037488, 1178.3514384627347, 1182.3682383894925, 1200.163616406918, 1225.9210770010952, 1245.084227097035, 1252.6927457213408, 1265.9719449400907, 1284.1153958916668, 1307.2561311364177, 1312.6947692632677, 1336.1470053911212, 1349.2935978174212, 1359.1964772343638, 1371.5445358514787, 1395.5275847673418, 1405.0864850282671, 1427.371983742714, 1444.0583171129229, 1464.5581510543825, 1488.6376533627513, 1509.057513868809, 1519.8407110929493, 1539.8960843801501, 1562.9995580673221, 1587.4112347602847, 1606.118822383881, 1623.7126229286198, 1640.3055376529699, 1640.72523765564, 1662.1463873863224, 1683.5003093957905, 1699.895595955849, 1721.5309898853307, 1742.2137962102895, 1765.649760985375, 1783.5439752340321, 1801.9755758047108, 1817.929146099091, 1818.3488461017612, 1838.950893545151, 1845.0706541299824, 1866.040606093407, 1877.217726683617, 1902.6691255331043, 1917.5000331878666, 1943.329591917992, 1956.109911859036, 1976.918041455746, 1998.1987683892253, 2006.9208915591244, 2022.2445305943493, 2048.6457786202436, 2069.31110316515, 2094.7625020146374, 2107.2885502219206, 2132.4819244027144, 2146.5511443614964, 2165.698281168938, 2186.979007506371, 2202.2740369796757, 2210.0305945754053, 2234.7077246546746, 2252.98889220953, 2278.929741036892, 2295.4490410685544, 2310.2250624537473, 2319.310175478459, 2337.1144601225856, 2357.652836143971, 2378.231299221516, 2394.409308660031, 2414.277268874646, 2427.7358972668653, 2452.208396160603, 2464.6839977860454, 2483.2701178073885, 2497.4586395382885, 2518.003291547299, 2538.2942164063456, 2546.03215713501, 2561.299153995514, 2572.5098190486433, 2592.07037987113, 2616.542878764868, 2629.7562518775467, 2644.233351993561, 2656.652133333683, 2671.409458768368, 2688.2360796332364, 2698.006963729859, 2720.5113530159, 2736.6526513576514, 2748.8378700494773, 2763.4873441815384, 2784.044243252278, 2790.5427426457413, 2807.4991003632554, 2822.0838770508776, 2831.425944697858, 2843.573791551591, 2862.4982007741937, 2881.3771604299554, 2902.0387580156334, 2924.3130477190025, 2938.211759495736, 2946.023947227002, 2959.576093733311, 2977.3678213715557, 3003.3421160340313, 3008.500268423558, 3028.6675938725475, 3036.61030753851, 3060.930327689648, 3085.367210114003, 3107.067177498341, 3119.3695285916333, 3136.963329136372, 3152.0040522217755, 3152.4237522244457, 3171.4163512349132, 3187.6457152009016, 3205.6463970065124, 3228.4807284235962, 3248.471730554105, 3268.049729669095, 3276.6024299025544, 3303.0576949477204, 3315.078481328488, 3315.078481328488, 3334.5516045093545, 3356.104672574998, 3368.2605848789226, 3379.574744898082, 3395.073550134898, 3416.1198991835126, 3423.330999380351, 3448.0386136114607, 3472.257710009814, 3486.239233046771, 3499.226883393527, 3518.4707468330867, 3536.144666510821, 3559.6897576153283, 3581.5039224445823, 3597.8982236444954, 3605.422258716822, 3617.1489663898947, 3628.528528171778, 3650.724743610621, 3655.9045276939873, 3676.4854894459254, 3689.3792627871044, 3699.9123084425933, 3714.9099593758588, 3738.403558313847, 3748.1943580031398, 3772.41750921011, 3787.3452290654186, 3789.6754829049114, 3799.6567841649057, 3820.642005646229, 3832.5115847706797, 3846.8673918128015, 3866.07004557848, 3886.468014919758, 3904.362229168415, 3921.956029713154, 3934.2878195166586, 3934.707519519329, 3954.1159210085866]</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>[0, 1.17, 1.49, 1.89, 10.19, 27.95, 38.77, 39.41, 40.04, 40.76, 52.34, 52.79, 55.76, 59.6, 61.32, 61.85, 63.44, 63.98, 64.45, 64.92, 65.65, 66.09, 66.67, 68.35, 68.81, 69.37, 69.93, 81.94, 98.32, 98.85, 99.47, 100.37, 102.0, 104.74, 105.23, 105.7, 106.62, 107.11, 119.91, 127.53, 128.95, 129.75, 141.21, 146.06, 146.44, 147.48, 148.0, 149.03, 157.12, 157.62, 158.15, 172.01, 172.81, 178.96, 179.47, 195.6, 208.15, 225.1, 232.65, 235.32, 238.25, 240.53, 242.7, 244.17, 246.27, 261.33, 269.16, 270.12, 271.34, 272.28, 277.0, 277.67, 278.56, 279.67, 286.46, 289.3, 292.72, 299.13, 306.5, 307.61, 314.03, 320.78, 321.34, 328.31, 329.01, 345.97, 360.22, 372.14, 376.51, 381.75, 383.76, 388.62, 389.25, 390.76, 392.12, 395.7, 397.92, 412.05, 430.51, 432.7, 440.76, 448.92, 450.5, 453.59, 454.94, 455.66, 456.39, 470.81, 486.58, 487.17, 499.15, 501.21, 516.35, 517.57, 518.9, 531.26, 532.82, 538.14, 541.73, 542.69, 550.23, 552.79, 564.82, 569.8, 571.33, 579.77, 581.78, 589.1, 592.97, 594.6, 599.83, 610.98, 632.25, 633.03, 633.81, 645.75, 646.5, 649.04, 651.39, 652.66, 653.94, 656.29, 670.86, 673.78, 675.05, 691.41, 693.94, 696.94, 707.14, 707.98, 724.49, 728.38, 731.14, 738.55, 740.16, 750.69, 753.49, 756.94, 761.53, 762.2, 766.21, 788.81, 789.55, 798.4, 799.25, 811.45, 827.41, 838.49, 844.21, 847.65, 850.26, 850.86, 851.52, 852.98, 861.65, 863.21, 864.42, 871.38, 878.68, 880.37, 882.95, 890.16, 891.65, 892.54, 893.32, 894.99, 899.26, 907.99, 922.24, 923.07, 940.8, 949.41, 951.26, 952.35, 954.45, 977.06, 982.46, 983.76, 985.52, 986.56, 989.87, 999.05, 999.79, 1004.1, 1005.28, 1017.89, 1027.51, 1043.25, 1074.89, 1078.11, 1082.97, 1083.86, 1086.56, 1088.49, 1090.08, 1092.41, 1093.28, 1102.63, 1107.47, 1108.21, 1109.0, 1112.0, 1112.92, 1119.72, 1122.69, 1133.74, 1148.12, 1165.18, 1167.08, 1171.14, 1173.61, 1188.8, 1189.71, 1190.45, 1191.33, 1192.21, 1193.04, 1207.06, 1219.77, 1221.68, 1228.52]</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>[-20, -10, -10, 0, -20, -10, 0, -20, 0, -20, 0, -20, -10, -20, 0, 0, -10, -20, 0, -10, 0, -10, 0, -10, -20, -10, -10, 0, 0, 0, -10, -10, -20, 0, -10, 0, 0, 0, 0, -20, -20, -20, 0, 0, 0, 0, -20, -20, -10, -10, 0, -10, -10, 0, 0, 0, -20, 0, -20, -20, -20, -10, -20, 0, 0, -20, 0, 0, -10, 0, 0, 0, 0, 0, -20, 0, 0, 0, -10, 0, 0, 0, -10, 0, 0, -20, 0, -20, -20, -10, -10, -10, -20, 0, 0, 0, -10, 0, 0, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
-      <c r="O24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2']</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>[100, 114, 117, 117, 119, 159, 187, 187, 187, 187, 212, 219, 224, 231, 234, 270, 282, 282, 282, 282, 301, 301, 301, 304, 304, 304, 304, 311, 333, 333, 333, 340, 388, 418, 419, 451, 451, 455, 465, 465, 472, 472, 472, 472, 509, 509, 509, 535, 565, 565, 566, 566, 566, 566, 566, 566, 566, 589, 617, 617, 617, 621, 627, 636, 638, 682, 702, 702, 702, 702, 741, 759, 759, 759, 759, 759, 759, 799, 852, 852, 877, 877, 877, 877, 877, 888, 888, 897, 923, 923, 923, 923, 923, 923, 930, 931, 931, 948, 981, 981, 982, 998, 1000, 1005, 1025, 1066, 1067, 1067, 1067, 1067, 1087, 1107, 1107, 1121, 1126, 1161, 1217, 1261, 1278, 1287, 1290, 1302, 1302, 1302, 1302, 1302, 1302, 1337, 1396, 1396, 1415, 1415, 1415, 1415, 1415, 1415, 1415, 1442, 1457, 1457, 1458, 1496, 1496, 1524, 1524, 1547, 1603, 1657, 1658, 1681, 1684, 1696, 1729, 1729, 1729, 1770, 1770, 1772, 1774, 1774, 1776, 1776, 1781, 1789, 1789, 1789, 1789, 1789, 1798, 1798, 1798, 1804, 1814, 1827, 1829, 1872, 1883, 1883, 1883, 1883, 1907, 1937, 1937, 1943, 1943, 1987, 2046, 2103, 2104, 2112, 2118, 2118, 2147, 2163, 2163, 2163, 2163, 2163, 2167, 2167, 2167, 2201, 2201, 2201, 2201, 2201, 2201, 2234, 2290, 2290, 2300, 2302, 2302, 2302, 2337, 2364, 2364, 2372, 2396, 2396, 2396, 2396, 2427, 2448, 2448, 2449, 2449, 2449, 2464, 2464, 2464, 2466, 2506, 2524, 2524, 2554, 2554, 2554, 2558, 2558, 2565]</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>[0.198, 0.182, 0.182, 0.182, 0.184, 0.171, 0.178, 0.178, 0.178, 0.178, 0.186, 0.184, 0.184, 0.187, 0.19, 0.18, 0.179, 0.179, 0.179, 0.179, 0.179, 0.179, 0.179, 0.18, 0.18, 0.18, 0.18, 0.187, 0.188, 0.188, 0.188, 0.192, 0.186, 0.184, 0.187, 0.192, 0.192, 0.196, 0.194, 0.194, 0.195, 0.195, 0.195, 0.195, 0.194, 0.194, 0.194, 0.208, 0.208, 0.208, 0.208, 0.208, 0.208, 0.208, 0.208, 0.208, 0.208, 0.207, 0.208, 0.208, 0.208, 0.208, 0.208, 0.208, 0.207, 0.207, 0.207, 0.207, 0.207, 0.207, 0.211, 0.215, 0.215, 0.215, 0.215, 0.215, 0.215, 0.227, 0.234, 0.234, 0.236, 0.236, 0.236, 0.236, 0.236, 0.239, 0.239, 0.237, 0.237, 0.237, 0.237, 0.237, 0.237, 0.237, 0.237, 0.237, 0.237, 0.236, 0.238, 0.238, 0.238, 0.238, 0.238, 0.242, 0.246, 0.243, 0.243, 0.243, 0.243, 0.243, 0.244, 0.245, 0.245, 0.244, 0.245, 0.244, 0.243, 0.25, 0.256, 0.257, 0.257, 0.256, 0.256, 0.256, 0.256, 0.256, 0.256, 0.259, 0.259, 0.259, 0.26, 0.26, 0.26, 0.26, 0.26, 0.26, 0.26, 0.27, 0.27, 0.27, 0.27, 0.269, 0.269, 0.268, 0.268, 0.269, 0.265, 0.263, 0.263, 0.264, 0.264, 0.265, 0.266, 0.266, 0.266, 0.27, 0.27, 0.271, 0.271, 0.271, 0.272, 0.272, 0.273, 0.272, 0.272, 0.272, 0.272, 0.272, 0.278, 0.278, 0.278, 0.278, 0.279, 0.283, 0.283, 0.283, 0.282, 0.282, 0.282, 0.282, 0.283, 0.282, 0.282, 0.282, 0.282, 0.281, 0.281, 0.28, 0.28, 0.28, 0.28, 0.28, 0.283, 0.283, 0.283, 0.283, 0.283, 0.283, 0.283, 0.283, 0.283, 0.284, 0.284, 0.284, 0.284, 0.284, 0.284, 0.285, 0.286, 0.286, 0.287, 0.287, 0.287, 0.287, 0.288, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.292, 0.293, 0.293, 0.293, 0.294, 0.294, 0.294, 0.295, 0.295, 0.295, 0.295, 0.295, 0.302, 0.302, 0.304, 0.304, 0.304, 0.304, 0.304, 0.304]</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600, 3630, 3660, 3690, 3720, 3750, 3780, 3810, 3840, 3870, 3900, 3930, 3960, 3990, 4020, 4050, 4080, 4110, 4140, 4170, 4200, 4230, 4260, 4290, 4320, 4350, 4380, 4410, 4440, 4470, 4500, 4530, 4560, 4590, 4620, 4650, 4680, 4710, 4740, 4770, 4800, 4830, 4860, 4890, 4920, 4950, 4980, 5010, 5040, 5070, 5100, 5130, 5160, 5190, 5220, 5250, 5280, 5310, 5340, 5370, 5400, 5430, 5460, 5490, 5520, 5550, 5580, 5610, 5640, 5670, 5700, 5730, 5760, 5790, 5820, 5850, 5880, 5910, 5940, 5970, 6000, 6030, 6060, 6090, 6120, 6150, 6180, 6210, 6240, 6270, 6300, 6330, 6360, 6390, 6420, 6450, 6480, 6510, 6540, 6570, 6600, 6630, 6660, 6690, 6720, 6750, 6780, 6810, 6840, 6870, 6900, 6930, 6960, 6990, 7020, 7050, 7080, 7110, 7140, 7170, 7200]</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>[0, 19.8122772693634, 35.085855460166925, 51.360508608818066, 74.60585992336276, 94.18385903835299, 103.74275929927828, 125.49661836624149, 137.93367021083836, 137.93367021083836, 147.05501996278767, 166.70348545312885, 188.27499684095386, 212.75821546316152, 228.5650543570519, 246.18525356054312, 254.90565379858023, 279.47125705480585, 292.6317093491555, 292.6317093491555, 302.4684590816499, 319.088096523285, 335.55697622299203, 359.7816426038743, 377.3529217004777, 391.43120267391214, 398.31735194921504, 408.3705502152444, 424.0357118964196, 435.3699495673181, 440.67221025228514, 455.14791070222867, 473.45393697023405, 485.7180929303171, 508.7222418904306, 522.295738899708, 533.9423539578917, 541.5002479135992, 557.5957582294943, 575.4121806442739, 583.54814530015, 600.0988472044469, 616.5677269041539, 637.3706167042257, 660.1252811729909, 674.7664572536946, 682.2497164070608, 696.0755527436735, 715.3174590051176, 726.179436773062, 731.3268012464049, 748.589169687033, 756.6227695405486, 779.2670635402205, 801.545724743605, 818.7338840186599, 826.2938829839233, 836.5418354809287, 855.5023630917076, 880.5321379482749, 885.9510060846809, 903.2263996183875, 917.5052463352683, 934.9847722828391, 955.4406814396384, 976.9764804661277, 984.1875806629661, 1002.6117831051353, 1014.8235333263877, 1014.8235333263877, 1022.1928381443028, 1041.2207993745808, 1050.0075737178329, 1070.8781582772735, 1093.9078762233262, 1116.0418429553513, 1131.7458005130295, 1148.5018010318283, 1162.5077296912675, 1162.9274296939377, 1184.2964992702011, 1194.2021977841857, 1211.005530804396, 1231.2290504872801, 1252.5995250642302, 1267.5384660422803, 1274.909122401476, 1287.7028216183187, 1306.2034880220892, 1309.981567245722, 1314.9282178938392, 1327.5706600725655, 1345.2445797502999, 1368.2577194511894, 1388.1202712357046, 1402.145255404711, 1408.952756327391, 1422.0561710298064, 1440.9734132707122, 1468.36448764205, 1473.8506200492386, 1489.7471088111404, 1505.02068695426, 1523.1908709943298, 1544.11168717742, 1564.179136270285, 1569.210136407614, 1598.0274786889556, 1609.4202786862854, 1609.4202786862854, 1617.1108284771447, 1632.4181035339836, 1645.5646959602836, 1653.4965638279918, 1667.0785678505902, 1684.2093170762066, 1692.9277635574344, 1714.2443275451665, 1732.2284699916845, 1768.473864781857, 1776.6411148190502, 1793.9966424107556, 1803.3318128943447, 1822.8619412541393, 1846.6330057501796, 1866.5969757437708, 1882.0510698676112, 1896.7125703215602, 1912.2706906199458, 1912.690390622616, 1932.0950413107873, 1944.138438999653, 1964.2224386334422, 1982.7183962464335, 2005.9676624417307, 2018.7921838641169, 2025.9067535042764, 2045.2756832957268, 2060.7676876664164, 2065.9625465989116, 2069.767467427254, 2092.761331820488, 2109.1139302253723, 2115.291678071022, 2132.189728951454, 2143.4470784425735, 2152.631277537346, 2178.7925151586533, 2194.5914155483247, 2215.1076015710833, 2226.525859475136, 2233.5564617395403, 2248.0178467512133, 2263.816315793991, 2283.883764886856, 2299.8756309747696, 2322.0674864172934, 2329.7321581840515, 2349.973268890381, 2372.7386967897414, 2392.6207563877106, 2399.3820056438444, 2408.8962639331817, 2424.297787332535, 2433.0109606504443, 2450.9640869855884, 2484.554082798958, 2502.3334532022477, 2517.454674267769, 2538.3958708047867, 2544.548244845867, 2563.2225646853444, 2583.7774754643438, 2597.5243679404257, 2618.9100911498067, 2639.956440198421, 2646.9080375313756, 2672.4184716820714, 2684.845224058628, 2684.845224058628, 2694.32427380085, 2716.328762745857, 2728.7168979167936, 2740.4946835041046, 2752.7172806978224, 2774.2530797243116, 2784.1473799943924, 2811.762019705772, 2822.7867770195007, 2836.8571058273315, 2856.5732216000556, 2863.2879841685294, 2880.9776366591454, 2903.0569016575814, 2910.834935128689, 2928.7880619883535, 2959.6060581564902, 2978.660577905178, 2994.817741215229, 3017.065739452839, 3021.901843369007, 3042.360077917576, 3057.0475221276283, 3074.2813249468804, 3091.5929669499396, 3114.1609330296515, 3132.0551472783086, 3145.8788477063176, 3160.66087218523, 3161.0805721879, 3178.8745241761203, 3195.1699252724643, 3207.978867256641, 3226.129457175731, 3249.457758891582, 3269.2660118699073, 3276.2685812592504, 3289.4775295376776, 3305.2833805441855, 3312.8395389914513, 3317.4799920201303, 3335.654738008976, 3350.407690680027, 3370.5445402503015, 3381.401525628567, 3403.6067163348202, 3429.353313004971, 3448.860714185238, 3465.1450356125833, 3486.1212334275247, 3491.682761156559, 3506.4179506182672, 3521.7438978075984, 3535.8572272419933, 3558.371926224232, 3571.810291254521, 3583.4508677899844, 3592.963027244807, 3612.501939588786, 3632.5454146921643, 3639.140546482802]</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>[0, 0.42, 0.77, 1.41, 1.93, 2.64, 3.7, 4.38, 5.82, 6.7, 7.32, 8.01, 8.7, 9.35, 10.22, 12.04, 12.78, 14.28, 15.09, 16.98, 17.9, 18.93, 19.68, 20.44, 21.36, 22.12, 22.9, 23.67, 24.46, 25.3, 26.5, 27.6, 28.69, 29.87, 30.99, 32.06, 33.19, 35.82, 37.38, 38.59, 39.71, 40.89, 43.54, 44.53, 47.2, 49.67, 51.88, 55.84, 58.44, 61.24, 63.31, 65.22, 67.19, 68.7, 70.38, 71.76, 73.83, 76.83, 79.19, 81.24, 83.79, 85.24, 86.78, 89.41, 91.78, 96.86, 99.58, 101.26, 102.73, 104.29, 106.24, 107.89, 110.53, 114.34, 115.91, 119.13, 122.19, 124.94, 128.14, 130.26, 132.29, 133.97, 135.56, 137.73, 139.31, 145.56, 149.98, 156.56, 159.45, 162.17, 165.86, 169.95, 171.95, 173.71, 175.72, 177.88, 182.63, 187.41, 192.67, 197.59, 201.41, 204.2, 206.79, 212.16, 217.06, 220.0, 222.64, 225.15, 228.01, 231.14, 234.08, 239.0, 243.6, 247.46, 252.41, 255.15, 257.96, 260.1, 262.9, 266.54, 268.74, 272.62, 275.85, 278.95, 282.3, 286.13, 291.83, 299.44, 306.97, 311.36, 319.02, 324.97, 329.17, 333.81, 338.7, 345.94, 353.17, 358.38, 364.74, 368.97, 374.14, 382.18, 386.71, 391.68, 395.3, 399.57, 403.86, 409.28, 414.25, 419.27, 424.51, 429.19, 434.43, 439.56, 444.48, 448.54, 453.19, 457.94, 461.58, 466.65, 472.49, 477.93, 483.4, 488.92, 494.45, 499.84, 506.08, 511.77, 517.2, 527.1, 533.48, 541.92, 546.63, 551.56, 558.35, 563.19, 570.28, 579.18, 584.56, 589.25, 597.3, 604.06, 609.99, 616.5, 621.82, 626.45, 632.71, 639.4, 645.95, 652.63, 659.72, 668.4, 677.1, 682.87, 688.32, 699.65, 705.83, 712.51, 718.75, 725.48, 733.32, 739.81, 748.91, 760.42, 768.68, 775.18, 787.81, 801.1, 810.51, 816.42, 822.48, 829.84, 836.77, 848.56, 858.9, 867.87, 875.79, 882.73, 889.68, 897.27, 907.53, 916.81, 924.86, 934.45, 944.5, 952.16, 958.34, 965.7, 971.88, 978.82, 985.84, 992.96, 1001.25, 1011.46, 1020.97, 1027.95, 1038.77, 1045.14, 1053.96, 1061.38, 1068.47]</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>[-10, 0, 0, -10, 0, -20, -20, 0, -20, 0, 0, 0, 0, 0, -20, -10, -20, 0, 0, 0, 0, -20, -20, 0, 0, 0, 0, -10, 0, 0, -10, -20, 0, -20, -10, -10, -20, -10, 0, 0, 0, 0, 0, -20, 0, -10, -10, 0, 0, 0, -10, 0, -20, 0, -10, -10, -20, 0, -10, 0, 0, 0, -10, 0, 0, 0, 0, -20, -20, -20, -20, -10, -10, 0, -10, 0, -20, 0, 0, 0, 0, -20, 0, -10, -10, -20, -10, -10, 0, -20, 0, -10, -10, 0, 0, -10, -20, -20, -20, -20]</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
-      <c r="O25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>redistrict</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1']</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>[100, 111, 111, 123, 165, 207, 207, 207, 207, 207]</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>[0.198, 0.199, 0.199, 0.203, 0.172, 0.167, 0.167, 0.167, 0.167, 0.167]</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270]</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>[0, 17.304834759235387, 35.616900861263275, 55.39017730951309, 77.2408075451851, 97.79770661592485, 104.06006765365602, 131.4601140022278, 144.17682921886447, 144.17682921886447]</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>[0, 0.59, 0.59, 1.21, 2.27, 4.52, 4.52, 4.52, 4.52, 4.52]</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>[0, -20, -10, 0, 0, 0, -10, 0, 0, -10, 0, 0, -20, 0, 0, 0, 0, -20, -20, -20, 0, 0, -10, -10, 0, -10, -10, -20, 0, 0, 0, -20, 0, 0, -10, -10, -20, -10, 0, -10, -10, -10, -10, 0, 0, 0, 0, 0, -20, 0, -10, 0, -10, -20, 0, -10, -20, -20, -10, 0, 0, 0, -10, 0, 0, 0, -10, 0, -10, 0, -20, 0, -20, -20, -20, 0, -20, 0, -20, -10, -10, -20, -10, -20, -20, 0, 0, 0, 0, 0, -20, -20, -20, 0, 0, -20, -10, 0, 0, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1260,134 +1760,484 @@
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
-      <c r="O31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>29</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>classWt</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3']</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>[81, 81, 81, 81, 81, 94, 110, 152, 201, 201, 209, 209, 230, 230, 230, 230, 230, 243, 245, 245, 269, 269, 272, 297, 300, 301, 301, 301, 335, 335, 335, 335, 335, 335, 335, 335, 335, 360, 388, 388, 388, 392, 392, 430, 430, 482, 519, 566, 574, 582, 587, 594, 594, 600, 600, 632, 632, 632, 633, 642, 642, 642, 647, 647, 647, 647, 647, 647, 664, 664, 664, 664, 665, 665, 665, 665, 665, 687, 700, 700, 700, 705, 726, 729, 772, 797, 816, 816, 816, 816, 836, 836, 836, 851, 851, 876, 876, 876, 877, 882, 882, 888, 938, 955, 955, 970, 970, 973, 976, 976, 989, 989, 989, 989, 1010, 1020, 1020, 1023, 1027, 1027, 1027]</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>[0.34, 0.34, 0.34, 0.34, 0.34, 0.331, 0.323, 0.31, 0.325, 0.325, 0.318, 0.318, 0.31, 0.31, 0.31, 0.31, 0.31, 0.31, 0.312, 0.312, 0.308, 0.308, 0.308, 0.314, 0.314, 0.318, 0.318, 0.318, 0.333, 0.333, 0.333, 0.333, 0.333, 0.333, 0.333, 0.333, 0.333, 0.336, 0.34, 0.34, 0.34, 0.34, 0.34, 0.35, 0.35, 0.34, 0.344, 0.348, 0.361, 0.361, 0.361, 0.361, 0.361, 0.361, 0.361, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.387, 0.391, 0.391, 0.391, 0.4, 0.423, 0.43, 0.432, 0.43, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.432, 0.442, 0.451, 0.451, 0.459, 0.459, 0.459, 0.459, 0.459, 0.459, 0.459, 0.459, 0.459, 0.466, 0.477, 0.477, 0.477, 0.477, 0.477, 0.477]</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>[0, 23.856158828735367, 42.300856208801285, 64.29429633617404, 90.1213070392609, 115.54642777442935, 131.59105591773988, 149.18485646247865, 164.2255795478821, 164.64527955055237, 185.23783984184266, 208.24199299812318, 229.33870725631715, 251.83971436023714, 277.1819151878357, 296.2778864860535, 313.35872735977176, 323.83122768402103, 338.0958549499512, 338.5155549526215, 360.32590594291696, 376.225103545189, 387.94243004322055, 412.6397286176682, 427.9298955440522, 451.5524374485017, 483.76703329086314, 503.39724545478833, 524.8309981346132, 540.5401240348817, 547.1715670943262, 557.0152592778207, 577.4422900319101, 596.5349129319193, 619.288473570347, 636.017285692692, 640.8850603580477, 653.0523926496508, 668.5011116504671, 693.6983852863314, 699.1202330946924, 722.116598236561, 735.4533750891687, 744.0469370245935, 761.7990160346033, 787.2504148840906, 796.4739151358606, 821.1817506670953, 836.3633979201318, 873.6474593520165, 883.6186181426049, 905.1162817835808, 917.9064456164838, 928.8631145298482, 945.29586699605, 970.7472658455373, 977.9061150610448, 1004.5515813887121, 1019.6064639151098, 1024.231721931696, 1034.8634219348432, 1039.7977311432364, 1049.2797328293327, 1069.6136255800727, 1082.5091286242011, 1105.6592113077643, 1123.8021601498128, 1145.164771538973, 1168.7109821140766, 1189.5049803555012, 1196.3964284360409, 1219.6578366935253, 1240.5153177917002, 1262.202307552099, 1284.987077373266, 1300.8046348273751, 1308.5445832431315, 1319.726883715391, 1342.1473517358302, 1366.2326067864894, 1369.3684320032596, 1390.2111294806002, 1406.3593386948107, 1428.3726532280443, 1450.6881904900072, 1475.6501393616197, 1484.2028395950792, 1510.7279166758058, 1523.1649366676804, 1523.1649366676804, 1530.8554864585396, 1553.7905689418312, 1565.4291837155815, 1582.7663772284982, 1599.5989309251306, 1624.0714298188684, 1633.6203767478464, 1659.2971470057962, 1674.4902663648127, 1683.3452309548852, 1694.8435811817644, 1707.7193357765673, 1732.2347803890702, 1755.4478998959062, 1780.8992987453935, 1793.9706556618212, 1818.3041283428668, 1829.2660163223743, 1854.2804545700549, 1875.8086318075655, 1883.241963046789, 1900.766563862562, 1921.6464538514613, 1944.3667514979838, 1964.3079737365244, 1980.665978783369, 1986.815974396467, 1999.5936750233172, 2017.4286880314348, 2024.5125865757464, 2029.5968315541743]</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>[0, 0.04, 0.07, 0.11, 0.15, 6.15, 12.55, 19.66, 28.33, 28.38, 29.66, 29.72, 35.73, 35.86, 35.94, 36.02, 36.08, 41.27, 41.83, 41.88, 49.86, 49.91, 50.68, 62.46, 63.85, 63.91, 63.96, 64.02, 68.01, 68.08, 68.14, 68.2, 68.28, 68.33, 68.4, 68.48, 68.55, 75.84, 84.05, 84.12, 84.2, 86.07, 86.13, 95.58, 95.73, 104.44, 115.08, 124.88, 126.41, 128.53, 131.25, 133.52, 133.74, 137.74, 137.86, 147.04, 147.38, 147.67, 148.32, 152.23, 152.34, 152.54, 154.32, 154.43, 154.54, 154.71, 154.89, 154.99, 160.36, 160.57, 160.83, 160.93, 162.43, 162.54, 162.66, 162.76, 162.85, 166.46, 169.08, 169.19, 169.38, 170.8, 175.14, 175.29, 190.0, 198.22, 205.66, 205.9, 206.07, 206.18, 214.83, 214.92, 215.03, 221.42, 221.53, 230.71, 231.04, 231.34, 231.85, 234.18, 234.28, 235.91, 254.96, 262.39, 262.53, 268.87, 269.02, 271.55, 273.07, 273.19, 280.32, 280.46, 280.55, 280.66, 293.12, 296.44, 296.56, 299.29, 301.3, 301.53, 301.69]</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>[0, -20, -20, 0, -10, -10, -20, -10, 0, -10, -20, 0, -10, -10, 0, -10, 0, -10, -20, 0, -10, 0, 0, 0, -20, -10, -20, 0, -20, 0, 0, -20, -10, -10, -10, 0, -20, -10, 0, 0, -20, -20, -20, 0, 0, -20, 0, 0, 0, 0, -20, -20, 0, -20, 0, 0, 0, -10, -10, 0, -20, -20, 0, 0, -20, -10, 0, 0, 0, 0, 0, 0, 0, -10, -10, 0, 0, 0, 0, -10, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>30</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5']</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>[81, 81, 81, 81, 81, 81, 81, 123, 173, 173, 197, 197, 197, 197, 197, 197, 207, 231, 253, 253, 253, 256, 256, 256, 256, 256, 256, 263, 290, 290, 290, 292, 292, 295, 329, 329, 329, 345, 360, 360, 360, 364, 414, 414, 414, 447, 447, 449, 450, 450, 453, 470, 475, 483, 500, 520, 521, 543, 543, 543, 568, 574, 582, 582, 582, 617, 622, 625, 625, 625, 636, 636, 670, 670, 670, 670, 670, 670, 670, 670, 689, 691, 694, 698, 701, 726, 726, 726, 726, 726, 748, 751, 753, 756, 759, 788, 788, 788, 788, 788, 806, 806, 815, 815, 815, 815, 832, 834, 834, 834, 834, 845, 845, 878, 878, 904, 941, 991, 992, 1006, 1016]</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>[0.34, 0.34, 0.34, 0.34, 0.34, 0.34, 0.34, 0.32, 0.336, 0.336, 0.331, 0.331, 0.331, 0.331, 0.331, 0.331, 0.331, 0.327, 0.323, 0.323, 0.323, 0.331, 0.331, 0.331, 0.331, 0.331, 0.331, 0.329, 0.316, 0.316, 0.316, 0.314, 0.314, 0.31, 0.316, 0.316, 0.316, 0.338, 0.338, 0.338, 0.338, 0.336, 0.336, 0.336, 0.336, 0.35, 0.35, 0.352, 0.352, 0.352, 0.363, 0.363, 0.37, 0.376, 0.376, 0.376, 0.376, 0.387, 0.387, 0.387, 0.387, 0.387, 0.387, 0.387, 0.387, 0.385, 0.385, 0.391, 0.391, 0.391, 0.393, 0.393, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.395, 0.408, 0.414, 0.415, 0.429, 0.429, 0.429, 0.429, 0.429, 0.43, 0.43, 0.436, 0.436, 0.436, 0.436, 0.436, 0.436, 0.436, 0.436, 0.438, 0.438, 0.44, 0.44, 0.44, 0.44, 0.436, 0.438, 0.438, 0.438, 0.438, 0.44, 0.44, 0.442, 0.442, 0.438, 0.444, 0.453, 0.459, 0.466, 0.466]</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>[0, 21.922707271575923, 39.34269924163818, 56.52800204753875, 70.43494615554809, 93.08077051639557, 111.78835813999177, 129.38215868473054, 145.59442758560184, 146.01412758827212, 167.80468773841858, 185.39314777851106, 204.56921260356904, 226.30742008686067, 249.57749235630035, 265.9266706943512, 272.9049094557762, 283.7868059515953, 302.3786983132362, 304.7399978280067, 309.6218179821968, 322.6179186701774, 342.6720397830009, 366.4298694014549, 388.27524341344827, 405.4395485043525, 410.9327019453048, 422.4424002170562, 439.806651186943, 462.47512652873985, 467.90175985097875, 483.43209398984897, 506.63989800214756, 529.9966602206229, 554.1601445078849, 568.2816426634788, 575.0788566350936, 588.983668398857, 607.4842513561248, 619.7630088329314, 626.2652058839797, 641.7854815959929, 668.1867307662963, 686.5845162391661, 711.4633664131163, 724.3558951616286, 743.198791873455, 757.6831400394439, 779.8035799264907, 801.0843041419981, 806.434346783161, 814.2742400765418, 831.8608782708644, 848.3311093747615, 873.7167581021785, 887.5096353471279, 896.9028989076614, 916.4298953533173, 936.6710060596466, 958.1991832971573, 969.7699946045876, 980.0758841633798, 994.2733806788923, 1015.1171404302122, 1042.0368892133238, 1059.8515006005766, 1072.8340750634673, 1081.677668744326, 1103.8901950180534, 1124.6760200798515, 1129.350602179766, 1135.4210808932783, 1156.4111414134504, 1175.8531144797803, 1201.7939633071423, 1220.4231270968914, 1235.3836155354977, 1252.3714719355107, 1273.9425081312656, 1292.996181732416, 1300.0654648840427, 1322.8372196495534, 1344.8506752073765, 1365.8514264166356, 1388.6318707048895, 1413.593819576502, 1421.475719791651, 1445.8750679552559, 1458.1689590990547, 1458.1689590990547, 1466.574908870459, 1485.981618970633, 1500.3381455600265, 1523.5618314445023, 1539.8335773646836, 1565.7744261920457, 1572.8178263843065, 1598.3281614482407, 1611.8297307431703, 1611.8297307431703, 1623.3923134803777, 1639.4602664709096, 1651.2741932034496, 1668.3021254658702, 1688.85902453661, 1702.255607569218, 1713.4407410562042, 1726.416945511103, 1747.9604556858542, 1769.4886323273183, 1777.8733648240568, 1802.2871642053128, 1815.6897361934186, 1821.9422197520735, 1837.4921159207822, 1862.9435147702695, 1871.496215003729, 1896.6885178983214, 1908.580880993605, 1922.4253074586395, 1941.8136782705787]</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>[0, 0.03, 0.09, 0.13, 0.17, 0.21, 0.25, 13.99, 28.31, 28.36, 34.81, 34.85, 34.9, 34.94, 34.99, 35.1, 37.2, 43.95, 52.58, 52.65, 52.74, 53.38, 53.44, 53.6, 53.66, 53.73, 53.92, 56.41, 67.66, 67.72, 67.82, 70.3, 70.42, 72.35, 84.16, 84.31, 84.37, 89.13, 93.74, 93.82, 93.89, 98.5, 113.85, 113.89, 113.96, 123.41, 123.63, 124.8, 124.86, 124.98, 125.51, 132.45, 134.69, 137.12, 143.49, 149.34, 149.49, 155.87, 156.03, 156.18, 163.19, 166.91, 170.38, 170.47, 170.56, 185.16, 187.0, 188.83, 188.91, 189.01, 194.01, 194.31, 202.6, 202.72, 203.09, 203.19, 203.31, 203.42, 203.53, 203.67, 217.49, 219.06, 219.83, 221.22, 223.19, 227.24, 227.42, 227.53, 227.77, 227.9, 235.44, 236.84, 237.6, 238.78, 241.66, 259.38, 259.51, 259.62, 259.78, 259.89, 269.35, 269.45, 274.24, 274.35, 274.45, 274.56, 282.8, 284.13, 284.28, 284.38, 284.49, 291.47, 291.56, 299.0, 299.33, 310.75, 325.05, 342.43, 343.49, 352.24, 354.65]</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>[-20, -20, 0, 0, 0, 0, -10, -20, -20, -20, -20, 0, 0, 0, 0, 0, 0, 0, 0, -20, -20, -20, 0, -20, 0, -10, -10, -10, -20, -10, -10, -10, 0, 0, -20, -20, 0, -20, -10, 0, -10, 0, 0, 0, 0, -10, -20, 0, 0, -10, -10, 0, 0, 0, -10, 0, -20, -10, 0, 0, 0, -20, -20, -10, -10, 0, 0, 0, -20, 0, 0, 0, -10, -20, -10, 0, 0, 0, 0, -10, -10]</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>31</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>clusterWt</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5']</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>[81, 81, 81, 81, 81, 86, 86, 121, 171, 171, 196, 196, 243, 243, 243, 247, 247, 272, 274, 274, 295, 295, 295, 295, 295, 296, 297, 344, 374, 374, 374, 382, 387, 392, 395, 449, 460, 460, 460, 460, 479, 479, 483, 513, 518, 537, 537, 537, 546, 546, 546, 555, 555, 566, 566, 613, 650, 691, 693, 748, 748, 748, 748, 748, 754, 755, 755, 779, 807, 807, 807, 807, 807, 807, 807, 807, 807, 826, 838, 838, 838, 838, 838, 857, 857, 887, 887, 887, 887, 887, 887, 901, 904, 909, 927, 953, 980, 980, 980, 980, 997, 999, 1005, 1008, 1027, 1027, 1051, 1051, 1051, 1051, 1065, 1065, 1065, 1065, 1065, 1065, 1065, 1085, 1088, 1088, 1089]</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>[0.34, 0.34, 0.34, 0.34, 0.34, 0.316, 0.316, 0.308, 0.325, 0.325, 0.325, 0.325, 0.318, 0.318, 0.318, 0.329, 0.329, 0.325, 0.325, 0.325, 0.318, 0.318, 0.318, 0.318, 0.318, 0.323, 0.321, 0.34, 0.35, 0.35, 0.35, 0.342, 0.353, 0.359, 0.357, 0.353, 0.353, 0.353, 0.353, 0.353, 0.357, 0.357, 0.359, 0.365, 0.365, 0.378, 0.378, 0.378, 0.389, 0.389, 0.389, 0.389, 0.389, 0.391, 0.391, 0.391, 0.397, 0.397, 0.402, 0.41, 0.41, 0.41, 0.41, 0.41, 0.417, 0.417, 0.417, 0.417, 0.425, 0.425, 0.425, 0.425, 0.425, 0.425, 0.425, 0.425, 0.425, 0.436, 0.44, 0.44, 0.44, 0.44, 0.44, 0.44, 0.44, 0.44, 0.44, 0.44, 0.44, 0.44, 0.44, 0.449, 0.457, 0.459, 0.464, 0.462, 0.457, 0.457, 0.457, 0.457, 0.461, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.468, 0.47, 0.47, 0.47, 0.47]</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>[0, 21.726144647598275, 39.14613661766053, 61.00708584785464, 87.8597085952759, 110.57727770805361, 129.69155201911929, 144.35305247306826, 158.75443112850192, 159.1741311311722, 180.54789798259736, 203.12604830265047, 226.27637164592747, 246.18836541175847, 268.2576874494553, 290.24190847873695, 306.50937597751624, 324.103176522255, 339.66129682064064, 340.08099682331095, 360.69554693698893, 382.2973785161973, 404.5897780895234, 428.5922714233399, 450.34401788711557, 467.29314527511605, 474.50054817199714, 487.84452316761025, 506.3072294473649, 512.4466081857682, 532.0929569602014, 550.1044395565988, 568.5100787997247, 587.3215319991114, 610.1019762873651, 636.5322750926019, 645.0849753260615, 663.5091089606287, 676.2095657229426, 676.2095657229426, 685.5097654700281, 709.0296098828318, 711.4091183781626, 733.7653115630152, 747.8043572545054, 770.9544307351115, 803.1584267258647, 823.5437591195109, 844.6734031796458, 868.1932018399241, 874.580899512768, 888.4716507792475, 901.2079439401629, 911.9809962511065, 928.1311363935473, 953.5825352430346, 962.1352354764941, 987.3275383710865, 1001.0784038722519, 1026.7111961066726, 1034.9362959444525, 1048.36754835248, 1070.445562773943, 1094.812150079012, 1117.7466780483724, 1135.0838474571706, 1142.8264281451702, 1155.535363394022, 1174.5283589899539, 1177.8341783106325, 1182.9280461013316, 1196.7982217252254, 1217.239083570242, 1237.9922945201397, 1256.0176669299603, 1267.5729251086714, 1275.0677368938925, 1287.0413744032385, 1305.2227020323278, 1311.8343406736851, 1317.3505568861963, 1335.0326438307764, 1342.4597284793856, 1350.917275631428, 1366.2140154957774, 1392.6443143010142, 1399.687714493275, 1424.8800173878674, 1439.568729937077, 1460.3266152262693, 1472.189840650559, 1491.6251911640172, 1506.2358679056172, 1530.2750841856007, 1553.9853425264362, 1579.4367413759235, 1588.4925416231158, 1615.892637562752, 1627.4458522558216, 1627.4458522558216, 1633.4389057874682, 1654.8959494352343, 1671.5503826618196, 1687.8662372589113, 1711.111588573456, 1735.094637489319, 1744.318137741089, 1763.2147556304933, 1774.0411908626559, 1774.0411908626559, 1783.5202406048777, 1803.5423739075663, 1823.7691734433176, 1844.8512981534006, 1868.322266495228, 1892.1922306180002, 1907.2395851254464, 1924.4144856572152, 1938.5571657061578, 1938.976865708828, 1959.568219792843]</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>[0, 0.03, 0.08, 0.11, 0.14, 2.88, 2.94, 23.49, 37.62, 37.67, 43.52, 43.57, 54.63, 54.68, 54.85, 56.2, 56.27, 64.22, 65.32, 65.41, 69.88, 69.96, 70.13, 70.18, 70.24, 70.29, 70.36, 88.83, 95.65, 95.74, 95.81, 102.75, 104.25, 104.68, 107.6, 121.79, 124.28, 124.34, 124.49, 124.57, 129.72, 129.91, 131.53, 140.13, 142.59, 145.14, 145.36, 145.47, 147.25, 147.34, 147.43, 152.03, 152.14, 155.61, 155.7, 172.01, 180.62, 190.22, 190.68, 204.58, 204.75, 204.85, 204.95, 205.05, 206.98, 207.94, 208.21, 215.53, 222.22, 222.55, 222.68, 222.92, 223.03, 223.13, 223.27, 223.38, 223.49, 230.2, 235.15, 235.26, 235.37, 235.48, 235.72, 242.91, 243.2, 253.22, 253.34, 253.45, 253.58, 253.98, 254.09, 261.81, 263.37, 265.95, 271.86, 280.53, 289.47, 289.79, 290.14, 290.25, 299.46, 301.3, 302.99, 304.15, 317.33, 317.43, 329.22, 329.33, 329.59, 329.69, 338.39, 338.49, 338.66, 338.79, 338.94, 339.14, 339.24, 352.17, 354.45, 354.57, 354.73]</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>[0, 0, -10, 0, -10, -10, -10, -10, 0, -10, -10, 0, -10, 0, 0, -10, 0, -10, -10, 0, 0, 0, -20, 0, -20, -20, -20, 0, -20, 0, -20, -20, 0, -20, -20, -20, 0, -10, 0, 0, -20, -20, -20, 0, 0, -20, 0, 0, -20, 0, -20, -20, 0, -20, 0, -20, 0, -10, -10, 0, -10, 0, 0, 0, -10, 0, 0, -10, 0, 0, 0, 0, 0, -10, -10, -10, 0, 0, 0, -20, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
-      <c r="O34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>32</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>clusterStdLow</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5']</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>[81, 81, 81, 82, 82, 83, 83, 127, 176, 176, 197, 197, 197, 198, 238, 243, 245, 263, 291, 291, 291, 291, 291, 300, 300, 302, 302, 332, 364, 364, 364, 364, 367, 388, 388, 388, 388, 388, 418, 418, 418, 450, 503, 503, 514, 542, 551, 553, 553, 553, 579, 592, 592, 605, 605, 649, 686, 729, 752, 770, 770, 801, 806, 813, 854, 880, 880, 880, 880, 880, 899, 900, 900, 900, 909, 916, 916, 943, 950, 950, 950, 950, 985, 986, 986, 986, 990, 1011, 1014, 1014, 1025, 1025, 1025, 1046, 1046, 1065, 1065, 1065, 1081, 1081, 1081, 1081, 1081, 1081, 1081, 1081, 1081, 1109, 1130, 1130, 1130, 1130, 1130, 1130, 1130, 1130, 1130, 1130, 1130, 1130, 1130]</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>[0.34, 0.34, 0.34, 0.34, 0.34, 0.338, 0.338, 0.321, 0.336, 0.336, 0.333, 0.333, 0.333, 0.331, 0.316, 0.316, 0.325, 0.336, 0.327, 0.327, 0.327, 0.327, 0.327, 0.325, 0.325, 0.333, 0.333, 0.367, 0.382, 0.382, 0.382, 0.382, 0.383, 0.382, 0.382, 0.382, 0.382, 0.382, 0.389, 0.389, 0.389, 0.389, 0.393, 0.393, 0.389, 0.4, 0.404, 0.406, 0.406, 0.406, 0.41, 0.41, 0.41, 0.412, 0.412, 0.412, 0.415, 0.417, 0.43, 0.43, 0.43, 0.457, 0.462, 0.47, 0.468, 0.466, 0.466, 0.466, 0.466, 0.466, 0.477, 0.479, 0.479, 0.479, 0.477, 0.477, 0.477, 0.485, 0.487, 0.487, 0.487, 0.487, 0.489, 0.489, 0.489, 0.489, 0.489, 0.489, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.492, 0.496, 0.502, 0.502, 0.502, 0.502, 0.502, 0.502, 0.502, 0.502, 0.502, 0.502, 0.502, 0.502, 0.502]</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>[0, 19.596130466461183, 33.94200620651245, 57.6383748292923, 78.83580725193025, 102.0829753637314, 119.57050292491915, 138.00210349559785, 153.81892240047458, 154.23862240314486, 175.66227262020112, 193.19207646846772, 203.59093849658967, 227.35545599460602, 251.97586262226105, 267.6092005252838, 272.7922296583653, 283.67898043990135, 297.85067812800406, 315.32429453730583, 320.35395511984825, 341.419963568449, 361.37125806212424, 379.3068043410778, 401.10016304850575, 416.3692533433437, 423.20595727562903, 437.1810567200184, 455.0732391178608, 482.93657339215275, 488.2484609663486, 510.8090600311756, 523.0710148155689, 543.0286626636981, 553.820187741518, 576.9702790558338, 608.9335749924182, 630.9482578098773, 655.3188226044177, 677.7490204155445, 684.7613814651966, 695.5349841892719, 723.8220367729664, 745.1778134405613, 773.9896122515202, 787.2009940445423, 800.7610552072525, 812.1668034791946, 834.062025475502, 855.0953021049498, 863.499031293392, 886.0171519637106, 899.4165634751319, 913.7319386601447, 930.6181389927863, 955.5800878643988, 966.0762359976767, 993.2061653494834, 1012.7259951233863, 1029.5038227677344, 1039.4514601469039, 1054.6632717370985, 1078.698614645004, 1100.0056664466856, 1122.3212037086485, 1148.2620525360105, 1157.820952796936, 1183.3313869476317, 1195.696739554405, 1195.696739554405, 1205.8743126630782, 1220.8807174682615, 1238.9563171386717, 1260.7343644618986, 1285.9003931522368, 1301.4365975141525, 1309.525385272503, 1319.9662921071053, 1339.315213406086, 1347.81589165926, 1353.3320616841318, 1374.2062006592753, 1397.4013743996622, 1420.1546790480616, 1440.6790503621103, 1463.681015789509, 1480.8076468586924, 1499.239247429371, 1515.2035175919534, 1516.665368962288, 1538.89811937809, 1561.8884588956835, 1576.0463276624682, 1580.993284839392, 1592.3139805972578, 1616.2970295131208, 1625.9325783312322, 1652.5782833158971, 1672.316094762087, 1688.6278716385366, 1698.1178412139418, 1715.4650863826278, 1733.1065323293212, 1757.1715266168121, 1777.3240040719513, 1792.6547310292724, 1797.8712844431404, 1815.834473997355, 1835.6716055452828, 1857.3955610811715, 1862.7459137260919, 1886.1889055550103, 1901.728897982836, 1913.6834874689582, 1926.3304812729361, 1949.8240802109244, 1957.7059804260734, 1982.8982833206658, 1999.7895637810234, 2015.028240090609, 2025.475190085173]</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>[0, 0.09, 0.15, 0.2, 0.22, 0.29, 0.33, 11.99, 20.79, 20.82, 27.13, 27.18, 27.23, 27.31, 45.36, 46.09, 46.14, 52.72, 62.64, 62.72, 62.85, 62.91, 62.97, 66.49, 66.68, 67.04, 67.11, 73.97, 89.28, 89.36, 89.42, 89.53, 91.98, 106.53, 106.6, 106.67, 106.74, 106.83, 114.24, 114.33, 114.5, 125.29, 146.0, 146.09, 155.18, 160.09, 162.2, 162.66, 162.75, 163.03, 173.98, 181.19, 181.46, 185.93, 186.04, 197.75, 213.8, 240.93, 247.2, 253.97, 254.08, 262.7, 265.23, 266.76, 282.58, 294.97, 295.09, 295.21, 295.35, 295.47, 299.34, 300.22, 300.37, 300.46, 304.4, 306.52, 306.66, 313.32, 315.53, 315.67, 315.79, 315.97, 325.17, 326.18, 326.47, 326.72, 332.46, 340.5, 342.58, 342.72, 348.25, 348.4, 348.57, 363.93, 364.06, 370.28, 370.38, 370.51, 383.11, 383.25, 383.41, 383.54, 383.66, 383.83, 384.17, 384.3, 384.43, 391.23, 397.06, 397.2, 397.38, 397.56, 397.71, 397.81, 397.98, 398.11, 398.34, 398.68, 398.86, 399.04, 399.16]</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>[0, -10, -10, 0, -10, -10, -10, -10, 0, -10, -10, 0, -10, -10, 0, -10, 0, -10, -10, 0, 0, 0, -20, 0, -20, -20, -20, 0, -20, 0, 0, -20, 0, -20, -20, 0, -20, -20, 0, -20, -20, -10, -20, 0, 0, -20, 0, 0, 0, 0, -20, -20, 0, -20, 0, -20, 0, -20, -20, 0, -10, -10, 0, 0, -10, 0, 0, 0, 0, 0, 0, 0, 0, -10, -10, 0, 0, -10, 0, 0, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>33</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>clusterStdHigh</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4']</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>[81, 81, 81, 81, 81, 85, 86, 110, 160, 160, 179, 210, 210, 222, 223, 268, 305, 355, 391, 410, 413, 423, 423, 448, 448, 480, 480, 480, 481, 482, 482, 482, 530, 530, 532, 532, 532, 563, 565, 565, 574, 585, 591, 595, 638, 664, 671, 671, 671, 671, 683, 683, 686, 686, 686, 686, 686, 686, 686, 686, 686, 695, 699, 703, 714, 731, 749, 749, 749, 749, 764, 765, 765, 765, 800, 802, 805, 833, 862, 862, 862, 862, 866, 866, 866, 866, 866, 866, 875, 875, 875, 878, 905, 905, 905, 932, 932, 942, 948, 948, 962, 962, 965, 965, 965, 965, 965, 965, 988, 988, 988, 988, 990, 990, 990, 1033, 1033, 1033, 1033, 1033, 1033]</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>[0.34, 0.34, 0.34, 0.34, 0.34, 0.333, 0.331, 0.312, 0.329, 0.329, 0.327, 0.32, 0.32, 0.329, 0.329, 0.318, 0.321, 0.325, 0.338, 0.338, 0.34, 0.34, 0.34, 0.344, 0.344, 0.338, 0.338, 0.338, 0.338, 0.338, 0.338, 0.338, 0.336, 0.336, 0.34, 0.34, 0.34, 0.34, 0.34, 0.34, 0.342, 0.357, 0.368, 0.372, 0.378, 0.38, 0.383, 0.383, 0.383, 0.383, 0.395, 0.395, 0.393, 0.393, 0.393, 0.393, 0.393, 0.393, 0.393, 0.393, 0.393, 0.389, 0.389, 0.391, 0.395, 0.393, 0.393, 0.393, 0.393, 0.393, 0.398, 0.398, 0.398, 0.398, 0.406, 0.406, 0.406, 0.442, 0.447, 0.447, 0.447, 0.447, 0.451, 0.451, 0.451, 0.451, 0.451, 0.451, 0.459, 0.459, 0.459, 0.459, 0.459, 0.459, 0.459, 0.468, 0.468, 0.474, 0.47, 0.47, 0.472, 0.472, 0.472, 0.472, 0.472, 0.472, 0.472, 0.472, 0.474, 0.474, 0.474, 0.474, 0.474, 0.474, 0.474, 0.479, 0.479, 0.479, 0.479, 0.479, 0.479]</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>[0, 21.300141811370857, 39.887219572067266, 62.55583891868592, 85.74716260433199, 108.40188162326815, 123.20224168300632, 133.25584199428562, 146.62242622375493, 147.0421262264252, 164.41777520179753, 183.10300822258, 194.7385937929154, 203.9368206083775, 219.26949195265775, 241.29474095702176, 251.5244412362576, 278.1701462209225, 298.6471780240536, 313.1025563657284, 330.62475715279584, 355.5350684702397, 369.6929372370244, 384.08985684514056, 396.89323244690905, 412.55563173890124, 420.9406319677831, 447.586336952448, 461.465710002184, 466.1262176811696, 474.87154607176785, 497.0236935555935, 521.295103687048, 539.1348004043103, 566.0641493737699, 589.9341134965421, 608.2350144326688, 626.2477149903775, 643.3580269277097, 643.77772693038, 666.8258288323881, 685.7369387567045, 704.4909392535689, 724.2163348853591, 746.531872147322, 771.9832709968093, 780.3682712256912, 804.9338744819167, 817.886127084494, 817.886127084494, 823.7410146594051, 830.4690760254863, 832.3726828217509, 850.8871530175212, 864.6142657160761, 888.2368081927302, 919.5478545069698, 940.907718408108, 961.0608115077022, 981.6026076197627, 988.6175620317462, 1006.7083109140399, 1023.6945741653445, 1045.7438145160677, 1067.1295377254487, 1092.0914865970612, 1101.0350868225098, 1127.962767314911, 1141.0649610757828, 1141.0649610757828, 1150.5440108180046, 1164.0242672801019, 1186.0206698536874, 1209.3784827828408, 1233.0723604798318, 1247.675607788563, 1255.883793950081, 1270.9590573310854, 1288.7832529544833, 1312.8685080051425, 1318.4855572700503, 1324.9682680606845, 1332.949624681473, 1359.236613798142, 1367.4915650129321, 1390.1662002801897, 1424.6801959753038, 1440.986847996712, 1459.135565853119, 1469.8970279693606, 1476.4257682561877, 1491.579498112202, 1512.323337042332, 1530.6623793244364, 1557.0926781296732, 1570.9447108864786, 1594.627580022812, 1608.1846350550652, 1633.7053838849067, 1650.5320047259331, 1658.1868440032006, 1670.242247593403, 1683.0327023625375, 1706.119749748707, 1717.1614248633387, 1740.7839651942254, 1768.6278616309166, 1783.1055141329766, 1804.9765327572823, 1819.4436793684959, 1825.730623757839, 1853.6596663355826, 1855.087371432781, 1873.7347331643102, 1883.4601977944371, 1906.6102672219274, 1934.204863655567, 1959.2054611325261, 1979.3483237385747, 2011.5122946858403, 2017.9201418519017]</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>[0, 0.18, 0.22, 0.25, 0.3, 0.34, 0.38, 6.81, 17.66, 17.71, 23.07, 35.55, 35.6, 40.27, 40.76, 57.51, 70.82, 85.24, 102.45, 110.74, 113.2, 119.51, 119.62, 131.09, 131.16, 143.08, 143.15, 143.24, 143.56, 143.98, 144.12, 144.22, 168.61, 168.7, 169.4, 169.56, 169.64, 185.88, 187.09, 187.19, 190.77, 193.54, 195.04, 195.77, 208.59, 216.22, 217.54, 217.72, 217.83, 217.95, 220.69, 220.87, 223.4, 223.52, 223.74, 223.83, 223.95, 224.08, 224.16, 224.25, 224.34, 228.49, 231.28, 233.89, 238.82, 247.87, 254.38, 254.47, 254.56, 254.66, 259.04, 260.1, 260.2, 260.3, 268.97, 270.09, 271.41, 279.75, 287.88, 287.98, 288.12, 288.24, 291.22, 291.32, 291.44, 291.54, 291.67, 291.84, 295.39, 295.55, 295.66, 295.98, 311.64, 311.91, 312.02, 321.58, 321.74, 324.79, 326.62, 326.76, 331.62, 331.77, 333.03, 333.15, 333.35, 333.46, 333.59, 333.68, 338.35, 338.68, 338.81, 338.94, 340.21, 340.3, 340.42, 350.85, 351.16, 351.34, 351.47, 351.59, 351.74]</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>[-10, 0, 0, -10, 0, 0, 0, 0, -20, 0, 0, -10, 0, 0, -10, 0, -20, 0, 0, -20, -20, -10, 0, -20, 0, -20, 0, -20, 0, -20, -10, 0, -20, 0, 0, 0, 0, 0, -20, 0, -20, 0, -10, -20, -20, 0, -20, -20, -10, -20, 0, 0, -10, 0, -10, 0, -10, 0, 0, -20, 0, 0, -10, -20, 0, 0, -10, -20, -10, -10, -10, -20, -10, 0, 0, 0, -10, 0, -10, 0, -10]</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>complete</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>34</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4']</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>[81, 81, 81, 81, 81, 81, 81, 122, 171, 171, 193, 218, 218, 246, 246, 298, 331, 378, 400, 409, 419, 419, 435, 435, 435, 435, 435, 461, 463, 463, 479, 479, 515, 524, 524, 540, 540, 540, 540, 540, 540, 540, 559, 559, 559, 559, 559, 568, 570, 570, 572, 572, 572, 572, 572, 574, 574, 600, 631, 631, 631, 631, 650, 650, 650, 650, 650, 652, 654, 654, 656, 658, 677, 677, 677, 692, 700, 700, 745, 745, 745, 745, 758, 758, 758, 758, 758, 758, 763, 763, 763, 771, 776, 776, 776, 799, 799, 802, 804, 804, 804, 811, 817, 822, 824, 863, 863, 863, 863, 863, 877, 877, 877, 877, 877, 877, 877, 877, 901, 925, 925]</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>[0.338, 0.338, 0.338, 0.338, 0.338, 0.338, 0.338, 0.327, 0.342, 0.342, 0.335, 0.327, 0.327, 0.335, 0.335, 0.308, 0.306, 0.301, 0.314, 0.314, 0.314, 0.314, 0.314, 0.314, 0.314, 0.314, 0.314, 0.312, 0.314, 0.314, 0.314, 0.314, 0.316, 0.316, 0.316, 0.321, 0.321, 0.321, 0.321, 0.321, 0.321, 0.321, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.32, 0.321, 0.321, 0.336, 0.344, 0.344, 0.344, 0.344, 0.344, 0.344, 0.344, 0.344, 0.344, 0.344, 0.344, 0.344, 0.344, 0.34, 0.346, 0.346, 0.346, 0.355, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.365, 0.374, 0.374, 0.374, 0.382, 0.383, 0.383, 0.383, 0.385, 0.385, 0.385, 0.383, 0.383, 0.383, 0.389, 0.397, 0.402, 0.406, 0.412, 0.412, 0.412, 0.412, 0.412, 0.421, 0.421, 0.421, 0.421, 0.421, 0.421, 0.421, 0.421, 0.421, 0.432, 0.432]</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600]</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>[0, 21.174196553230264, 34.83693535327909, 54.5662326335907, 75.06220047473907, 91.55417568683625, 106.6015831232071, 123.7764836549759, 138.81720674037936, 139.23690674304964, 159.02886674404147, 178.65846850872043, 190.74156444668773, 199.82547436952595, 214.23935793638233, 239.69075678586964, 245.22485693693164, 271.38609455823905, 290.3669052720071, 296.85636631250395, 308.13712353706376, 330.71527385711687, 354.01827645301836, 376.1764125585558, 400.8534509420397, 426.04911382198355, 437.84302775859857, 458.36912839412713, 472.8924542665484, 473.3121542692187, 496.3025676488879, 510.54211685657526, 527.6745780229571, 548.9404264688494, 563.4568665027621, 587.5518502235415, 620.2178461551669, 641.6535946369173, 661.3656582355502, 693.0566296100619, 699.9480776906016, 720.822216665745, 733.3340707898143, 754.8294030070308, 778.5877518296245, 802.4577159523967, 819.1318701386455, 837.5634707093242, 852.0867965817455, 852.5064965844158, 869.4813462853435, 884.947803795338, 906.6086448788647, 930.0638345599178, 950.9282005190853, 967.3851331114772, 974.2712420701984, 984.7314329504969, 1001.9874625802042, 1027.0172374367717, 1032.3259065032007, 1054.9040568232538, 1077.2676833987239, 1100.1912030816081, 1124.8011721968653, 1148.3721367716792, 1165.4529776453974, 1183.0467781901361, 1194.695680910349, 1195.1153809130192, 1216.9523331224918, 1233.6671654284, 1248.7172618448735, 1269.3601649343968, 1293.3432138502599, 1303.9072830259802, 1316.6981552600862, 1325.8129725933077, 1344.359841990471, 1365.888019371033, 1379.8238275527956, 1385.7244856119157, 1401.429241681099, 1426.2682893037797, 1438.5398235797884, 1454.603150367737, 1473.4197479248048, 1493.9982809066773, 1515.2749605178833, 1539.6671591758727, 1546.424054789543, 1560.6564653635025, 1562.9207699537278, 1572.6402609825136, 1598.5811098098757, 1613.2130636930467, 1627.2890592038632, 1639.428964227438, 1663.6129061162471, 1682.6665790498255, 1700.2195829689501, 1714.0716726124285, 1735.1348836958407, 1756.840734630823, 1778.691364866495, 1803.1638637602327, 1809.03336392045, 1835.9609351694583, 1847.7905199348925, 1847.7905199348925, 1856.5541696965693, 1857.783019608259, 1871.160915416479, 1894.0288350522517, 1905.751048272848, 1926.066417068243, 1950.416414064169, 1967.203779166937, 1991.182788461447, 2007.8645148694518, 2014.3932551562789]</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>[0, 0.07, 0.11, 0.15, 0.18, 0.22, 0.32, 0.36, 0.47, 0.54, 0.63, 0.74, 0.84, 0.93, 1.02, 1.12, 1.42, 1.58, 1.73, 1.91, 2.09, 2.24, 2.44, 2.54, 2.68, 2.83, 2.97, 3.13, 3.34, 3.73, 3.9, 4.05, 4.61, 5.09, 5.34, 5.68, 5.85, 6.45, 6.73, 6.95, 7.19, 7.42, 7.85, 8.09, 8.33, 8.53, 8.77, 9.06, 9.29, 9.49, 9.75, 10.26, 10.5, 10.98, 11.18, 11.4, 11.64, 11.92, 12.15, 12.4, 12.79, 13.01, 13.25, 13.49, 13.75, 14.04, 14.24, 14.84, 15.15, 15.36, 15.7, 16.0, 16.27, 16.59, 16.9, 17.17, 17.53, 17.79, 18.06, 18.44, 19.2, 19.49, 19.88, 20.2, 20.55, 20.84, 21.16, 21.63, 22.0, 22.64, 23.03, 23.4, 23.71, 24.0, 24.63, 25.06, 25.42, 25.77, 26.14, 26.46, 26.81, 27.12, 27.53, 28.25, 28.63, 29.04, 29.49, 29.92, 30.28, 30.76, 31.19, 31.6, 31.99, 32.39, 32.75, 33.19, 33.5, 34.18, 35.11, 35.5, 36.16]</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>[0, -10, 0, 0, 0, -10, -10, -10, 0, -20, 0, 0, 0, 0, -20, 0, -10, -10, 0, -20, 0, -20, 0, 0, 0, 0, -10, 0, -20, 0, 0, -10, 0, -10, -10, -20, -10, 0, 0, -20, -10, -20, 0, -10, -20, -10, 0, 0, 0, 0, -20, -10, -20, -20, 0, -20, -20, -20, -10, 0, -20, -10, -20, 0, -20, 0, -10, -10, -20, 0, 0, 0, 0, -20, 0, 0, 0, 0, 0, 0, -10]</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>35</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>grocery</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>redistrict</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3']</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>[81, 81, 81, 81]</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>[0.338, 0.338, 0.338, 0.338]</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90]</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>[0, 23.00415315628053, 41.79809532165529, 59.90197055339816]</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>[0, 0.0, 0.0, 0.0]</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>[0, -20, -10, 0, -20, 0, 0, -10, 0, -10, -10, 0, -10, 0, 0, -20, 0, 0, 0, -20, -20, 0, 0, -10, 0, 0, 0, 0, -20, -20, -10, 0, 0, -10, 0, -20, 0, 0, -20, 0, -10, -10, -10, 0, -10, 0, -20, -10, 0, 0, 0, -20, 0, 0, 0, 0, -20, 0, -20, -20, 0, -10, -10, 0, -10, 0, 0, 0, -20, -10, 0, 0, 0, -20, -20, -20, -10, -20, -10, -20, -10]</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1488,96 +2338,346 @@
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>41</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>classWt</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1']</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>[100, 105, 108, 141, 141, 177, 177, 182, 187, 187, 194, 227, 275, 275, 275, 311, 311, 312, 318, 318, 334, 334, 337, 349, 349, 349, 349, 349, 349, 349, 349, 357, 357, 357, 357, 357, 357, 400, 459, 459, 463, 502, 502, 547, 551, 597, 644, 698, 699, 755, 761, 799, 799, 807, 807, 851, 907, 962, 969, 974, 980, 1016, 1016, 1038, 1042, 1087, 1138, 1194, 1197, 1213, 1218, 1255, 1255, 1265, 1269, 1313, 1369, 1420, 1421, 1474, 1478, 1517, 1517, 1523, 1525, 1572, 1628, 1678, 1679, 1687, 1694, 1698, 1698, 1698, 1698, 1698, 1706, 1747, 1798, 1798, 1815, 1821, 1826, 1830, 1833, 1873, 1899, 1899, 1899, 1899, 1916, 1916, 1916, 1916, 1945, 1945, 1945, 1959, 1986, 1986, 1986, 1994, 1996, 1996, 2013, 2054, 2074, 2074, 2074, 2074]</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>[0.175, 0.164, 0.168, 0.169, 0.169, 0.154, 0.154, 0.163, 0.164, 0.164, 0.17, 0.162, 0.162, 0.162, 0.162, 0.162, 0.162, 0.163, 0.162, 0.162, 0.166, 0.166, 0.172, 0.173, 0.173, 0.173, 0.173, 0.173, 0.173, 0.173, 0.173, 0.177, 0.177, 0.177, 0.177, 0.177, 0.177, 0.186, 0.192, 0.192, 0.197, 0.198, 0.198, 0.197, 0.197, 0.203, 0.198, 0.203, 0.206, 0.209, 0.209, 0.209, 0.209, 0.21, 0.21, 0.21, 0.208, 0.208, 0.208, 0.208, 0.21, 0.209, 0.209, 0.209, 0.209, 0.209, 0.206, 0.207, 0.207, 0.206, 0.206, 0.206, 0.206, 0.206, 0.206, 0.206, 0.205, 0.204, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.206, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.205, 0.21, 0.213, 0.213, 0.213, 0.216, 0.221, 0.224, 0.226, 0.228, 0.228, 0.228, 0.228, 0.228, 0.228, 0.228, 0.228, 0.228, 0.228, 0.232, 0.232, 0.232, 0.242, 0.243, 0.243, 0.243, 0.246, 0.247, 0.247, 0.256, 0.256, 0.258, 0.258, 0.258, 0.258]</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770, 1800, 1830, 1860, 1890, 1920, 1950, 1980, 2010, 2040, 2070, 2100, 2130, 2160, 2190, 2220, 2250, 2280, 2310, 2340, 2370, 2400, 2430, 2460, 2490, 2520, 2550, 2580, 2610, 2640, 2670, 2700, 2730, 2760, 2790, 2820, 2850, 2880, 2910, 2940, 2970, 3000, 3030, 3060, 3090, 3120, 3150, 3180, 3210, 3240, 3270, 3300, 3330, 3360, 3390, 3420, 3450, 3480, 3510, 3540, 3570, 3600, 3630, 3660, 3690, 3720, 3750, 3780, 3810, 3840, 3870]</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>[0, 15.377138078212727, 27.21240472793577, 39.61688039302824, 65.06827924251554, 79.17661390304565, 93.19360697865486, 104.55545499920844, 126.63968327641484, 148.4153095543384, 153.611894840002, 160.69296286702152, 179.01496565937993, 197.3653018057346, 221.83780069947238, 235.43005791306493, 250.67595230340956, 263.13396958112713, 284.64429749250405, 306.6673735022544, 318.482655930519, 326.1438147306441, 337.986434650421, 359.60388281345354, 369.6449577808379, 389.487890434265, 410.1581399440764, 434.2808062076567, 452.29349544048296, 469.2624547243117, 475.30758461952195, 496.6413098096846, 514.1573836088179, 537.4623982429503, 557.3667608737944, 580.8264263629912, 599.9407006740569, 617.9534012317656, 633.6482729196547, 634.067972922325, 656.4695755720137, 680.8972234487532, 696.4046216011045, 702.3192432045935, 720.9866619944571, 743.5013609766959, 751.3832611918448, 777.5444988131521, 791.461275398731, 817.5601184010503, 825.5708667039869, 849.5194583177564, 862.5830127000806, 875.3819208621976, 890.4749338626859, 912.0107328891752, 921.3183315753935, 947.9640365600584, 965.6403567552564, 968.4366613626478, 978.0646505832669, 1000.0483098030088, 1016.2652360439298, 1027.6176486015318, 1042.4561325192449, 1064.481381523609, 1073.0340817570684, 1100.164254105091, 1116.466926229, 1132.077853810787, 1156.11351313591, 1179.568975019455, 1183.1946407079697, 1194.843490087986, 1211.0917439818384, 1232.6275430083276, 1242.0187432646753, 1266.72657879591, 1280.9398817658425, 1305.6405724644662, 1315.506672525406, 1338.9518831253054, 1352.3512946367266, 1364.3467159271243, 1379.15815666914, 1402.1623056292535, 1411.354952156544, 1435.5781033635142, 1449.7466783404352, 1454.5873368382456, 1465.7711828351023, 1487.5074258923532, 1505.2689863324167, 1523.5709646344187, 1543.5491364598277, 1566.595752632618, 1579.9213245987894, 1597.0962251305582, 1610.7322078347208, 1611.151907837391, 1632.1694123387338, 1653.7688000321389, 1676.5937578082085, 1700.583504474163, 1720.1095995783805, 1739.6875986933708, 1748.743398940563, 1775.6710794329642, 1788.510594189167, 1788.510594189167, 1797.2742439508438, 1815.0783352851868, 1830.721446108818, 1848.0103147983552, 1867.0490082740785, 1884.5554654836656, 1892.3214426875115, 1905.9103573918344, 1924.8005403399468, 1936.1347780108451, 1941.7182123064995, 1960.9992050528526, 1976.781083548069, 2000.0991516709328, 2021.9497819066048, 2042.0172309994698, 2049.9603314042092, 2074.99835010767, 2088.0800086379054, 2088.0800086379054]</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>[0, 1.98, 3.29, 14.86, 15.99, 21.76, 22.22, 24.27, 24.7, 25.28, 28.46, 35.53, 46.26, 46.75, 47.2, 58.97, 59.52, 61.11, 65.33, 65.84, 73.88, 74.39, 75.94, 78.51, 79.01, 79.39, 79.87, 80.38, 80.83, 81.23, 82.19, 85.06, 85.61, 86.08, 86.77, 87.26, 87.74, 102.13, 119.78, 120.26, 121.7, 137.37, 137.9, 155.16, 157.47, 178.29, 198.45, 216.86, 217.42, 241.43, 245.86, 257.36, 257.93, 264.53, 265.16, 281.65, 309.61, 329.42, 334.85, 338.43, 340.7, 356.92, 357.58, 377.85, 379.91, 395.67, 410.12, 426.95, 429.04, 438.93, 441.42, 455.61, 456.64, 462.78, 466.84, 484.75, 504.06, 518.6, 520.01, 537.45, 539.11, 553.49, 554.2, 558.57, 561.47, 577.16, 602.12, 614.76, 616.08, 618.09, 621.8, 623.88, 624.58, 625.27, 625.92, 626.62, 633.65, 650.54, 669.47, 670.52, 679.22, 682.1, 683.99, 685.45, 687.7, 701.8, 711.35, 713.56, 714.94, 715.69, 724.1, 725.01, 725.74, 726.62, 749.77, 750.52, 751.18, 756.31, 766.87, 768.02, 768.81, 774.24, 775.48, 776.28, 781.31, 790.37, 796.04, 797.65, 799.33, 800.98]</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 0, 0, 0, 0, -10, 0, -10, 0, 0, 0, -20, 0, 0, 0, -20, 0, -20, 0, -10, 0, -20, 0, -20, -20, -20, 0, 0, 0, 0, -20, 0, 0, -20, -10, -10, 0, 0, -20, 0, -20, 0, -20, 0, 0, 0, 0, 0, 0, 0, -20, -20, -20, 0, -20, 0, 0, 0, 0, 0, -20, -20, 0, -20, -20, -10, -20, -20, -10, 0, -20, -10, -10, -10, -10, 0, 0, -10, -10, 0, -10, -10, -10, -10, -10, -10, -10, 0, 0, 0, -10, -10, -10, -10, -10, -20, -20]</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>42</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>uniform</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4']</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>[100, 142, 166, 195, 195, 230, 230, 239, 241, 241, 269, 273, 278, 278, 296, 340, 363, 363, 363, 363, 388, 395, 451, 468, 468, 497, 497, 498, 544, 544, 558, 560, 578, 578, 578, 609, 611, 621, 623, 623, 653, 653, 688, 706, 706, 739, 739, 739, 739, 739, 739, 756, 756, 756, 756, 764, 764, 805, 862, 862]</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>[0.175, 0.149, 0.15, 0.157, 0.157, 0.156, 0.156, 0.165, 0.165, 0.165, 0.171, 0.173, 0.177, 0.177, 0.188, 0.191, 0.19, 0.19, 0.19, 0.19, 0.194, 0.193, 0.192, 0.198, 0.198, 0.198, 0.198, 0.198, 0.198, 0.198, 0.199, 0.198, 0.198, 0.198, 0.198, 0.197, 0.198, 0.198, 0.199, 0.199, 0.201, 0.201, 0.206, 0.209, 0.209, 0.217, 0.217, 0.217, 0.217, 0.217, 0.217, 0.223, 0.223, 0.223, 0.223, 0.223, 0.223, 0.226, 0.229, 0.229]</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590, 1620, 1650, 1680, 1710, 1740, 1770]</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>[0, 8.532829105854036, 32.385429680347464, 43.786703407764456, 67.7697523236275, 83.86252280473713, 98.48199352622036, 112.21912265419964, 137.36185892224313, 159.87983737587928, 168.31447529196737, 191.55719642043113, 208.0351593673229, 232.09231578707693, 254.87276007533072, 276.40855910181995, 284.9612593352794, 310.9441089332103, 324.3637432277202, 324.3637432277202, 333.842792969942, 349.17125651240343, 370.5532214343547, 386.7867395341396, 409.7908884942531, 421.3423391520977, 436.3474037051201, 443.0240105867386, 457.62000839710237, 474.4466292619705, 483.57557423114775, 499.4687935352325, 520.926863002777, 538.1401619672774, 563.10211083889, 575.5777124643325, 590.2019501447677, 604.4984607815742, 625.6307761549949, 646.1691513180732, 655.2231950879096, 683.0835373759269, 699.7400968432426, 722.0501949429511, 728.8276282668112, 751.0328036189078, 780.0028000235557, 799.6712016940116, 818.5208828091621, 843.2038814663887, 849.7326314091682, 871.3774625182152, 889.1390229582787, 914.6265386939049, 938.4838922142983, 961.1125090241433, 979.0067232728005, 996.1816238045693, 1011.2223468899728, 1011.6420468926431]</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>[0, 11.01, 20.1, 27.22, 27.56, 49.81, 50.46, 55.93, 56.41, 56.85, 67.4, 69.68, 71.49, 72.58, 75.71, 91.7, 99.38, 100.62, 101.1, 101.97, 112.26, 115.75, 137.16, 146.09, 146.77, 158.92, 159.41, 160.29, 174.32, 175.4, 180.25, 183.03, 190.76, 191.29, 192.38, 201.87, 203.73, 208.65, 209.92, 211.1, 220.47, 221.53, 237.13, 245.26, 246.16, 255.4, 256.32, 256.9, 257.95, 258.55, 259.27, 268.99, 269.94, 270.6, 271.26, 276.5, 277.52, 289.7, 303.06, 304.37]</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>[-10, 0, 0, -10, 0, 0, -10, 0, 0, 0, -10, 0, -20, 0, -10, 0, -10, 0, -20, 0, -20, -20, -10, 0, 0, 0, -10, 0, 0, 0, 0, -10, -20, -20, 0, -10, -10, -10, 0, -20, -20, -10, 0, -20, -20, 0, -20, -20, -20, 0, -20, 0, -20, -20, 0, 0, 0, -20, -20, 0, 0, 0, -10, 0, 0, -20, -10, 0, -20, -10, -10, 0, -10, 0, 0, -10, 0, 0, 0, -20, 0, 0, 0, 0, -20, 0, -10, -10, -10, -10, 0, -20, -10, 0, 0, 0, -20, 0, -10, -20]</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>43</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>clusterWt</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3']</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>[100, 103, 120, 154, 154, 191, 191, 211, 220, 220, 259, 270, 274, 275, 300, 343, 364, 364, 364, 364, 383, 410, 411, 437, 443, 484, 526, 580, 581, 595, 600, 600, 600, 600, 633, 633, 633, 673, 689, 689, 689, 691, 726, 733, 733, 763, 778, 787, 816, 816, 849, 881, 881, 881]</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>[0.175, 0.17, 0.167, 0.172, 0.172, 0.162, 0.162, 0.172, 0.172, 0.172, 0.178, 0.178, 0.183, 0.185, 0.194, 0.198, 0.199, 0.199, 0.199, 0.199, 0.204, 0.206, 0.206, 0.205, 0.209, 0.21, 0.207, 0.212, 0.215, 0.219, 0.219, 0.219, 0.219, 0.219, 0.22, 0.22, 0.22, 0.24, 0.245, 0.245, 0.245, 0.244, 0.244, 0.247, 0.247, 0.25, 0.256, 0.257, 0.259, 0.259, 0.258, 0.263, 0.263, 0.263]</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440, 1470, 1500, 1530, 1560, 1590]</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>[0, 15.61377530097961, 37.244000625610354, 48.80762026309967, 73.28011915683746, 87.38104672431946, 111.86604731678966, 130.35512863993648, 152.91177369952203, 174.6874009311199, 183.74438795447347, 203.24752616286275, 226.17839135527606, 248.90898837447162, 270.29471158385275, 291.34106063246725, 300.06146087050433, 327.9339722573757, 339.32677225470536, 339.32677225470536, 346.8384720504283, 365.5168534457683, 376.5317718803882, 383.7229489147662, 397.69495854973786, 417.76240764260285, 424.8058078348636, 450.967045456171, 463.24944377541533, 478.1457698166369, 492.33523406386365, 507.57353035807597, 526.0433403909205, 547.8173657834529, 567.8007478654384, 583.8040451228618, 590.8163665115833, 605.3056156218051, 616.7176453888416, 619.5512048065661, 624.8552451074122, 640.4230005681513, 662.2932051122187, 677.334156936407, 702.2961058080195, 714.791988056898, 725.8755062758922, 739.6537706911564, 756.3528340637685, 776.8912094891072, 785.5019850790501, 807.7446593821049, 824.823082882166, 843.8503737986089]</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>[0, 0.97, 5.89, 17.64, 18.52, 29.17, 29.69, 38.94, 41.12, 41.6, 56.24, 60.59, 61.11, 63.27, 70.93, 80.51, 89.88, 90.39, 90.97, 91.68, 97.46, 105.37, 106.53, 114.58, 119.53, 130.13, 139.24, 147.97, 149.37, 155.9, 158.43, 159.28, 160.62, 161.98, 172.96, 174.12, 174.78, 179.8, 185.41, 186.61, 187.56, 188.85, 202.0, 204.02, 204.69, 213.38, 218.51, 222.41, 231.76, 233.19, 242.34, 253.58, 254.99, 255.97]</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 0, 0, -20, 0, -10, -20, -20, 0, -20, 0, 0, -20, 0, 0, -20, -20, -20, -20, 0, 0, -20, 0, -20, -20, 0, -10, 0, 0, 0, -10, 0, -10, -10, -10, -10, -10, -10, -10, -20, -20, -20, -20, -20, 0, 0, 0, -20, 0, 0, -20, -20, -20, 0, -20, 0, 0, 0, 0, 0, -10, -20, -10, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, 0, -10, 0, -10, -10, 0, -10, -10, -10, -10, -10, 0, -10, -10, -10, 0, 0, 0, -20, -20]</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>44</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>clusterStdLow</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_3', 'FloorPlan_Train2_3', 'FloorPlan_Train3_3', 'FloorPlan_Train4_3', 'FloorPlan_Train5_3', 'FloorPlan_Train6_3', 'FloorPlan_Train7_3', 'FloorPlan_Train8_3', 'FloorPlan_Train9_3', 'FloorPlan_Train10_3', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4']</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>[100, 103, 105, 138, 138, 171, 171, 172, 180, 180, 213, 213, 213, 213, 213, 213, 213, 236, 272, 272, 272, 303, 303, 340, 344, 388, 436, 487, 488, 497, 505, 535, 535, 542, 544, 592, 641, 685, 686, 712, 717, 717, 721, 733, 733, 751, 751, 751, 757]</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>[0.175, 0.17, 0.176, 0.168, 0.168, 0.153, 0.153, 0.153, 0.154, 0.154, 0.16, 0.16, 0.16, 0.16, 0.16, 0.16, 0.16, 0.17, 0.182, 0.182, 0.182, 0.182, 0.182, 0.189, 0.189, 0.192, 0.186, 0.191, 0.194, 0.196, 0.197, 0.198, 0.198, 0.198, 0.198, 0.198, 0.196, 0.196, 0.196, 0.198, 0.198, 0.198, 0.203, 0.203, 0.203, 0.204, 0.204, 0.204, 0.208]</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350, 1380, 1410, 1440]</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>[0, 15.684278547763812, 36.428117477893835, 49.84248615503313, 73.82553507089617, 87.80777167081835, 102.89830083847048, 113.10807307958603, 136.33322056531904, 158.356297814846, 166.7059346914291, 190.34394702911374, 192.35234699249264, 211.4070512771606, 233.23161916732784, 246.60018749237054, 253.32775410413737, 272.06769443750375, 292.68455005884164, 315.3530254006385, 337.5341205239295, 360.4864355206489, 365.0516448795795, 373.1598515808582, 393.5996916115283, 415.1354906380176, 423.18509085774417, 447.89292638897894, 462.750764876604, 467.7699422419071, 486.4475129306316, 507.4971626460552, 510.8700092732906, 518.435766261816, 535.6349851787089, 559.1285841166972, 567.3458843410014, 588.6624483287333, 602.5792249143121, 621.8053601682184, 633.375839692354, 638.6297005474565, 649.5178070843218, 668.0558386862276, 680.1051645338533, 701.8274025499818, 728.9817494451997, 749.9706059038637, 768.2703845679757]</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>[0, 0.44, 0.92, 8.81, 9.91, 21.69, 22.33, 22.73, 24.21, 25.35, 33.88, 34.32, 34.89, 35.37, 35.9, 36.92, 37.37, 47.4, 63.91, 64.6, 65.1, 75.33, 76.13, 86.11, 88.42, 100.09, 108.38, 119.18, 120.11, 124.65, 129.8, 142.22, 143.19, 147.36, 148.89, 161.45, 175.65, 187.33, 188.08, 194.76, 196.39, 197.88, 199.2, 204.95, 206.55, 212.6, 213.47, 214.43, 218.62]</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>[-10, 0, -20, -10, 0, -10, -10, 0, -10, -10, -10, -10, -10, -10, 0, -10, -10, 0, -10, -10, -10, -10, 0, 0, -10, -20, -20, -20, 0, -20, -20, -20, 0, -20, 0, -20, -20, -20, -20, -20, -20, -20, -20, -20, -20, -20, -20, 0, 0, 0, -20, 0, 0, 0, -20, -10, -20, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, -10, -10, 0, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, -10, 0, 0, 0, 0, -20, -20]</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
-      <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>45</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>cifar</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>CBCLSVM</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>clusterStdHigh</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>['FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_2', 'FloorPlan_Train2_2', 'FloorPlan_Train3_2', 'FloorPlan_Train4_2', 'FloorPlan_Train5_2', 'FloorPlan_Train6_2', 'FloorPlan_Train7_2', 'FloorPlan_Train8_2', 'FloorPlan_Train9_2', 'FloorPlan_Train10_2', 'FloorPlan_Train1_5', 'FloorPlan_Train2_5', 'FloorPlan_Train3_5', 'FloorPlan_Train4_5', 'FloorPlan_Train5_1', 'FloorPlan_Train6_5', 'FloorPlan_Train7_5', 'FloorPlan_Train8_5', 'FloorPlan_Train9_5', 'FloorPlan_Train10_5', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1']</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>[100, 103, 132, 138, 138, 158, 158, 161, 163, 163, 187, 198, 205, 209, 209, 236, 236, 250, 272, 272, 285, 322, 322, 332, 353, 401, 449, 500, 508, 530, 533, 560, 560, 560, 561, 561, 561, 605, 619, 619, 642, 650, 652, 652, 675, 715]</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>[0.175, 0.17, 0.158, 0.17, 0.17, 0.164, 0.164, 0.166, 0.165, 0.165, 0.171, 0.167, 0.168, 0.171, 0.171, 0.17, 0.17, 0.176, 0.175, 0.175, 0.177, 0.177, 0.177, 0.18, 0.184, 0.19, 0.183, 0.189, 0.194, 0.196, 0.196, 0.202, 0.202, 0.202, 0.202, 0.202, 0.202, 0.212, 0.216, 0.216, 0.218, 0.219, 0.221, 0.221, 0.227, 0.228]</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600, 630, 660, 690, 720, 750, 780, 810, 840, 870, 900, 930, 960, 990, 1020, 1050, 1080, 1110, 1140, 1170, 1200, 1230, 1260, 1290, 1320, 1350]</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>[0, 13.12116733789443, 24.469501554965966, 36.70203067064285, 63.132329475879665, 75.28112615346909, 100.98499888181684, 111.85392761230464, 132.54064064025874, 153.8213667869567, 161.554130578041, 169.10603463649744, 179.9760035336017, 192.4756721556186, 214.99037113785738, 227.65783589482302, 243.45608955621717, 258.4623858213424, 279.5740566968917, 301.3496812582015, 310.5078018665313, 334.9389204025268, 348.5694865822791, 361.3624842762946, 381.7847644686698, 405.27836340665806, 413.30706323385226, 438.014898765087, 453.77526637315736, 472.4290038943289, 480.896104121208, 502.9815459251402, 519.7184009552, 540.5743508577344, 565.9066036224363, 589.7765677452085, 607.2640337944028, 625.6956343650816, 642.5341018319127, 642.953801834583, 663.9704014897344, 685.4540596127508, 702.5248088717459, 725.3378479838369, 747.188478219509, 766.7664773344992]</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>[0, 0.44, 7.44, 10.15, 10.52, 15.66, 16.44, 18.42, 18.89, 19.36, 28.47, 33.37, 35.46, 36.73, 37.83, 44.11, 44.91, 48.85, 56.06, 56.62, 62.69, 75.84, 76.82, 81.61, 88.06, 101.76, 113.86, 129.69, 132.72, 141.3, 144.05, 149.85, 150.67, 151.43, 152.04, 152.66, 153.19, 169.9, 172.29, 173.34, 180.94, 185.48, 187.08, 188.66, 194.37, 203.13]</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>[0, -10, -20, 0, -20, -20, 0, -10, -10, -10, -10, -10, -20, -10, -10, -10, -20, -20, -10, -10, 0, -20, -20, -20, 0, 0, 0, -10, -10, -10, -10, -10, -20, -10, -10, -20, -10, -10, -10, 0, 0, 0, 0, 0, 0, 0, -20, -20, -20, -20, 0, -20, -10, -20, 0, 0, -20, 0, -20, -10, -10, -20, -20, 0, 0, 0, 0, 0, 0, 0, 0, 0, -20, 0, 0, 0, 0, 0, -10, 0, 0, 0, -20, 0, 0, 0, 0, 0, 0, 0, -20, -20, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">

</xml_diff>